<commit_message>
fix: cardinality contactPoint in DatasetSeries
Compliant to HealthDCAT-AP
</commit_message>
<xml_diff>
--- a/Documents/Metadata_CoreGenericHealth_v2.xlsx
+++ b/Documents/Metadata_CoreGenericHealth_v2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://healthri-my.sharepoint.com/personal/hannah_neikes_health-ri_nl/Documents/Documenten/Plateau2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://healthri-my.sharepoint.com/personal/hannah_neikes_health-ri_nl/Documents/Documenten/GitHub/health-ri-metadata/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3206" documentId="13_ncr:1_{F400FBA4-788C-A049-BCFC-7AF7AD8163AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CB4AE5F-FFF7-4440-BD51-E643CDE18398}"/>
+  <xr:revisionPtr revIDLastSave="3208" documentId="13_ncr:1_{F400FBA4-788C-A049-BCFC-7AF7AD8163AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D941DCCA-04DE-4EAA-A3D3-3922BE451E31}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-12765" windowWidth="38640" windowHeight="21120" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-9225" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="14" r:id="rId1"/>
@@ -2613,7 +2613,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="237">
+  <cellXfs count="230">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -3239,28 +3239,40 @@
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3271,39 +3283,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -10227,102 +10206,102 @@
       <c r="L13" s="130"/>
     </row>
     <row r="14" spans="1:12" ht="43.2">
-      <c r="A14" s="215" t="s">
+      <c r="A14" s="220" t="s">
         <v>95</v>
       </c>
-      <c r="B14" s="216" t="s">
+      <c r="B14" s="221" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="215" t="s">
+      <c r="C14" s="220" t="s">
         <v>97</v>
       </c>
       <c r="D14" s="154" t="s">
         <v>98</v>
       </c>
-      <c r="E14" s="218" t="s">
+      <c r="E14" s="222" t="s">
         <v>99</v>
       </c>
-      <c r="F14" s="217" t="s">
+      <c r="F14" s="219" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="217" t="s">
+      <c r="G14" s="219" t="s">
         <v>100</v>
       </c>
-      <c r="H14" s="217" t="s">
+      <c r="H14" s="219" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="219" t="s">
+      <c r="I14" s="217" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="219" t="s">
+      <c r="J14" s="217" t="s">
         <v>30</v>
       </c>
-      <c r="K14" s="220"/>
-      <c r="L14" s="219"/>
+      <c r="K14" s="218"/>
+      <c r="L14" s="217"/>
     </row>
     <row r="15" spans="1:12" ht="43.2">
-      <c r="A15" s="215"/>
-      <c r="B15" s="216"/>
-      <c r="C15" s="215"/>
+      <c r="A15" s="220"/>
+      <c r="B15" s="221"/>
+      <c r="C15" s="220"/>
       <c r="D15" s="155" t="s">
         <v>101</v>
       </c>
-      <c r="E15" s="218"/>
-      <c r="F15" s="217"/>
-      <c r="G15" s="217"/>
-      <c r="H15" s="217"/>
-      <c r="I15" s="219"/>
-      <c r="J15" s="219"/>
-      <c r="K15" s="220"/>
-      <c r="L15" s="219"/>
+      <c r="E15" s="222"/>
+      <c r="F15" s="219"/>
+      <c r="G15" s="219"/>
+      <c r="H15" s="219"/>
+      <c r="I15" s="217"/>
+      <c r="J15" s="217"/>
+      <c r="K15" s="218"/>
+      <c r="L15" s="217"/>
     </row>
     <row r="16" spans="1:12" ht="28.8">
-      <c r="A16" s="215"/>
-      <c r="B16" s="216"/>
-      <c r="C16" s="215"/>
+      <c r="A16" s="220"/>
+      <c r="B16" s="221"/>
+      <c r="C16" s="220"/>
       <c r="D16" s="155" t="s">
         <v>102</v>
       </c>
-      <c r="E16" s="218"/>
-      <c r="F16" s="217"/>
-      <c r="G16" s="217"/>
-      <c r="H16" s="217"/>
-      <c r="I16" s="219"/>
-      <c r="J16" s="219"/>
-      <c r="K16" s="220"/>
-      <c r="L16" s="219"/>
+      <c r="E16" s="222"/>
+      <c r="F16" s="219"/>
+      <c r="G16" s="219"/>
+      <c r="H16" s="219"/>
+      <c r="I16" s="217"/>
+      <c r="J16" s="217"/>
+      <c r="K16" s="218"/>
+      <c r="L16" s="217"/>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="215"/>
-      <c r="B17" s="216"/>
-      <c r="C17" s="215"/>
+      <c r="A17" s="220"/>
+      <c r="B17" s="221"/>
+      <c r="C17" s="220"/>
       <c r="D17" s="155" t="s">
         <v>103</v>
       </c>
-      <c r="E17" s="218"/>
-      <c r="F17" s="217"/>
-      <c r="G17" s="217"/>
-      <c r="H17" s="217"/>
-      <c r="I17" s="219"/>
-      <c r="J17" s="219"/>
-      <c r="K17" s="220"/>
-      <c r="L17" s="219"/>
+      <c r="E17" s="222"/>
+      <c r="F17" s="219"/>
+      <c r="G17" s="219"/>
+      <c r="H17" s="219"/>
+      <c r="I17" s="217"/>
+      <c r="J17" s="217"/>
+      <c r="K17" s="218"/>
+      <c r="L17" s="217"/>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="215"/>
-      <c r="B18" s="216"/>
-      <c r="C18" s="215"/>
+      <c r="A18" s="220"/>
+      <c r="B18" s="221"/>
+      <c r="C18" s="220"/>
       <c r="D18" s="155" t="s">
         <v>104</v>
       </c>
-      <c r="E18" s="218"/>
-      <c r="F18" s="217"/>
-      <c r="G18" s="217"/>
-      <c r="H18" s="217"/>
-      <c r="I18" s="219"/>
-      <c r="J18" s="219"/>
-      <c r="K18" s="220"/>
-      <c r="L18" s="219"/>
+      <c r="E18" s="222"/>
+      <c r="F18" s="219"/>
+      <c r="G18" s="219"/>
+      <c r="H18" s="219"/>
+      <c r="I18" s="217"/>
+      <c r="J18" s="217"/>
+      <c r="K18" s="218"/>
+      <c r="L18" s="217"/>
     </row>
     <row r="19" spans="1:12" ht="28.8">
       <c r="A19" s="126" t="s">
@@ -11558,17 +11537,17 @@
     <sortCondition ref="A2:A53"/>
   </sortState>
   <mergeCells count="11">
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="C14:C18"/>
+    <mergeCell ref="F14:F18"/>
+    <mergeCell ref="E14:E18"/>
     <mergeCell ref="L14:L18"/>
     <mergeCell ref="K14:K18"/>
     <mergeCell ref="G14:G18"/>
     <mergeCell ref="H14:H18"/>
     <mergeCell ref="I14:I18"/>
     <mergeCell ref="J14:J18"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="C14:C18"/>
-    <mergeCell ref="F14:F18"/>
-    <mergeCell ref="E14:E18"/>
   </mergeCells>
   <conditionalFormatting sqref="F2:F14 F19:F53">
     <cfRule type="cellIs" dxfId="190" priority="8" operator="equal">
@@ -11940,102 +11919,102 @@
       <c r="L7" s="130"/>
     </row>
     <row r="8" spans="1:12" ht="28.8">
-      <c r="A8" s="215" t="s">
+      <c r="A8" s="220" t="s">
         <v>95</v>
       </c>
-      <c r="B8" s="221" t="s">
+      <c r="B8" s="223" t="s">
         <v>96</v>
       </c>
-      <c r="C8" s="215" t="s">
+      <c r="C8" s="220" t="s">
         <v>97</v>
       </c>
       <c r="D8" s="154" t="s">
         <v>98</v>
       </c>
-      <c r="E8" s="218" t="s">
+      <c r="E8" s="222" t="s">
         <v>307</v>
       </c>
-      <c r="F8" s="217" t="s">
+      <c r="F8" s="219" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="217" t="s">
+      <c r="G8" s="219" t="s">
         <v>100</v>
       </c>
-      <c r="H8" s="217" t="s">
+      <c r="H8" s="219" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="219" t="s">
+      <c r="I8" s="217" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="219" t="s">
+      <c r="J8" s="217" t="s">
         <v>30</v>
       </c>
       <c r="K8" s="138"/>
-      <c r="L8" s="219"/>
+      <c r="L8" s="217"/>
     </row>
     <row r="9" spans="1:12" ht="28.8">
-      <c r="A9" s="215"/>
-      <c r="B9" s="221"/>
-      <c r="C9" s="215"/>
+      <c r="A9" s="220"/>
+      <c r="B9" s="223"/>
+      <c r="C9" s="220"/>
       <c r="D9" s="155" t="s">
         <v>101</v>
       </c>
-      <c r="E9" s="218"/>
-      <c r="F9" s="217"/>
-      <c r="G9" s="217"/>
-      <c r="H9" s="217"/>
-      <c r="I9" s="219"/>
-      <c r="J9" s="219"/>
+      <c r="E9" s="222"/>
+      <c r="F9" s="219"/>
+      <c r="G9" s="219"/>
+      <c r="H9" s="219"/>
+      <c r="I9" s="217"/>
+      <c r="J9" s="217"/>
       <c r="K9" s="138"/>
-      <c r="L9" s="219"/>
+      <c r="L9" s="217"/>
     </row>
     <row r="10" spans="1:12" ht="28.8">
-      <c r="A10" s="215"/>
-      <c r="B10" s="221"/>
-      <c r="C10" s="215"/>
+      <c r="A10" s="220"/>
+      <c r="B10" s="223"/>
+      <c r="C10" s="220"/>
       <c r="D10" s="155" t="s">
         <v>102</v>
       </c>
-      <c r="E10" s="218"/>
-      <c r="F10" s="217"/>
-      <c r="G10" s="217"/>
-      <c r="H10" s="217"/>
-      <c r="I10" s="219"/>
-      <c r="J10" s="219"/>
+      <c r="E10" s="222"/>
+      <c r="F10" s="219"/>
+      <c r="G10" s="219"/>
+      <c r="H10" s="219"/>
+      <c r="I10" s="217"/>
+      <c r="J10" s="217"/>
       <c r="K10" s="138"/>
-      <c r="L10" s="219"/>
+      <c r="L10" s="217"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="215"/>
-      <c r="B11" s="221"/>
-      <c r="C11" s="215"/>
+      <c r="A11" s="220"/>
+      <c r="B11" s="223"/>
+      <c r="C11" s="220"/>
       <c r="D11" s="155" t="s">
         <v>103</v>
       </c>
-      <c r="E11" s="218"/>
-      <c r="F11" s="217"/>
-      <c r="G11" s="217"/>
-      <c r="H11" s="217"/>
-      <c r="I11" s="219"/>
-      <c r="J11" s="219"/>
+      <c r="E11" s="222"/>
+      <c r="F11" s="219"/>
+      <c r="G11" s="219"/>
+      <c r="H11" s="219"/>
+      <c r="I11" s="217"/>
+      <c r="J11" s="217"/>
       <c r="K11" s="156"/>
-      <c r="L11" s="219"/>
+      <c r="L11" s="217"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="215"/>
-      <c r="B12" s="221"/>
-      <c r="C12" s="215"/>
+      <c r="A12" s="220"/>
+      <c r="B12" s="223"/>
+      <c r="C12" s="220"/>
       <c r="D12" s="155" t="s">
         <v>104</v>
       </c>
-      <c r="E12" s="218"/>
-      <c r="F12" s="217"/>
-      <c r="G12" s="217"/>
-      <c r="H12" s="217"/>
-      <c r="I12" s="219"/>
-      <c r="J12" s="219"/>
+      <c r="E12" s="222"/>
+      <c r="F12" s="219"/>
+      <c r="G12" s="219"/>
+      <c r="H12" s="219"/>
+      <c r="I12" s="217"/>
+      <c r="J12" s="217"/>
       <c r="K12" s="138"/>
-      <c r="L12" s="219"/>
+      <c r="L12" s="217"/>
     </row>
     <row r="13" spans="1:12" ht="43.2">
       <c r="A13" s="126" t="s">
@@ -12247,7 +12226,7 @@
       </c>
       <c r="L18" s="107"/>
     </row>
-    <row r="19" spans="1:12" s="233" customFormat="1">
+    <row r="19" spans="1:12">
       <c r="A19" s="126" t="s">
         <v>225</v>
       </c>
@@ -12281,41 +12260,41 @@
       </c>
       <c r="L19" s="130"/>
     </row>
-    <row r="20" spans="1:12" s="233" customFormat="1" ht="43.2">
-      <c r="A20" s="228" t="s">
+    <row r="20" spans="1:12" ht="43.2">
+      <c r="A20" s="122" t="s">
         <v>325</v>
       </c>
-      <c r="B20" s="229" t="s">
+      <c r="B20" s="35" t="s">
         <v>326</v>
       </c>
-      <c r="C20" s="228" t="s">
+      <c r="C20" s="122" t="s">
         <v>327</v>
       </c>
-      <c r="D20" s="230" t="s">
+      <c r="D20" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="234" t="s">
+      <c r="E20" s="215" t="s">
         <v>328</v>
       </c>
-      <c r="F20" s="231" t="s">
+      <c r="F20" s="125" t="s">
         <v>27</v>
       </c>
-      <c r="G20" s="231" t="s">
+      <c r="G20" s="125" t="s">
         <v>18</v>
       </c>
-      <c r="H20" s="231" t="s">
+      <c r="H20" s="125" t="s">
         <v>93</v>
       </c>
-      <c r="I20" s="232" t="s">
+      <c r="I20" s="107" t="s">
         <v>19</v>
       </c>
-      <c r="J20" s="232" t="s">
+      <c r="J20" s="107" t="s">
         <v>76</v>
       </c>
-      <c r="K20" s="235"/>
-      <c r="L20" s="232"/>
-    </row>
-    <row r="21" spans="1:12" s="233" customFormat="1" ht="72">
+      <c r="K20" s="106"/>
+      <c r="L20" s="107"/>
+    </row>
+    <row r="21" spans="1:12" ht="72">
       <c r="A21" s="126" t="s">
         <v>329</v>
       </c>
@@ -12349,41 +12328,41 @@
       <c r="K21" s="131"/>
       <c r="L21" s="130"/>
     </row>
-    <row r="22" spans="1:12" s="233" customFormat="1">
-      <c r="A22" s="228" t="s">
+    <row r="22" spans="1:12">
+      <c r="A22" s="122" t="s">
         <v>252</v>
       </c>
-      <c r="B22" s="229" t="s">
+      <c r="B22" s="35" t="s">
         <v>253</v>
       </c>
-      <c r="C22" s="228" t="s">
+      <c r="C22" s="122" t="s">
         <v>254</v>
       </c>
-      <c r="D22" s="230" t="s">
+      <c r="D22" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="229"/>
-      <c r="F22" s="231" t="s">
+      <c r="E22" s="35"/>
+      <c r="F22" s="125" t="s">
         <v>27</v>
       </c>
-      <c r="G22" s="231" t="s">
+      <c r="G22" s="125" t="s">
         <v>234</v>
       </c>
-      <c r="H22" s="231" t="s">
+      <c r="H22" s="125" t="s">
         <v>29</v>
       </c>
-      <c r="I22" s="232" t="s">
+      <c r="I22" s="107" t="s">
         <v>19</v>
       </c>
-      <c r="J22" s="232" t="s">
+      <c r="J22" s="107" t="s">
         <v>76</v>
       </c>
-      <c r="K22" s="235" t="s">
+      <c r="K22" s="106" t="s">
         <v>256</v>
       </c>
-      <c r="L22" s="232"/>
-    </row>
-    <row r="23" spans="1:12" s="233" customFormat="1" ht="57.6">
+      <c r="L22" s="107"/>
+    </row>
+    <row r="23" spans="1:12" ht="57.6">
       <c r="A23" s="126" t="s">
         <v>334</v>
       </c>
@@ -12417,41 +12396,41 @@
       <c r="K23" s="212"/>
       <c r="L23" s="130"/>
     </row>
-    <row r="24" spans="1:12" s="233" customFormat="1" ht="28.8">
-      <c r="A24" s="228" t="s">
+    <row r="24" spans="1:12" ht="28.8">
+      <c r="A24" s="122" t="s">
         <v>269</v>
       </c>
-      <c r="B24" s="229" t="s">
+      <c r="B24" s="35" t="s">
         <v>270</v>
       </c>
-      <c r="C24" s="228" t="s">
+      <c r="C24" s="122" t="s">
         <v>271</v>
       </c>
-      <c r="D24" s="230" t="s">
+      <c r="D24" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="236" t="s">
+      <c r="E24" s="216" t="s">
         <v>338</v>
       </c>
-      <c r="F24" s="231" t="s">
+      <c r="F24" s="125" t="s">
         <v>17</v>
       </c>
-      <c r="G24" s="231" t="s">
+      <c r="G24" s="125" t="s">
         <v>75</v>
       </c>
-      <c r="H24" s="231" t="s">
+      <c r="H24" s="125" t="s">
         <v>37</v>
       </c>
-      <c r="I24" s="232" t="s">
+      <c r="I24" s="107" t="s">
         <v>69</v>
       </c>
-      <c r="J24" s="232" t="s">
+      <c r="J24" s="107" t="s">
         <v>76</v>
       </c>
-      <c r="K24" s="235" t="s">
+      <c r="K24" s="106" t="s">
         <v>269</v>
       </c>
-      <c r="L24" s="232"/>
+      <c r="L24" s="107"/>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" s="33"/>
@@ -14854,8 +14833,8 @@
   </sheetPr>
   <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
@@ -16120,9 +16099,9 @@
   </sheetPr>
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -16233,13 +16212,13 @@
         <v>466</v>
       </c>
       <c r="F3" s="125" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="G3" s="129" t="s">
         <v>60</v>
       </c>
       <c r="H3" s="125" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="I3" s="107" t="s">
         <v>61</v>
@@ -16323,104 +16302,104 @@
       <c r="L5" s="107"/>
     </row>
     <row r="6" spans="1:12" ht="28.8">
-      <c r="A6" s="223" t="s">
+      <c r="A6" s="227" t="s">
         <v>95</v>
       </c>
-      <c r="B6" s="224" t="s">
+      <c r="B6" s="228" t="s">
         <v>96</v>
       </c>
-      <c r="C6" s="223" t="s">
+      <c r="C6" s="227" t="s">
         <v>97</v>
       </c>
       <c r="D6" s="140" t="s">
         <v>98</v>
       </c>
-      <c r="E6" s="225" t="s">
+      <c r="E6" s="229" t="s">
         <v>99</v>
       </c>
-      <c r="F6" s="222" t="s">
+      <c r="F6" s="226" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="222" t="s">
+      <c r="G6" s="226" t="s">
         <v>100</v>
       </c>
-      <c r="H6" s="222" t="s">
+      <c r="H6" s="226" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="226" t="s">
+      <c r="I6" s="224" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="219" t="s">
+      <c r="J6" s="217" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="227" t="s">
+      <c r="K6" s="225" t="s">
         <v>471</v>
       </c>
-      <c r="L6" s="226"/>
+      <c r="L6" s="224"/>
     </row>
     <row r="7" spans="1:12" ht="28.8">
-      <c r="A7" s="223"/>
-      <c r="B7" s="224"/>
-      <c r="C7" s="223"/>
+      <c r="A7" s="227"/>
+      <c r="B7" s="228"/>
+      <c r="C7" s="227"/>
       <c r="D7" s="141" t="s">
         <v>101</v>
       </c>
-      <c r="E7" s="225"/>
-      <c r="F7" s="222"/>
-      <c r="G7" s="222"/>
-      <c r="H7" s="222"/>
-      <c r="I7" s="226"/>
-      <c r="J7" s="219"/>
-      <c r="K7" s="227"/>
-      <c r="L7" s="226"/>
+      <c r="E7" s="229"/>
+      <c r="F7" s="226"/>
+      <c r="G7" s="226"/>
+      <c r="H7" s="226"/>
+      <c r="I7" s="224"/>
+      <c r="J7" s="217"/>
+      <c r="K7" s="225"/>
+      <c r="L7" s="224"/>
     </row>
     <row r="8" spans="1:12" ht="28.8">
-      <c r="A8" s="223"/>
-      <c r="B8" s="224"/>
-      <c r="C8" s="223"/>
+      <c r="A8" s="227"/>
+      <c r="B8" s="228"/>
+      <c r="C8" s="227"/>
       <c r="D8" s="141" t="s">
         <v>102</v>
       </c>
-      <c r="E8" s="225"/>
-      <c r="F8" s="222"/>
-      <c r="G8" s="222"/>
-      <c r="H8" s="222"/>
-      <c r="I8" s="226"/>
-      <c r="J8" s="219"/>
-      <c r="K8" s="227"/>
-      <c r="L8" s="226"/>
+      <c r="E8" s="229"/>
+      <c r="F8" s="226"/>
+      <c r="G8" s="226"/>
+      <c r="H8" s="226"/>
+      <c r="I8" s="224"/>
+      <c r="J8" s="217"/>
+      <c r="K8" s="225"/>
+      <c r="L8" s="224"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="223"/>
-      <c r="B9" s="224"/>
-      <c r="C9" s="223"/>
+      <c r="A9" s="227"/>
+      <c r="B9" s="228"/>
+      <c r="C9" s="227"/>
       <c r="D9" s="141" t="s">
         <v>103</v>
       </c>
-      <c r="E9" s="225"/>
-      <c r="F9" s="222"/>
-      <c r="G9" s="222"/>
-      <c r="H9" s="222"/>
-      <c r="I9" s="226"/>
-      <c r="J9" s="219"/>
-      <c r="K9" s="227"/>
-      <c r="L9" s="226"/>
+      <c r="E9" s="229"/>
+      <c r="F9" s="226"/>
+      <c r="G9" s="226"/>
+      <c r="H9" s="226"/>
+      <c r="I9" s="224"/>
+      <c r="J9" s="217"/>
+      <c r="K9" s="225"/>
+      <c r="L9" s="224"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="223"/>
-      <c r="B10" s="224"/>
-      <c r="C10" s="223"/>
+      <c r="A10" s="227"/>
+      <c r="B10" s="228"/>
+      <c r="C10" s="227"/>
       <c r="D10" s="141" t="s">
         <v>104</v>
       </c>
-      <c r="E10" s="225"/>
-      <c r="F10" s="222"/>
-      <c r="G10" s="222"/>
-      <c r="H10" s="222"/>
-      <c r="I10" s="226"/>
-      <c r="J10" s="219"/>
-      <c r="K10" s="227"/>
-      <c r="L10" s="226"/>
+      <c r="E10" s="229"/>
+      <c r="F10" s="226"/>
+      <c r="G10" s="226"/>
+      <c r="H10" s="226"/>
+      <c r="I10" s="224"/>
+      <c r="J10" s="217"/>
+      <c r="K10" s="225"/>
+      <c r="L10" s="224"/>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="122" t="s">
@@ -16725,17 +16704,17 @@
   </sheetData>
   <autoFilter ref="A1:L15" xr:uid="{FBE7E653-2382-46E4-9C76-9C694EDC9195}"/>
   <mergeCells count="11">
-    <mergeCell ref="L6:L10"/>
-    <mergeCell ref="K6:K10"/>
-    <mergeCell ref="H6:H10"/>
-    <mergeCell ref="I6:I10"/>
-    <mergeCell ref="J6:J10"/>
     <mergeCell ref="G6:G10"/>
     <mergeCell ref="A6:A10"/>
     <mergeCell ref="B6:B10"/>
     <mergeCell ref="C6:C10"/>
     <mergeCell ref="E6:E10"/>
     <mergeCell ref="F6:F10"/>
+    <mergeCell ref="L6:L10"/>
+    <mergeCell ref="K6:K10"/>
+    <mergeCell ref="H6:H10"/>
+    <mergeCell ref="I6:I10"/>
+    <mergeCell ref="J6:J10"/>
   </mergeCells>
   <conditionalFormatting sqref="F2:F6 F11:F15">
     <cfRule type="cellIs" dxfId="127" priority="7" operator="equal">
@@ -18112,15 +18091,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Status xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">Draft</Status>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="221af607-abea-4d5e-830c-567dcc03c0ec" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18367,21 +18343,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Status xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">Draft</Status>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="221af607-abea-4d5e-830c-567dcc03c0ec" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16D2CAB5-B21B-4A93-9D82-49FE3E36CF14}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1A00443-9B7C-473F-A198-CBEB23A0BCC5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cfc87205-1831-4b6c-a7b4-76d40079a43e"/>
-    <ds:schemaRef ds:uri="221af607-abea-4d5e-830c-567dcc03c0ec"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -18406,9 +18382,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1A00443-9B7C-473F-A198-CBEB23A0BCC5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16D2CAB5-B21B-4A93-9D82-49FE3E36CF14}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cfc87205-1831-4b6c-a7b4-76d40079a43e"/>
+    <ds:schemaRef ds:uri="221af607-abea-4d5e-830c-567dcc03c0ec"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix: range endpoint description data service
</commit_message>
<xml_diff>
--- a/Documents/Metadata_CoreGenericHealth_v2.xlsx
+++ b/Documents/Metadata_CoreGenericHealth_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://healthri-my.sharepoint.com/personal/hannah_neikes_health-ri_nl/Documents/Documenten/GitHub/health-ri-metadata/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3208" documentId="13_ncr:1_{F400FBA4-788C-A049-BCFC-7AF7AD8163AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D941DCCA-04DE-4EAA-A3D3-3922BE451E31}"/>
+  <xr:revisionPtr revIDLastSave="3216" documentId="13_ncr:1_{F400FBA4-788C-A049-BCFC-7AF7AD8163AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B34781B7-C461-4DB0-AF31-0C0F180972E1}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-9225" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-12765" windowWidth="38640" windowHeight="21120" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="14" r:id="rId1"/>
@@ -1794,56 +1794,6 @@
     <t>dcat:endpointDescription</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Display"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>Old</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Display"/>
-        <scheme val="major"/>
-      </rPr>
-      <t xml:space="preserve">: A description of the technical details or documentation for accessing the data service's endpoint. It helps users understand how to interact with the service.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Display"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>New</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Display"/>
-        <scheme val="major"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Display"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>Provides technical documentation that explains how to access and interact with the data service’s endpoint.</t>
-    </r>
-  </si>
-  <si>
     <t>access_service:endpoint_description</t>
   </si>
   <si>
@@ -2192,13 +2142,16 @@
   </si>
   <si>
     <t>xsd:hexBinary</t>
+  </si>
+  <si>
+    <t>Provides technical documentation that explains how to access and interact with the data service’s endpoint.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="50">
+  <fonts count="51">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2516,8 +2469,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2584,12 +2543,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -3219,9 +3172,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -3246,43 +3196,46 @@
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="50" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6904,19 +6857,19 @@
     </row>
     <row r="2" spans="1:12" ht="72">
       <c r="A2" s="199" t="s">
+        <v>518</v>
+      </c>
+      <c r="B2" s="45" t="s">
         <v>519</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="C2" s="76" t="s">
         <v>520</v>
-      </c>
-      <c r="C2" s="76" t="s">
-        <v>521</v>
       </c>
       <c r="D2" s="199" t="s">
         <v>25</v>
       </c>
       <c r="E2" s="200" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F2" s="201" t="s">
         <v>17</v>
@@ -6925,7 +6878,7 @@
         <v>75</v>
       </c>
       <c r="H2" s="201" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I2" s="163" t="s">
         <v>19</v>
@@ -6938,13 +6891,13 @@
     </row>
     <row r="3" spans="1:12" ht="28.8">
       <c r="A3" s="68" t="s">
+        <v>523</v>
+      </c>
+      <c r="B3" s="61" t="s">
         <v>524</v>
       </c>
-      <c r="B3" s="61" t="s">
+      <c r="C3" s="77" t="s">
         <v>525</v>
-      </c>
-      <c r="C3" s="77" t="s">
-        <v>526</v>
       </c>
       <c r="D3" s="68" t="s">
         <v>25</v>
@@ -7089,13 +7042,13 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="58" t="s">
+        <v>526</v>
+      </c>
+      <c r="B2" s="44" t="s">
         <v>527</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="C2" s="76" t="s">
         <v>528</v>
-      </c>
-      <c r="C2" s="76" t="s">
-        <v>529</v>
       </c>
       <c r="D2" s="58" t="s">
         <v>25</v>
@@ -7119,13 +7072,13 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="48" t="s">
+        <v>529</v>
+      </c>
+      <c r="B3" s="49" t="s">
         <v>530</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="C3" s="77" t="s">
         <v>531</v>
-      </c>
-      <c r="C3" s="77" t="s">
-        <v>532</v>
       </c>
       <c r="D3" s="48" t="s">
         <v>25</v>
@@ -7787,19 +7740,19 @@
     </row>
     <row r="2" spans="1:12" ht="43.2">
       <c r="A2" s="84" t="s">
+        <v>532</v>
+      </c>
+      <c r="B2" s="44" t="s">
         <v>533</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="C2" s="58" t="s">
         <v>534</v>
-      </c>
-      <c r="C2" s="58" t="s">
-        <v>535</v>
       </c>
       <c r="D2" s="58" t="s">
         <v>25</v>
       </c>
       <c r="E2" s="59" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="F2" s="60" t="s">
         <v>27</v>
@@ -7820,19 +7773,19 @@
     </row>
     <row r="3" spans="1:12" ht="86.4">
       <c r="A3" s="48" t="s">
+        <v>536</v>
+      </c>
+      <c r="B3" s="49" t="s">
         <v>537</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="C3" s="77" t="s">
         <v>538</v>
       </c>
-      <c r="C3" s="77" t="s">
+      <c r="D3" s="115" t="s">
         <v>539</v>
       </c>
-      <c r="D3" s="115" t="s">
+      <c r="E3" s="50" t="s">
         <v>540</v>
-      </c>
-      <c r="E3" s="50" t="s">
-        <v>541</v>
       </c>
       <c r="F3" s="51" t="s">
         <v>27</v>
@@ -7965,19 +7918,19 @@
     </row>
     <row r="2" spans="1:12" ht="158.4">
       <c r="A2" s="84" t="s">
+        <v>541</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>537</v>
+      </c>
+      <c r="C2" s="58" t="s">
+        <v>538</v>
+      </c>
+      <c r="D2" s="59" t="s">
         <v>542</v>
       </c>
-      <c r="B2" s="44" t="s">
-        <v>538</v>
-      </c>
-      <c r="C2" s="58" t="s">
-        <v>539</v>
-      </c>
-      <c r="D2" s="59" t="s">
+      <c r="E2" s="59" t="s">
         <v>543</v>
-      </c>
-      <c r="E2" s="59" t="s">
-        <v>544</v>
       </c>
       <c r="F2" s="60" t="s">
         <v>17</v>
@@ -7998,19 +7951,19 @@
     </row>
     <row r="3" spans="1:12" ht="43.2">
       <c r="A3" s="48" t="s">
+        <v>544</v>
+      </c>
+      <c r="B3" s="49" t="s">
         <v>545</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="C3" s="77" t="s">
         <v>546</v>
-      </c>
-      <c r="C3" s="77" t="s">
-        <v>547</v>
       </c>
       <c r="D3" s="117" t="s">
         <v>25</v>
       </c>
       <c r="E3" s="50" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="F3" s="51" t="s">
         <v>17</v>
@@ -8142,19 +8095,19 @@
     </row>
     <row r="2" spans="1:12" ht="100.8">
       <c r="A2" s="84" t="s">
+        <v>548</v>
+      </c>
+      <c r="B2" s="44" t="s">
         <v>549</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="C2" s="58" t="s">
         <v>550</v>
-      </c>
-      <c r="C2" s="58" t="s">
-        <v>551</v>
       </c>
       <c r="D2" s="58" t="s">
         <v>25</v>
       </c>
       <c r="E2" s="59" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="F2" s="60" t="s">
         <v>27</v>
@@ -8175,19 +8128,19 @@
     </row>
     <row r="3" spans="1:12" ht="57.6">
       <c r="A3" s="48" t="s">
+        <v>552</v>
+      </c>
+      <c r="B3" s="49" t="s">
         <v>553</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="C3" s="77" t="s">
         <v>554</v>
-      </c>
-      <c r="C3" s="77" t="s">
-        <v>555</v>
       </c>
       <c r="D3" s="117" t="s">
         <v>25</v>
       </c>
       <c r="E3" s="50" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F3" s="51" t="s">
         <v>27</v>
@@ -8295,7 +8248,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="56" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E1" s="56" t="s">
         <v>4</v>
@@ -8318,13 +8271,13 @@
     </row>
     <row r="2" spans="1:10" ht="28.8">
       <c r="A2" s="63" t="s">
+        <v>557</v>
+      </c>
+      <c r="B2" s="53" t="s">
         <v>558</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="C2" s="44" t="s">
         <v>559</v>
-      </c>
-      <c r="C2" s="44" t="s">
-        <v>560</v>
       </c>
       <c r="D2" s="43" t="s">
         <v>25</v>
@@ -8332,7 +8285,7 @@
       <c r="E2" s="45"/>
       <c r="F2" s="64"/>
       <c r="G2" s="63" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="H2" s="65" t="s">
         <v>93</v>
@@ -8346,13 +8299,13 @@
     </row>
     <row r="3" spans="1:10" ht="43.2">
       <c r="A3" s="67" t="s">
+        <v>561</v>
+      </c>
+      <c r="B3" s="50" t="s">
         <v>562</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="C3" s="49" t="s">
         <v>563</v>
-      </c>
-      <c r="C3" s="49" t="s">
-        <v>564</v>
       </c>
       <c r="D3" s="48" t="s">
         <v>25</v>
@@ -8360,10 +8313,10 @@
       <c r="E3" s="50"/>
       <c r="F3" s="68"/>
       <c r="G3" s="69" t="s">
+        <v>564</v>
+      </c>
+      <c r="H3" s="48" t="s">
         <v>565</v>
-      </c>
-      <c r="H3" s="48" t="s">
-        <v>566</v>
       </c>
       <c r="I3" s="69" t="s">
         <v>19</v>
@@ -8374,13 +8327,13 @@
     </row>
     <row r="4" spans="1:10" ht="43.2">
       <c r="A4" s="63" t="s">
+        <v>566</v>
+      </c>
+      <c r="B4" s="53" t="s">
         <v>567</v>
       </c>
-      <c r="B4" s="53" t="s">
+      <c r="C4" s="44" t="s">
         <v>568</v>
-      </c>
-      <c r="C4" s="44" t="s">
-        <v>569</v>
       </c>
       <c r="D4" s="43" t="s">
         <v>25</v>
@@ -8388,10 +8341,10 @@
       <c r="E4" s="53"/>
       <c r="F4" s="64"/>
       <c r="G4" s="63" t="s">
+        <v>569</v>
+      </c>
+      <c r="H4" s="65" t="s">
         <v>570</v>
-      </c>
-      <c r="H4" s="65" t="s">
-        <v>571</v>
       </c>
       <c r="I4" s="66" t="s">
         <v>19</v>
@@ -8402,26 +8355,26 @@
     </row>
     <row r="5" spans="1:10" ht="43.2">
       <c r="A5" s="67" t="s">
+        <v>571</v>
+      </c>
+      <c r="B5" s="50" t="s">
         <v>572</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="C5" s="49" t="s">
         <v>573</v>
-      </c>
-      <c r="C5" s="49" t="s">
-        <v>574</v>
       </c>
       <c r="D5" s="48" t="s">
         <v>25</v>
       </c>
       <c r="E5" s="49" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="F5" s="68"/>
       <c r="G5" s="67" t="s">
+        <v>575</v>
+      </c>
+      <c r="H5" s="48" t="s">
         <v>576</v>
-      </c>
-      <c r="H5" s="48" t="s">
-        <v>577</v>
       </c>
       <c r="I5" s="69" t="s">
         <v>19</v>
@@ -8432,13 +8385,13 @@
     </row>
     <row r="6" spans="1:10" ht="28.8">
       <c r="A6" s="63" t="s">
+        <v>577</v>
+      </c>
+      <c r="B6" s="73" t="s">
         <v>578</v>
       </c>
-      <c r="B6" s="73" t="s">
+      <c r="C6" s="44" t="s">
         <v>579</v>
-      </c>
-      <c r="C6" s="44" t="s">
-        <v>580</v>
       </c>
       <c r="D6" s="43" t="s">
         <v>25</v>
@@ -8449,7 +8402,7 @@
         <v>166</v>
       </c>
       <c r="H6" s="65" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="I6" s="66" t="s">
         <v>19</v>
@@ -8460,13 +8413,13 @@
     </row>
     <row r="7" spans="1:10" ht="28.8">
       <c r="A7" s="67" t="s">
+        <v>580</v>
+      </c>
+      <c r="B7" s="50" t="s">
         <v>581</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="C7" s="49" t="s">
         <v>582</v>
-      </c>
-      <c r="C7" s="49" t="s">
-        <v>583</v>
       </c>
       <c r="D7" s="48" t="s">
         <v>25</v>
@@ -8488,23 +8441,23 @@
     </row>
     <row r="8" spans="1:10" ht="86.4">
       <c r="A8" s="63" t="s">
+        <v>583</v>
+      </c>
+      <c r="B8" s="53" t="s">
         <v>584</v>
       </c>
-      <c r="B8" s="53" t="s">
+      <c r="C8" s="44" t="s">
         <v>585</v>
-      </c>
-      <c r="C8" s="44" t="s">
-        <v>586</v>
       </c>
       <c r="D8" s="43" t="s">
         <v>25</v>
       </c>
       <c r="E8" s="71" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F8" s="47"/>
       <c r="G8" s="63" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="H8" s="65">
         <v>1</v>
@@ -8518,13 +8471,13 @@
     </row>
     <row r="9" spans="1:10" ht="28.8">
       <c r="A9" s="67" t="s">
+        <v>588</v>
+      </c>
+      <c r="B9" s="50" t="s">
         <v>589</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="C9" s="49" t="s">
         <v>590</v>
-      </c>
-      <c r="C9" s="49" t="s">
-        <v>591</v>
       </c>
       <c r="D9" s="48" t="s">
         <v>25</v>
@@ -8532,7 +8485,7 @@
       <c r="E9" s="50"/>
       <c r="F9" s="68"/>
       <c r="G9" s="69" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="H9" s="48" t="s">
         <v>93</v>
@@ -8546,23 +8499,23 @@
     </row>
     <row r="10" spans="1:10" ht="28.8">
       <c r="A10" s="63" t="s">
+        <v>592</v>
+      </c>
+      <c r="B10" s="72" t="s">
         <v>593</v>
       </c>
-      <c r="B10" s="72" t="s">
+      <c r="C10" s="44" t="s">
         <v>594</v>
-      </c>
-      <c r="C10" s="44" t="s">
-        <v>595</v>
       </c>
       <c r="D10" s="43" t="s">
         <v>25</v>
       </c>
       <c r="E10" s="72" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="F10" s="64"/>
       <c r="G10" s="63" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H10" s="65" t="s">
         <v>29</v>
@@ -9035,25 +8988,25 @@
     </row>
     <row r="2" spans="1:12" ht="72">
       <c r="A2" s="44" t="s">
+        <v>596</v>
+      </c>
+      <c r="B2" s="57" t="s">
         <v>597</v>
       </c>
-      <c r="B2" s="57" t="s">
+      <c r="C2" s="58" t="s">
         <v>598</v>
       </c>
-      <c r="C2" s="58" t="s">
+      <c r="D2" s="78" t="s">
         <v>599</v>
       </c>
-      <c r="D2" s="78" t="s">
+      <c r="E2" s="200" t="s">
         <v>600</v>
-      </c>
-      <c r="E2" s="200" t="s">
-        <v>601</v>
       </c>
       <c r="F2" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="208" t="s">
-        <v>602</v>
+      <c r="G2" s="207" t="s">
+        <v>601</v>
       </c>
       <c r="H2" s="47">
         <v>1</v>
@@ -9067,13 +9020,13 @@
     </row>
     <row r="3" spans="1:12" ht="71.25" customHeight="1">
       <c r="A3" s="49" t="s">
+        <v>602</v>
+      </c>
+      <c r="B3" s="61" t="s">
         <v>603</v>
       </c>
-      <c r="B3" s="61" t="s">
+      <c r="C3" s="48" t="s">
         <v>604</v>
-      </c>
-      <c r="C3" s="48" t="s">
-        <v>605</v>
       </c>
       <c r="D3" s="50" t="s">
         <v>25</v>
@@ -9083,7 +9036,7 @@
         <v>17</v>
       </c>
       <c r="G3" s="51" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="H3" s="52">
         <v>1</v>
@@ -10094,12 +10047,12 @@
       <c r="J10" s="107" t="s">
         <v>76</v>
       </c>
-      <c r="K10" s="210" t="s">
+      <c r="K10" s="209" t="s">
         <v>77</v>
       </c>
       <c r="L10" s="107"/>
     </row>
-    <row r="11" spans="1:12" s="211" customFormat="1">
+    <row r="11" spans="1:12" s="210" customFormat="1">
       <c r="A11" s="126" t="s">
         <v>78</v>
       </c>
@@ -10206,102 +10159,102 @@
       <c r="L13" s="130"/>
     </row>
     <row r="14" spans="1:12" ht="43.2">
-      <c r="A14" s="220" t="s">
+      <c r="A14" s="216" t="s">
         <v>95</v>
       </c>
-      <c r="B14" s="221" t="s">
+      <c r="B14" s="217" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="220" t="s">
+      <c r="C14" s="216" t="s">
         <v>97</v>
       </c>
       <c r="D14" s="154" t="s">
         <v>98</v>
       </c>
-      <c r="E14" s="222" t="s">
+      <c r="E14" s="219" t="s">
         <v>99</v>
       </c>
-      <c r="F14" s="219" t="s">
+      <c r="F14" s="218" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="219" t="s">
+      <c r="G14" s="218" t="s">
         <v>100</v>
       </c>
-      <c r="H14" s="219" t="s">
+      <c r="H14" s="218" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="217" t="s">
+      <c r="I14" s="220" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="217" t="s">
+      <c r="J14" s="220" t="s">
         <v>30</v>
       </c>
-      <c r="K14" s="218"/>
-      <c r="L14" s="217"/>
+      <c r="K14" s="221"/>
+      <c r="L14" s="220"/>
     </row>
     <row r="15" spans="1:12" ht="43.2">
-      <c r="A15" s="220"/>
-      <c r="B15" s="221"/>
-      <c r="C15" s="220"/>
+      <c r="A15" s="216"/>
+      <c r="B15" s="217"/>
+      <c r="C15" s="216"/>
       <c r="D15" s="155" t="s">
         <v>101</v>
       </c>
-      <c r="E15" s="222"/>
-      <c r="F15" s="219"/>
-      <c r="G15" s="219"/>
-      <c r="H15" s="219"/>
-      <c r="I15" s="217"/>
-      <c r="J15" s="217"/>
-      <c r="K15" s="218"/>
-      <c r="L15" s="217"/>
+      <c r="E15" s="219"/>
+      <c r="F15" s="218"/>
+      <c r="G15" s="218"/>
+      <c r="H15" s="218"/>
+      <c r="I15" s="220"/>
+      <c r="J15" s="220"/>
+      <c r="K15" s="221"/>
+      <c r="L15" s="220"/>
     </row>
     <row r="16" spans="1:12" ht="28.8">
-      <c r="A16" s="220"/>
-      <c r="B16" s="221"/>
-      <c r="C16" s="220"/>
+      <c r="A16" s="216"/>
+      <c r="B16" s="217"/>
+      <c r="C16" s="216"/>
       <c r="D16" s="155" t="s">
         <v>102</v>
       </c>
-      <c r="E16" s="222"/>
-      <c r="F16" s="219"/>
-      <c r="G16" s="219"/>
-      <c r="H16" s="219"/>
-      <c r="I16" s="217"/>
-      <c r="J16" s="217"/>
-      <c r="K16" s="218"/>
-      <c r="L16" s="217"/>
+      <c r="E16" s="219"/>
+      <c r="F16" s="218"/>
+      <c r="G16" s="218"/>
+      <c r="H16" s="218"/>
+      <c r="I16" s="220"/>
+      <c r="J16" s="220"/>
+      <c r="K16" s="221"/>
+      <c r="L16" s="220"/>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="220"/>
-      <c r="B17" s="221"/>
-      <c r="C17" s="220"/>
+      <c r="A17" s="216"/>
+      <c r="B17" s="217"/>
+      <c r="C17" s="216"/>
       <c r="D17" s="155" t="s">
         <v>103</v>
       </c>
-      <c r="E17" s="222"/>
-      <c r="F17" s="219"/>
-      <c r="G17" s="219"/>
-      <c r="H17" s="219"/>
-      <c r="I17" s="217"/>
-      <c r="J17" s="217"/>
-      <c r="K17" s="218"/>
-      <c r="L17" s="217"/>
+      <c r="E17" s="219"/>
+      <c r="F17" s="218"/>
+      <c r="G17" s="218"/>
+      <c r="H17" s="218"/>
+      <c r="I17" s="220"/>
+      <c r="J17" s="220"/>
+      <c r="K17" s="221"/>
+      <c r="L17" s="220"/>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="220"/>
-      <c r="B18" s="221"/>
-      <c r="C18" s="220"/>
+      <c r="A18" s="216"/>
+      <c r="B18" s="217"/>
+      <c r="C18" s="216"/>
       <c r="D18" s="155" t="s">
         <v>104</v>
       </c>
-      <c r="E18" s="222"/>
-      <c r="F18" s="219"/>
-      <c r="G18" s="219"/>
-      <c r="H18" s="219"/>
-      <c r="I18" s="217"/>
-      <c r="J18" s="217"/>
-      <c r="K18" s="218"/>
-      <c r="L18" s="217"/>
+      <c r="E18" s="219"/>
+      <c r="F18" s="218"/>
+      <c r="G18" s="218"/>
+      <c r="H18" s="218"/>
+      <c r="I18" s="220"/>
+      <c r="J18" s="220"/>
+      <c r="K18" s="221"/>
+      <c r="L18" s="220"/>
     </row>
     <row r="19" spans="1:12" ht="28.8">
       <c r="A19" s="126" t="s">
@@ -10334,7 +10287,7 @@
       <c r="J19" s="130" t="s">
         <v>76</v>
       </c>
-      <c r="K19" s="212" t="s">
+      <c r="K19" s="211" t="s">
         <v>110</v>
       </c>
       <c r="L19" s="130"/>
@@ -10388,7 +10341,7 @@
       <c r="D21" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="213" t="s">
+      <c r="E21" s="212" t="s">
         <v>119</v>
       </c>
       <c r="F21" s="128" t="s">
@@ -10476,7 +10429,7 @@
       <c r="J23" s="130" t="s">
         <v>76</v>
       </c>
-      <c r="K23" s="212" t="s">
+      <c r="K23" s="211" t="s">
         <v>131</v>
       </c>
       <c r="L23" s="130"/>
@@ -10548,7 +10501,7 @@
       <c r="J25" s="130" t="s">
         <v>76</v>
       </c>
-      <c r="K25" s="214" t="s">
+      <c r="K25" s="213" t="s">
         <v>143</v>
       </c>
       <c r="L25" s="130"/>
@@ -10890,7 +10843,7 @@
       <c r="D35" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="E35" s="209" t="s">
+      <c r="E35" s="208" t="s">
         <v>200</v>
       </c>
       <c r="F35" s="128" t="s">
@@ -11537,17 +11490,17 @@
     <sortCondition ref="A2:A53"/>
   </sortState>
   <mergeCells count="11">
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="C14:C18"/>
-    <mergeCell ref="F14:F18"/>
-    <mergeCell ref="E14:E18"/>
     <mergeCell ref="L14:L18"/>
     <mergeCell ref="K14:K18"/>
     <mergeCell ref="G14:G18"/>
     <mergeCell ref="H14:H18"/>
     <mergeCell ref="I14:I18"/>
     <mergeCell ref="J14:J18"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="C14:C18"/>
+    <mergeCell ref="F14:F18"/>
+    <mergeCell ref="E14:E18"/>
   </mergeCells>
   <conditionalFormatting sqref="F2:F14 F19:F53">
     <cfRule type="cellIs" dxfId="190" priority="8" operator="equal">
@@ -11919,102 +11872,102 @@
       <c r="L7" s="130"/>
     </row>
     <row r="8" spans="1:12" ht="28.8">
-      <c r="A8" s="220" t="s">
+      <c r="A8" s="216" t="s">
         <v>95</v>
       </c>
-      <c r="B8" s="223" t="s">
+      <c r="B8" s="222" t="s">
         <v>96</v>
       </c>
-      <c r="C8" s="220" t="s">
+      <c r="C8" s="216" t="s">
         <v>97</v>
       </c>
       <c r="D8" s="154" t="s">
         <v>98</v>
       </c>
-      <c r="E8" s="222" t="s">
+      <c r="E8" s="219" t="s">
         <v>307</v>
       </c>
-      <c r="F8" s="219" t="s">
+      <c r="F8" s="218" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="219" t="s">
+      <c r="G8" s="218" t="s">
         <v>100</v>
       </c>
-      <c r="H8" s="219" t="s">
+      <c r="H8" s="218" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="217" t="s">
+      <c r="I8" s="220" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="217" t="s">
+      <c r="J8" s="220" t="s">
         <v>30</v>
       </c>
       <c r="K8" s="138"/>
-      <c r="L8" s="217"/>
+      <c r="L8" s="220"/>
     </row>
     <row r="9" spans="1:12" ht="28.8">
-      <c r="A9" s="220"/>
-      <c r="B9" s="223"/>
-      <c r="C9" s="220"/>
+      <c r="A9" s="216"/>
+      <c r="B9" s="222"/>
+      <c r="C9" s="216"/>
       <c r="D9" s="155" t="s">
         <v>101</v>
       </c>
-      <c r="E9" s="222"/>
-      <c r="F9" s="219"/>
-      <c r="G9" s="219"/>
-      <c r="H9" s="219"/>
-      <c r="I9" s="217"/>
-      <c r="J9" s="217"/>
+      <c r="E9" s="219"/>
+      <c r="F9" s="218"/>
+      <c r="G9" s="218"/>
+      <c r="H9" s="218"/>
+      <c r="I9" s="220"/>
+      <c r="J9" s="220"/>
       <c r="K9" s="138"/>
-      <c r="L9" s="217"/>
+      <c r="L9" s="220"/>
     </row>
     <row r="10" spans="1:12" ht="28.8">
-      <c r="A10" s="220"/>
-      <c r="B10" s="223"/>
-      <c r="C10" s="220"/>
+      <c r="A10" s="216"/>
+      <c r="B10" s="222"/>
+      <c r="C10" s="216"/>
       <c r="D10" s="155" t="s">
         <v>102</v>
       </c>
-      <c r="E10" s="222"/>
-      <c r="F10" s="219"/>
-      <c r="G10" s="219"/>
-      <c r="H10" s="219"/>
-      <c r="I10" s="217"/>
-      <c r="J10" s="217"/>
+      <c r="E10" s="219"/>
+      <c r="F10" s="218"/>
+      <c r="G10" s="218"/>
+      <c r="H10" s="218"/>
+      <c r="I10" s="220"/>
+      <c r="J10" s="220"/>
       <c r="K10" s="138"/>
-      <c r="L10" s="217"/>
+      <c r="L10" s="220"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="220"/>
-      <c r="B11" s="223"/>
-      <c r="C11" s="220"/>
+      <c r="A11" s="216"/>
+      <c r="B11" s="222"/>
+      <c r="C11" s="216"/>
       <c r="D11" s="155" t="s">
         <v>103</v>
       </c>
-      <c r="E11" s="222"/>
-      <c r="F11" s="219"/>
-      <c r="G11" s="219"/>
-      <c r="H11" s="219"/>
-      <c r="I11" s="217"/>
-      <c r="J11" s="217"/>
+      <c r="E11" s="219"/>
+      <c r="F11" s="218"/>
+      <c r="G11" s="218"/>
+      <c r="H11" s="218"/>
+      <c r="I11" s="220"/>
+      <c r="J11" s="220"/>
       <c r="K11" s="156"/>
-      <c r="L11" s="217"/>
+      <c r="L11" s="220"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="220"/>
-      <c r="B12" s="223"/>
-      <c r="C12" s="220"/>
+      <c r="A12" s="216"/>
+      <c r="B12" s="222"/>
+      <c r="C12" s="216"/>
       <c r="D12" s="155" t="s">
         <v>104</v>
       </c>
-      <c r="E12" s="222"/>
-      <c r="F12" s="219"/>
-      <c r="G12" s="219"/>
-      <c r="H12" s="219"/>
-      <c r="I12" s="217"/>
-      <c r="J12" s="217"/>
+      <c r="E12" s="219"/>
+      <c r="F12" s="218"/>
+      <c r="G12" s="218"/>
+      <c r="H12" s="218"/>
+      <c r="I12" s="220"/>
+      <c r="J12" s="220"/>
       <c r="K12" s="138"/>
-      <c r="L12" s="217"/>
+      <c r="L12" s="220"/>
     </row>
     <row r="13" spans="1:12" ht="43.2">
       <c r="A13" s="126" t="s">
@@ -12255,7 +12208,7 @@
       <c r="J19" s="130" t="s">
         <v>76</v>
       </c>
-      <c r="K19" s="212" t="s">
+      <c r="K19" s="211" t="s">
         <v>229</v>
       </c>
       <c r="L19" s="130"/>
@@ -12273,7 +12226,7 @@
       <c r="D20" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="215" t="s">
+      <c r="E20" s="214" t="s">
         <v>328</v>
       </c>
       <c r="F20" s="125" t="s">
@@ -12393,7 +12346,7 @@
       <c r="J23" s="130" t="s">
         <v>76</v>
       </c>
-      <c r="K23" s="212"/>
+      <c r="K23" s="211"/>
       <c r="L23" s="130"/>
     </row>
     <row r="24" spans="1:12" ht="28.8">
@@ -12409,7 +12362,7 @@
       <c r="D24" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="216" t="s">
+      <c r="E24" s="215" t="s">
         <v>338</v>
       </c>
       <c r="F24" s="125" t="s">
@@ -16099,7 +16052,7 @@
   </sheetPr>
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
@@ -16302,104 +16255,104 @@
       <c r="L5" s="107"/>
     </row>
     <row r="6" spans="1:12" ht="28.8">
-      <c r="A6" s="227" t="s">
+      <c r="A6" s="224" t="s">
         <v>95</v>
       </c>
-      <c r="B6" s="228" t="s">
+      <c r="B6" s="225" t="s">
         <v>96</v>
       </c>
-      <c r="C6" s="227" t="s">
+      <c r="C6" s="224" t="s">
         <v>97</v>
       </c>
       <c r="D6" s="140" t="s">
         <v>98</v>
       </c>
-      <c r="E6" s="229" t="s">
+      <c r="E6" s="226" t="s">
         <v>99</v>
       </c>
-      <c r="F6" s="226" t="s">
+      <c r="F6" s="223" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="226" t="s">
+      <c r="G6" s="223" t="s">
         <v>100</v>
       </c>
-      <c r="H6" s="226" t="s">
+      <c r="H6" s="223" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="224" t="s">
+      <c r="I6" s="227" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="217" t="s">
+      <c r="J6" s="220" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="225" t="s">
+      <c r="K6" s="228" t="s">
         <v>471</v>
       </c>
-      <c r="L6" s="224"/>
+      <c r="L6" s="227"/>
     </row>
     <row r="7" spans="1:12" ht="28.8">
-      <c r="A7" s="227"/>
-      <c r="B7" s="228"/>
-      <c r="C7" s="227"/>
+      <c r="A7" s="224"/>
+      <c r="B7" s="225"/>
+      <c r="C7" s="224"/>
       <c r="D7" s="141" t="s">
         <v>101</v>
       </c>
-      <c r="E7" s="229"/>
-      <c r="F7" s="226"/>
-      <c r="G7" s="226"/>
-      <c r="H7" s="226"/>
-      <c r="I7" s="224"/>
-      <c r="J7" s="217"/>
-      <c r="K7" s="225"/>
-      <c r="L7" s="224"/>
+      <c r="E7" s="226"/>
+      <c r="F7" s="223"/>
+      <c r="G7" s="223"/>
+      <c r="H7" s="223"/>
+      <c r="I7" s="227"/>
+      <c r="J7" s="220"/>
+      <c r="K7" s="228"/>
+      <c r="L7" s="227"/>
     </row>
     <row r="8" spans="1:12" ht="28.8">
-      <c r="A8" s="227"/>
-      <c r="B8" s="228"/>
-      <c r="C8" s="227"/>
+      <c r="A8" s="224"/>
+      <c r="B8" s="225"/>
+      <c r="C8" s="224"/>
       <c r="D8" s="141" t="s">
         <v>102</v>
       </c>
-      <c r="E8" s="229"/>
-      <c r="F8" s="226"/>
-      <c r="G8" s="226"/>
-      <c r="H8" s="226"/>
-      <c r="I8" s="224"/>
-      <c r="J8" s="217"/>
-      <c r="K8" s="225"/>
-      <c r="L8" s="224"/>
+      <c r="E8" s="226"/>
+      <c r="F8" s="223"/>
+      <c r="G8" s="223"/>
+      <c r="H8" s="223"/>
+      <c r="I8" s="227"/>
+      <c r="J8" s="220"/>
+      <c r="K8" s="228"/>
+      <c r="L8" s="227"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="227"/>
-      <c r="B9" s="228"/>
-      <c r="C9" s="227"/>
+      <c r="A9" s="224"/>
+      <c r="B9" s="225"/>
+      <c r="C9" s="224"/>
       <c r="D9" s="141" t="s">
         <v>103</v>
       </c>
-      <c r="E9" s="229"/>
-      <c r="F9" s="226"/>
-      <c r="G9" s="226"/>
-      <c r="H9" s="226"/>
-      <c r="I9" s="224"/>
-      <c r="J9" s="217"/>
-      <c r="K9" s="225"/>
-      <c r="L9" s="224"/>
+      <c r="E9" s="226"/>
+      <c r="F9" s="223"/>
+      <c r="G9" s="223"/>
+      <c r="H9" s="223"/>
+      <c r="I9" s="227"/>
+      <c r="J9" s="220"/>
+      <c r="K9" s="228"/>
+      <c r="L9" s="227"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="227"/>
-      <c r="B10" s="228"/>
-      <c r="C10" s="227"/>
+      <c r="A10" s="224"/>
+      <c r="B10" s="225"/>
+      <c r="C10" s="224"/>
       <c r="D10" s="141" t="s">
         <v>104</v>
       </c>
-      <c r="E10" s="229"/>
-      <c r="F10" s="226"/>
-      <c r="G10" s="226"/>
-      <c r="H10" s="226"/>
-      <c r="I10" s="224"/>
-      <c r="J10" s="217"/>
-      <c r="K10" s="225"/>
-      <c r="L10" s="224"/>
+      <c r="E10" s="226"/>
+      <c r="F10" s="223"/>
+      <c r="G10" s="223"/>
+      <c r="H10" s="223"/>
+      <c r="I10" s="227"/>
+      <c r="J10" s="220"/>
+      <c r="K10" s="228"/>
+      <c r="L10" s="227"/>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="122" t="s">
@@ -16704,17 +16657,17 @@
   </sheetData>
   <autoFilter ref="A1:L15" xr:uid="{FBE7E653-2382-46E4-9C76-9C694EDC9195}"/>
   <mergeCells count="11">
+    <mergeCell ref="L6:L10"/>
+    <mergeCell ref="K6:K10"/>
+    <mergeCell ref="H6:H10"/>
+    <mergeCell ref="I6:I10"/>
+    <mergeCell ref="J6:J10"/>
     <mergeCell ref="G6:G10"/>
     <mergeCell ref="A6:A10"/>
     <mergeCell ref="B6:B10"/>
     <mergeCell ref="C6:C10"/>
     <mergeCell ref="E6:E10"/>
     <mergeCell ref="F6:F10"/>
-    <mergeCell ref="L6:L10"/>
-    <mergeCell ref="K6:K10"/>
-    <mergeCell ref="H6:H10"/>
-    <mergeCell ref="I6:I10"/>
-    <mergeCell ref="J6:J10"/>
   </mergeCells>
   <conditionalFormatting sqref="F2:F6 F11:F15">
     <cfRule type="cellIs" dxfId="127" priority="7" operator="equal">
@@ -16806,9 +16759,9 @@
   </sheetPr>
   <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -17103,7 +17056,7 @@
       </c>
       <c r="L8" s="107"/>
     </row>
-    <row r="9" spans="1:12" ht="57.6">
+    <row r="9" spans="1:12" ht="43.2">
       <c r="A9" s="126" t="s">
         <v>488</v>
       </c>
@@ -17116,44 +17069,44 @@
       <c r="D9" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="207" t="s">
-        <v>491</v>
+      <c r="E9" s="229" t="s">
+        <v>606</v>
       </c>
       <c r="F9" s="128" t="s">
         <v>17</v>
       </c>
       <c r="G9" s="128" t="s">
-        <v>75</v>
+        <v>346</v>
       </c>
       <c r="H9" s="128">
         <v>1</v>
       </c>
       <c r="I9" s="130" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="J9" s="107" t="s">
         <v>62</v>
       </c>
       <c r="K9" s="106" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="L9" s="130"/>
     </row>
     <row r="10" spans="1:12" ht="43.2">
       <c r="A10" s="122" t="s">
+        <v>492</v>
+      </c>
+      <c r="B10" s="35" t="s">
         <v>493</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="C10" s="122" t="s">
         <v>494</v>
-      </c>
-      <c r="C10" s="122" t="s">
-        <v>495</v>
       </c>
       <c r="D10" s="133" t="s">
         <v>25</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F10" s="125" t="s">
         <v>17</v>
@@ -17171,7 +17124,7 @@
         <v>62</v>
       </c>
       <c r="K10" s="106" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="L10" s="107"/>
     </row>
@@ -17209,13 +17162,13 @@
     </row>
     <row r="12" spans="1:12" ht="28.8">
       <c r="A12" s="122" t="s">
+        <v>497</v>
+      </c>
+      <c r="B12" s="35" t="s">
         <v>498</v>
       </c>
-      <c r="B12" s="35" t="s">
+      <c r="C12" s="122" t="s">
         <v>499</v>
-      </c>
-      <c r="C12" s="122" t="s">
-        <v>500</v>
       </c>
       <c r="D12" s="133" t="s">
         <v>25</v>
@@ -17253,7 +17206,7 @@
         <v>25</v>
       </c>
       <c r="E13" s="127" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F13" s="128" t="s">
         <v>17</v>
@@ -17307,19 +17260,19 @@
     </row>
     <row r="15" spans="1:12" ht="57.6">
       <c r="A15" s="126" t="s">
+        <v>501</v>
+      </c>
+      <c r="B15" s="74" t="s">
         <v>502</v>
       </c>
-      <c r="B15" s="74" t="s">
+      <c r="C15" s="126" t="s">
         <v>503</v>
-      </c>
-      <c r="C15" s="126" t="s">
-        <v>504</v>
       </c>
       <c r="D15" s="127" t="s">
         <v>25</v>
       </c>
       <c r="E15" s="127" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F15" s="128" t="s">
         <v>27</v>
@@ -17353,7 +17306,7 @@
         <v>140</v>
       </c>
       <c r="E16" s="35" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F16" s="125" t="s">
         <v>27</v>
@@ -17387,7 +17340,7 @@
         <v>320</v>
       </c>
       <c r="E17" s="80" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F17" s="128" t="s">
         <v>17</v>
@@ -17405,7 +17358,7 @@
         <v>62</v>
       </c>
       <c r="K17" s="107" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="L17" s="130"/>
     </row>
@@ -17423,7 +17376,7 @@
         <v>25</v>
       </c>
       <c r="E18" s="35" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F18" s="125" t="s">
         <v>27</v>
@@ -17489,7 +17442,7 @@
         <v>25</v>
       </c>
       <c r="E20" s="35" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F20" s="125" t="s">
         <v>17</v>
@@ -17511,19 +17464,19 @@
     </row>
     <row r="21" spans="1:12" ht="57.6">
       <c r="A21" s="126" t="s">
+        <v>510</v>
+      </c>
+      <c r="B21" s="74" t="s">
         <v>511</v>
       </c>
-      <c r="B21" s="74" t="s">
+      <c r="C21" s="126" t="s">
         <v>512</v>
-      </c>
-      <c r="C21" s="126" t="s">
-        <v>513</v>
       </c>
       <c r="D21" s="127" t="s">
         <v>25</v>
       </c>
       <c r="E21" s="127" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F21" s="128" t="s">
         <v>27</v>
@@ -17541,7 +17494,7 @@
         <v>76</v>
       </c>
       <c r="K21" s="107" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="L21" s="130"/>
     </row>
@@ -17559,7 +17512,7 @@
         <v>266</v>
       </c>
       <c r="E22" s="35" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F22" s="125" t="s">
         <v>17</v>
@@ -17593,7 +17546,7 @@
         <v>25</v>
       </c>
       <c r="E23" s="127" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F23" s="128" t="s">
         <v>17</v>
@@ -17611,7 +17564,7 @@
         <v>76</v>
       </c>
       <c r="K23" s="106" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="L23" s="198"/>
     </row>
@@ -18091,12 +18044,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Status xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">Draft</Status>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="221af607-abea-4d5e-830c-567dcc03c0ec" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18343,21 +18299,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Status xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">Draft</Status>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="221af607-abea-4d5e-830c-567dcc03c0ec" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1A00443-9B7C-473F-A198-CBEB23A0BCC5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16D2CAB5-B21B-4A93-9D82-49FE3E36CF14}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cfc87205-1831-4b6c-a7b4-76d40079a43e"/>
+    <ds:schemaRef ds:uri="221af607-abea-4d5e-830c-567dcc03c0ec"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -18382,12 +18338,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16D2CAB5-B21B-4A93-9D82-49FE3E36CF14}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1A00443-9B7C-473F-A198-CBEB23A0BCC5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cfc87205-1831-4b6c-a7b4-76d40079a43e"/>
-    <ds:schemaRef ds:uri="221af607-abea-4d5e-830c-567dcc03c0ec"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix: range endpoint description data service (#230)
* fix: range endpoint description data service

* fix: example data for data service
</commit_message>
<xml_diff>
--- a/Documents/Metadata_CoreGenericHealth_v2.xlsx
+++ b/Documents/Metadata_CoreGenericHealth_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://healthri-my.sharepoint.com/personal/hannah_neikes_health-ri_nl/Documents/Documenten/GitHub/health-ri-metadata/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3208" documentId="13_ncr:1_{F400FBA4-788C-A049-BCFC-7AF7AD8163AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D941DCCA-04DE-4EAA-A3D3-3922BE451E31}"/>
+  <xr:revisionPtr revIDLastSave="3216" documentId="13_ncr:1_{F400FBA4-788C-A049-BCFC-7AF7AD8163AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B34781B7-C461-4DB0-AF31-0C0F180972E1}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-9225" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-12765" windowWidth="38640" windowHeight="21120" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="14" r:id="rId1"/>
@@ -1794,56 +1794,6 @@
     <t>dcat:endpointDescription</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Display"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>Old</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Display"/>
-        <scheme val="major"/>
-      </rPr>
-      <t xml:space="preserve">: A description of the technical details or documentation for accessing the data service's endpoint. It helps users understand how to interact with the service.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Display"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>New</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Aptos Display"/>
-        <scheme val="major"/>
-      </rPr>
-      <t xml:space="preserve">: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Display"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>Provides technical documentation that explains how to access and interact with the data service’s endpoint.</t>
-    </r>
-  </si>
-  <si>
     <t>access_service:endpoint_description</t>
   </si>
   <si>
@@ -2192,13 +2142,16 @@
   </si>
   <si>
     <t>xsd:hexBinary</t>
+  </si>
+  <si>
+    <t>Provides technical documentation that explains how to access and interact with the data service’s endpoint.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="50">
+  <fonts count="51">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2516,8 +2469,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Display"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2584,12 +2543,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -3219,9 +3172,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -3246,43 +3196,46 @@
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="50" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6904,19 +6857,19 @@
     </row>
     <row r="2" spans="1:12" ht="72">
       <c r="A2" s="199" t="s">
+        <v>518</v>
+      </c>
+      <c r="B2" s="45" t="s">
         <v>519</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="C2" s="76" t="s">
         <v>520</v>
-      </c>
-      <c r="C2" s="76" t="s">
-        <v>521</v>
       </c>
       <c r="D2" s="199" t="s">
         <v>25</v>
       </c>
       <c r="E2" s="200" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F2" s="201" t="s">
         <v>17</v>
@@ -6925,7 +6878,7 @@
         <v>75</v>
       </c>
       <c r="H2" s="201" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="I2" s="163" t="s">
         <v>19</v>
@@ -6938,13 +6891,13 @@
     </row>
     <row r="3" spans="1:12" ht="28.8">
       <c r="A3" s="68" t="s">
+        <v>523</v>
+      </c>
+      <c r="B3" s="61" t="s">
         <v>524</v>
       </c>
-      <c r="B3" s="61" t="s">
+      <c r="C3" s="77" t="s">
         <v>525</v>
-      </c>
-      <c r="C3" s="77" t="s">
-        <v>526</v>
       </c>
       <c r="D3" s="68" t="s">
         <v>25</v>
@@ -7089,13 +7042,13 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" s="58" t="s">
+        <v>526</v>
+      </c>
+      <c r="B2" s="44" t="s">
         <v>527</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="C2" s="76" t="s">
         <v>528</v>
-      </c>
-      <c r="C2" s="76" t="s">
-        <v>529</v>
       </c>
       <c r="D2" s="58" t="s">
         <v>25</v>
@@ -7119,13 +7072,13 @@
     </row>
     <row r="3" spans="1:12">
       <c r="A3" s="48" t="s">
+        <v>529</v>
+      </c>
+      <c r="B3" s="49" t="s">
         <v>530</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="C3" s="77" t="s">
         <v>531</v>
-      </c>
-      <c r="C3" s="77" t="s">
-        <v>532</v>
       </c>
       <c r="D3" s="48" t="s">
         <v>25</v>
@@ -7787,19 +7740,19 @@
     </row>
     <row r="2" spans="1:12" ht="43.2">
       <c r="A2" s="84" t="s">
+        <v>532</v>
+      </c>
+      <c r="B2" s="44" t="s">
         <v>533</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="C2" s="58" t="s">
         <v>534</v>
-      </c>
-      <c r="C2" s="58" t="s">
-        <v>535</v>
       </c>
       <c r="D2" s="58" t="s">
         <v>25</v>
       </c>
       <c r="E2" s="59" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="F2" s="60" t="s">
         <v>27</v>
@@ -7820,19 +7773,19 @@
     </row>
     <row r="3" spans="1:12" ht="86.4">
       <c r="A3" s="48" t="s">
+        <v>536</v>
+      </c>
+      <c r="B3" s="49" t="s">
         <v>537</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="C3" s="77" t="s">
         <v>538</v>
       </c>
-      <c r="C3" s="77" t="s">
+      <c r="D3" s="115" t="s">
         <v>539</v>
       </c>
-      <c r="D3" s="115" t="s">
+      <c r="E3" s="50" t="s">
         <v>540</v>
-      </c>
-      <c r="E3" s="50" t="s">
-        <v>541</v>
       </c>
       <c r="F3" s="51" t="s">
         <v>27</v>
@@ -7965,19 +7918,19 @@
     </row>
     <row r="2" spans="1:12" ht="158.4">
       <c r="A2" s="84" t="s">
+        <v>541</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>537</v>
+      </c>
+      <c r="C2" s="58" t="s">
+        <v>538</v>
+      </c>
+      <c r="D2" s="59" t="s">
         <v>542</v>
       </c>
-      <c r="B2" s="44" t="s">
-        <v>538</v>
-      </c>
-      <c r="C2" s="58" t="s">
-        <v>539</v>
-      </c>
-      <c r="D2" s="59" t="s">
+      <c r="E2" s="59" t="s">
         <v>543</v>
-      </c>
-      <c r="E2" s="59" t="s">
-        <v>544</v>
       </c>
       <c r="F2" s="60" t="s">
         <v>17</v>
@@ -7998,19 +7951,19 @@
     </row>
     <row r="3" spans="1:12" ht="43.2">
       <c r="A3" s="48" t="s">
+        <v>544</v>
+      </c>
+      <c r="B3" s="49" t="s">
         <v>545</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="C3" s="77" t="s">
         <v>546</v>
-      </c>
-      <c r="C3" s="77" t="s">
-        <v>547</v>
       </c>
       <c r="D3" s="117" t="s">
         <v>25</v>
       </c>
       <c r="E3" s="50" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="F3" s="51" t="s">
         <v>17</v>
@@ -8142,19 +8095,19 @@
     </row>
     <row r="2" spans="1:12" ht="100.8">
       <c r="A2" s="84" t="s">
+        <v>548</v>
+      </c>
+      <c r="B2" s="44" t="s">
         <v>549</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="C2" s="58" t="s">
         <v>550</v>
-      </c>
-      <c r="C2" s="58" t="s">
-        <v>551</v>
       </c>
       <c r="D2" s="58" t="s">
         <v>25</v>
       </c>
       <c r="E2" s="59" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="F2" s="60" t="s">
         <v>27</v>
@@ -8175,19 +8128,19 @@
     </row>
     <row r="3" spans="1:12" ht="57.6">
       <c r="A3" s="48" t="s">
+        <v>552</v>
+      </c>
+      <c r="B3" s="49" t="s">
         <v>553</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="C3" s="77" t="s">
         <v>554</v>
-      </c>
-      <c r="C3" s="77" t="s">
-        <v>555</v>
       </c>
       <c r="D3" s="117" t="s">
         <v>25</v>
       </c>
       <c r="E3" s="50" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F3" s="51" t="s">
         <v>27</v>
@@ -8295,7 +8248,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="56" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E1" s="56" t="s">
         <v>4</v>
@@ -8318,13 +8271,13 @@
     </row>
     <row r="2" spans="1:10" ht="28.8">
       <c r="A2" s="63" t="s">
+        <v>557</v>
+      </c>
+      <c r="B2" s="53" t="s">
         <v>558</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="C2" s="44" t="s">
         <v>559</v>
-      </c>
-      <c r="C2" s="44" t="s">
-        <v>560</v>
       </c>
       <c r="D2" s="43" t="s">
         <v>25</v>
@@ -8332,7 +8285,7 @@
       <c r="E2" s="45"/>
       <c r="F2" s="64"/>
       <c r="G2" s="63" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="H2" s="65" t="s">
         <v>93</v>
@@ -8346,13 +8299,13 @@
     </row>
     <row r="3" spans="1:10" ht="43.2">
       <c r="A3" s="67" t="s">
+        <v>561</v>
+      </c>
+      <c r="B3" s="50" t="s">
         <v>562</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="C3" s="49" t="s">
         <v>563</v>
-      </c>
-      <c r="C3" s="49" t="s">
-        <v>564</v>
       </c>
       <c r="D3" s="48" t="s">
         <v>25</v>
@@ -8360,10 +8313,10 @@
       <c r="E3" s="50"/>
       <c r="F3" s="68"/>
       <c r="G3" s="69" t="s">
+        <v>564</v>
+      </c>
+      <c r="H3" s="48" t="s">
         <v>565</v>
-      </c>
-      <c r="H3" s="48" t="s">
-        <v>566</v>
       </c>
       <c r="I3" s="69" t="s">
         <v>19</v>
@@ -8374,13 +8327,13 @@
     </row>
     <row r="4" spans="1:10" ht="43.2">
       <c r="A4" s="63" t="s">
+        <v>566</v>
+      </c>
+      <c r="B4" s="53" t="s">
         <v>567</v>
       </c>
-      <c r="B4" s="53" t="s">
+      <c r="C4" s="44" t="s">
         <v>568</v>
-      </c>
-      <c r="C4" s="44" t="s">
-        <v>569</v>
       </c>
       <c r="D4" s="43" t="s">
         <v>25</v>
@@ -8388,10 +8341,10 @@
       <c r="E4" s="53"/>
       <c r="F4" s="64"/>
       <c r="G4" s="63" t="s">
+        <v>569</v>
+      </c>
+      <c r="H4" s="65" t="s">
         <v>570</v>
-      </c>
-      <c r="H4" s="65" t="s">
-        <v>571</v>
       </c>
       <c r="I4" s="66" t="s">
         <v>19</v>
@@ -8402,26 +8355,26 @@
     </row>
     <row r="5" spans="1:10" ht="43.2">
       <c r="A5" s="67" t="s">
+        <v>571</v>
+      </c>
+      <c r="B5" s="50" t="s">
         <v>572</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="C5" s="49" t="s">
         <v>573</v>
-      </c>
-      <c r="C5" s="49" t="s">
-        <v>574</v>
       </c>
       <c r="D5" s="48" t="s">
         <v>25</v>
       </c>
       <c r="E5" s="49" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="F5" s="68"/>
       <c r="G5" s="67" t="s">
+        <v>575</v>
+      </c>
+      <c r="H5" s="48" t="s">
         <v>576</v>
-      </c>
-      <c r="H5" s="48" t="s">
-        <v>577</v>
       </c>
       <c r="I5" s="69" t="s">
         <v>19</v>
@@ -8432,13 +8385,13 @@
     </row>
     <row r="6" spans="1:10" ht="28.8">
       <c r="A6" s="63" t="s">
+        <v>577</v>
+      </c>
+      <c r="B6" s="73" t="s">
         <v>578</v>
       </c>
-      <c r="B6" s="73" t="s">
+      <c r="C6" s="44" t="s">
         <v>579</v>
-      </c>
-      <c r="C6" s="44" t="s">
-        <v>580</v>
       </c>
       <c r="D6" s="43" t="s">
         <v>25</v>
@@ -8449,7 +8402,7 @@
         <v>166</v>
       </c>
       <c r="H6" s="65" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="I6" s="66" t="s">
         <v>19</v>
@@ -8460,13 +8413,13 @@
     </row>
     <row r="7" spans="1:10" ht="28.8">
       <c r="A7" s="67" t="s">
+        <v>580</v>
+      </c>
+      <c r="B7" s="50" t="s">
         <v>581</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="C7" s="49" t="s">
         <v>582</v>
-      </c>
-      <c r="C7" s="49" t="s">
-        <v>583</v>
       </c>
       <c r="D7" s="48" t="s">
         <v>25</v>
@@ -8488,23 +8441,23 @@
     </row>
     <row r="8" spans="1:10" ht="86.4">
       <c r="A8" s="63" t="s">
+        <v>583</v>
+      </c>
+      <c r="B8" s="53" t="s">
         <v>584</v>
       </c>
-      <c r="B8" s="53" t="s">
+      <c r="C8" s="44" t="s">
         <v>585</v>
-      </c>
-      <c r="C8" s="44" t="s">
-        <v>586</v>
       </c>
       <c r="D8" s="43" t="s">
         <v>25</v>
       </c>
       <c r="E8" s="71" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F8" s="47"/>
       <c r="G8" s="63" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="H8" s="65">
         <v>1</v>
@@ -8518,13 +8471,13 @@
     </row>
     <row r="9" spans="1:10" ht="28.8">
       <c r="A9" s="67" t="s">
+        <v>588</v>
+      </c>
+      <c r="B9" s="50" t="s">
         <v>589</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="C9" s="49" t="s">
         <v>590</v>
-      </c>
-      <c r="C9" s="49" t="s">
-        <v>591</v>
       </c>
       <c r="D9" s="48" t="s">
         <v>25</v>
@@ -8532,7 +8485,7 @@
       <c r="E9" s="50"/>
       <c r="F9" s="68"/>
       <c r="G9" s="69" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="H9" s="48" t="s">
         <v>93</v>
@@ -8546,23 +8499,23 @@
     </row>
     <row r="10" spans="1:10" ht="28.8">
       <c r="A10" s="63" t="s">
+        <v>592</v>
+      </c>
+      <c r="B10" s="72" t="s">
         <v>593</v>
       </c>
-      <c r="B10" s="72" t="s">
+      <c r="C10" s="44" t="s">
         <v>594</v>
-      </c>
-      <c r="C10" s="44" t="s">
-        <v>595</v>
       </c>
       <c r="D10" s="43" t="s">
         <v>25</v>
       </c>
       <c r="E10" s="72" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="F10" s="64"/>
       <c r="G10" s="63" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="H10" s="65" t="s">
         <v>29</v>
@@ -9035,25 +8988,25 @@
     </row>
     <row r="2" spans="1:12" ht="72">
       <c r="A2" s="44" t="s">
+        <v>596</v>
+      </c>
+      <c r="B2" s="57" t="s">
         <v>597</v>
       </c>
-      <c r="B2" s="57" t="s">
+      <c r="C2" s="58" t="s">
         <v>598</v>
       </c>
-      <c r="C2" s="58" t="s">
+      <c r="D2" s="78" t="s">
         <v>599</v>
       </c>
-      <c r="D2" s="78" t="s">
+      <c r="E2" s="200" t="s">
         <v>600</v>
-      </c>
-      <c r="E2" s="200" t="s">
-        <v>601</v>
       </c>
       <c r="F2" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="208" t="s">
-        <v>602</v>
+      <c r="G2" s="207" t="s">
+        <v>601</v>
       </c>
       <c r="H2" s="47">
         <v>1</v>
@@ -9067,13 +9020,13 @@
     </row>
     <row r="3" spans="1:12" ht="71.25" customHeight="1">
       <c r="A3" s="49" t="s">
+        <v>602</v>
+      </c>
+      <c r="B3" s="61" t="s">
         <v>603</v>
       </c>
-      <c r="B3" s="61" t="s">
+      <c r="C3" s="48" t="s">
         <v>604</v>
-      </c>
-      <c r="C3" s="48" t="s">
-        <v>605</v>
       </c>
       <c r="D3" s="50" t="s">
         <v>25</v>
@@ -9083,7 +9036,7 @@
         <v>17</v>
       </c>
       <c r="G3" s="51" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="H3" s="52">
         <v>1</v>
@@ -10094,12 +10047,12 @@
       <c r="J10" s="107" t="s">
         <v>76</v>
       </c>
-      <c r="K10" s="210" t="s">
+      <c r="K10" s="209" t="s">
         <v>77</v>
       </c>
       <c r="L10" s="107"/>
     </row>
-    <row r="11" spans="1:12" s="211" customFormat="1">
+    <row r="11" spans="1:12" s="210" customFormat="1">
       <c r="A11" s="126" t="s">
         <v>78</v>
       </c>
@@ -10206,102 +10159,102 @@
       <c r="L13" s="130"/>
     </row>
     <row r="14" spans="1:12" ht="43.2">
-      <c r="A14" s="220" t="s">
+      <c r="A14" s="216" t="s">
         <v>95</v>
       </c>
-      <c r="B14" s="221" t="s">
+      <c r="B14" s="217" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="220" t="s">
+      <c r="C14" s="216" t="s">
         <v>97</v>
       </c>
       <c r="D14" s="154" t="s">
         <v>98</v>
       </c>
-      <c r="E14" s="222" t="s">
+      <c r="E14" s="219" t="s">
         <v>99</v>
       </c>
-      <c r="F14" s="219" t="s">
+      <c r="F14" s="218" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="219" t="s">
+      <c r="G14" s="218" t="s">
         <v>100</v>
       </c>
-      <c r="H14" s="219" t="s">
+      <c r="H14" s="218" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="217" t="s">
+      <c r="I14" s="220" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="217" t="s">
+      <c r="J14" s="220" t="s">
         <v>30</v>
       </c>
-      <c r="K14" s="218"/>
-      <c r="L14" s="217"/>
+      <c r="K14" s="221"/>
+      <c r="L14" s="220"/>
     </row>
     <row r="15" spans="1:12" ht="43.2">
-      <c r="A15" s="220"/>
-      <c r="B15" s="221"/>
-      <c r="C15" s="220"/>
+      <c r="A15" s="216"/>
+      <c r="B15" s="217"/>
+      <c r="C15" s="216"/>
       <c r="D15" s="155" t="s">
         <v>101</v>
       </c>
-      <c r="E15" s="222"/>
-      <c r="F15" s="219"/>
-      <c r="G15" s="219"/>
-      <c r="H15" s="219"/>
-      <c r="I15" s="217"/>
-      <c r="J15" s="217"/>
-      <c r="K15" s="218"/>
-      <c r="L15" s="217"/>
+      <c r="E15" s="219"/>
+      <c r="F15" s="218"/>
+      <c r="G15" s="218"/>
+      <c r="H15" s="218"/>
+      <c r="I15" s="220"/>
+      <c r="J15" s="220"/>
+      <c r="K15" s="221"/>
+      <c r="L15" s="220"/>
     </row>
     <row r="16" spans="1:12" ht="28.8">
-      <c r="A16" s="220"/>
-      <c r="B16" s="221"/>
-      <c r="C16" s="220"/>
+      <c r="A16" s="216"/>
+      <c r="B16" s="217"/>
+      <c r="C16" s="216"/>
       <c r="D16" s="155" t="s">
         <v>102</v>
       </c>
-      <c r="E16" s="222"/>
-      <c r="F16" s="219"/>
-      <c r="G16" s="219"/>
-      <c r="H16" s="219"/>
-      <c r="I16" s="217"/>
-      <c r="J16" s="217"/>
-      <c r="K16" s="218"/>
-      <c r="L16" s="217"/>
+      <c r="E16" s="219"/>
+      <c r="F16" s="218"/>
+      <c r="G16" s="218"/>
+      <c r="H16" s="218"/>
+      <c r="I16" s="220"/>
+      <c r="J16" s="220"/>
+      <c r="K16" s="221"/>
+      <c r="L16" s="220"/>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="220"/>
-      <c r="B17" s="221"/>
-      <c r="C17" s="220"/>
+      <c r="A17" s="216"/>
+      <c r="B17" s="217"/>
+      <c r="C17" s="216"/>
       <c r="D17" s="155" t="s">
         <v>103</v>
       </c>
-      <c r="E17" s="222"/>
-      <c r="F17" s="219"/>
-      <c r="G17" s="219"/>
-      <c r="H17" s="219"/>
-      <c r="I17" s="217"/>
-      <c r="J17" s="217"/>
-      <c r="K17" s="218"/>
-      <c r="L17" s="217"/>
+      <c r="E17" s="219"/>
+      <c r="F17" s="218"/>
+      <c r="G17" s="218"/>
+      <c r="H17" s="218"/>
+      <c r="I17" s="220"/>
+      <c r="J17" s="220"/>
+      <c r="K17" s="221"/>
+      <c r="L17" s="220"/>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="220"/>
-      <c r="B18" s="221"/>
-      <c r="C18" s="220"/>
+      <c r="A18" s="216"/>
+      <c r="B18" s="217"/>
+      <c r="C18" s="216"/>
       <c r="D18" s="155" t="s">
         <v>104</v>
       </c>
-      <c r="E18" s="222"/>
-      <c r="F18" s="219"/>
-      <c r="G18" s="219"/>
-      <c r="H18" s="219"/>
-      <c r="I18" s="217"/>
-      <c r="J18" s="217"/>
-      <c r="K18" s="218"/>
-      <c r="L18" s="217"/>
+      <c r="E18" s="219"/>
+      <c r="F18" s="218"/>
+      <c r="G18" s="218"/>
+      <c r="H18" s="218"/>
+      <c r="I18" s="220"/>
+      <c r="J18" s="220"/>
+      <c r="K18" s="221"/>
+      <c r="L18" s="220"/>
     </row>
     <row r="19" spans="1:12" ht="28.8">
       <c r="A19" s="126" t="s">
@@ -10334,7 +10287,7 @@
       <c r="J19" s="130" t="s">
         <v>76</v>
       </c>
-      <c r="K19" s="212" t="s">
+      <c r="K19" s="211" t="s">
         <v>110</v>
       </c>
       <c r="L19" s="130"/>
@@ -10388,7 +10341,7 @@
       <c r="D21" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="213" t="s">
+      <c r="E21" s="212" t="s">
         <v>119</v>
       </c>
       <c r="F21" s="128" t="s">
@@ -10476,7 +10429,7 @@
       <c r="J23" s="130" t="s">
         <v>76</v>
       </c>
-      <c r="K23" s="212" t="s">
+      <c r="K23" s="211" t="s">
         <v>131</v>
       </c>
       <c r="L23" s="130"/>
@@ -10548,7 +10501,7 @@
       <c r="J25" s="130" t="s">
         <v>76</v>
       </c>
-      <c r="K25" s="214" t="s">
+      <c r="K25" s="213" t="s">
         <v>143</v>
       </c>
       <c r="L25" s="130"/>
@@ -10890,7 +10843,7 @@
       <c r="D35" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="E35" s="209" t="s">
+      <c r="E35" s="208" t="s">
         <v>200</v>
       </c>
       <c r="F35" s="128" t="s">
@@ -11537,17 +11490,17 @@
     <sortCondition ref="A2:A53"/>
   </sortState>
   <mergeCells count="11">
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="C14:C18"/>
-    <mergeCell ref="F14:F18"/>
-    <mergeCell ref="E14:E18"/>
     <mergeCell ref="L14:L18"/>
     <mergeCell ref="K14:K18"/>
     <mergeCell ref="G14:G18"/>
     <mergeCell ref="H14:H18"/>
     <mergeCell ref="I14:I18"/>
     <mergeCell ref="J14:J18"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="C14:C18"/>
+    <mergeCell ref="F14:F18"/>
+    <mergeCell ref="E14:E18"/>
   </mergeCells>
   <conditionalFormatting sqref="F2:F14 F19:F53">
     <cfRule type="cellIs" dxfId="190" priority="8" operator="equal">
@@ -11919,102 +11872,102 @@
       <c r="L7" s="130"/>
     </row>
     <row r="8" spans="1:12" ht="28.8">
-      <c r="A8" s="220" t="s">
+      <c r="A8" s="216" t="s">
         <v>95</v>
       </c>
-      <c r="B8" s="223" t="s">
+      <c r="B8" s="222" t="s">
         <v>96</v>
       </c>
-      <c r="C8" s="220" t="s">
+      <c r="C8" s="216" t="s">
         <v>97</v>
       </c>
       <c r="D8" s="154" t="s">
         <v>98</v>
       </c>
-      <c r="E8" s="222" t="s">
+      <c r="E8" s="219" t="s">
         <v>307</v>
       </c>
-      <c r="F8" s="219" t="s">
+      <c r="F8" s="218" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="219" t="s">
+      <c r="G8" s="218" t="s">
         <v>100</v>
       </c>
-      <c r="H8" s="219" t="s">
+      <c r="H8" s="218" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="217" t="s">
+      <c r="I8" s="220" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="217" t="s">
+      <c r="J8" s="220" t="s">
         <v>30</v>
       </c>
       <c r="K8" s="138"/>
-      <c r="L8" s="217"/>
+      <c r="L8" s="220"/>
     </row>
     <row r="9" spans="1:12" ht="28.8">
-      <c r="A9" s="220"/>
-      <c r="B9" s="223"/>
-      <c r="C9" s="220"/>
+      <c r="A9" s="216"/>
+      <c r="B9" s="222"/>
+      <c r="C9" s="216"/>
       <c r="D9" s="155" t="s">
         <v>101</v>
       </c>
-      <c r="E9" s="222"/>
-      <c r="F9" s="219"/>
-      <c r="G9" s="219"/>
-      <c r="H9" s="219"/>
-      <c r="I9" s="217"/>
-      <c r="J9" s="217"/>
+      <c r="E9" s="219"/>
+      <c r="F9" s="218"/>
+      <c r="G9" s="218"/>
+      <c r="H9" s="218"/>
+      <c r="I9" s="220"/>
+      <c r="J9" s="220"/>
       <c r="K9" s="138"/>
-      <c r="L9" s="217"/>
+      <c r="L9" s="220"/>
     </row>
     <row r="10" spans="1:12" ht="28.8">
-      <c r="A10" s="220"/>
-      <c r="B10" s="223"/>
-      <c r="C10" s="220"/>
+      <c r="A10" s="216"/>
+      <c r="B10" s="222"/>
+      <c r="C10" s="216"/>
       <c r="D10" s="155" t="s">
         <v>102</v>
       </c>
-      <c r="E10" s="222"/>
-      <c r="F10" s="219"/>
-      <c r="G10" s="219"/>
-      <c r="H10" s="219"/>
-      <c r="I10" s="217"/>
-      <c r="J10" s="217"/>
+      <c r="E10" s="219"/>
+      <c r="F10" s="218"/>
+      <c r="G10" s="218"/>
+      <c r="H10" s="218"/>
+      <c r="I10" s="220"/>
+      <c r="J10" s="220"/>
       <c r="K10" s="138"/>
-      <c r="L10" s="217"/>
+      <c r="L10" s="220"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="220"/>
-      <c r="B11" s="223"/>
-      <c r="C11" s="220"/>
+      <c r="A11" s="216"/>
+      <c r="B11" s="222"/>
+      <c r="C11" s="216"/>
       <c r="D11" s="155" t="s">
         <v>103</v>
       </c>
-      <c r="E11" s="222"/>
-      <c r="F11" s="219"/>
-      <c r="G11" s="219"/>
-      <c r="H11" s="219"/>
-      <c r="I11" s="217"/>
-      <c r="J11" s="217"/>
+      <c r="E11" s="219"/>
+      <c r="F11" s="218"/>
+      <c r="G11" s="218"/>
+      <c r="H11" s="218"/>
+      <c r="I11" s="220"/>
+      <c r="J11" s="220"/>
       <c r="K11" s="156"/>
-      <c r="L11" s="217"/>
+      <c r="L11" s="220"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="220"/>
-      <c r="B12" s="223"/>
-      <c r="C12" s="220"/>
+      <c r="A12" s="216"/>
+      <c r="B12" s="222"/>
+      <c r="C12" s="216"/>
       <c r="D12" s="155" t="s">
         <v>104</v>
       </c>
-      <c r="E12" s="222"/>
-      <c r="F12" s="219"/>
-      <c r="G12" s="219"/>
-      <c r="H12" s="219"/>
-      <c r="I12" s="217"/>
-      <c r="J12" s="217"/>
+      <c r="E12" s="219"/>
+      <c r="F12" s="218"/>
+      <c r="G12" s="218"/>
+      <c r="H12" s="218"/>
+      <c r="I12" s="220"/>
+      <c r="J12" s="220"/>
       <c r="K12" s="138"/>
-      <c r="L12" s="217"/>
+      <c r="L12" s="220"/>
     </row>
     <row r="13" spans="1:12" ht="43.2">
       <c r="A13" s="126" t="s">
@@ -12255,7 +12208,7 @@
       <c r="J19" s="130" t="s">
         <v>76</v>
       </c>
-      <c r="K19" s="212" t="s">
+      <c r="K19" s="211" t="s">
         <v>229</v>
       </c>
       <c r="L19" s="130"/>
@@ -12273,7 +12226,7 @@
       <c r="D20" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="215" t="s">
+      <c r="E20" s="214" t="s">
         <v>328</v>
       </c>
       <c r="F20" s="125" t="s">
@@ -12393,7 +12346,7 @@
       <c r="J23" s="130" t="s">
         <v>76</v>
       </c>
-      <c r="K23" s="212"/>
+      <c r="K23" s="211"/>
       <c r="L23" s="130"/>
     </row>
     <row r="24" spans="1:12" ht="28.8">
@@ -12409,7 +12362,7 @@
       <c r="D24" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="216" t="s">
+      <c r="E24" s="215" t="s">
         <v>338</v>
       </c>
       <c r="F24" s="125" t="s">
@@ -16099,7 +16052,7 @@
   </sheetPr>
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
@@ -16302,104 +16255,104 @@
       <c r="L5" s="107"/>
     </row>
     <row r="6" spans="1:12" ht="28.8">
-      <c r="A6" s="227" t="s">
+      <c r="A6" s="224" t="s">
         <v>95</v>
       </c>
-      <c r="B6" s="228" t="s">
+      <c r="B6" s="225" t="s">
         <v>96</v>
       </c>
-      <c r="C6" s="227" t="s">
+      <c r="C6" s="224" t="s">
         <v>97</v>
       </c>
       <c r="D6" s="140" t="s">
         <v>98</v>
       </c>
-      <c r="E6" s="229" t="s">
+      <c r="E6" s="226" t="s">
         <v>99</v>
       </c>
-      <c r="F6" s="226" t="s">
+      <c r="F6" s="223" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="226" t="s">
+      <c r="G6" s="223" t="s">
         <v>100</v>
       </c>
-      <c r="H6" s="226" t="s">
+      <c r="H6" s="223" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="224" t="s">
+      <c r="I6" s="227" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="217" t="s">
+      <c r="J6" s="220" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="225" t="s">
+      <c r="K6" s="228" t="s">
         <v>471</v>
       </c>
-      <c r="L6" s="224"/>
+      <c r="L6" s="227"/>
     </row>
     <row r="7" spans="1:12" ht="28.8">
-      <c r="A7" s="227"/>
-      <c r="B7" s="228"/>
-      <c r="C7" s="227"/>
+      <c r="A7" s="224"/>
+      <c r="B7" s="225"/>
+      <c r="C7" s="224"/>
       <c r="D7" s="141" t="s">
         <v>101</v>
       </c>
-      <c r="E7" s="229"/>
-      <c r="F7" s="226"/>
-      <c r="G7" s="226"/>
-      <c r="H7" s="226"/>
-      <c r="I7" s="224"/>
-      <c r="J7" s="217"/>
-      <c r="K7" s="225"/>
-      <c r="L7" s="224"/>
+      <c r="E7" s="226"/>
+      <c r="F7" s="223"/>
+      <c r="G7" s="223"/>
+      <c r="H7" s="223"/>
+      <c r="I7" s="227"/>
+      <c r="J7" s="220"/>
+      <c r="K7" s="228"/>
+      <c r="L7" s="227"/>
     </row>
     <row r="8" spans="1:12" ht="28.8">
-      <c r="A8" s="227"/>
-      <c r="B8" s="228"/>
-      <c r="C8" s="227"/>
+      <c r="A8" s="224"/>
+      <c r="B8" s="225"/>
+      <c r="C8" s="224"/>
       <c r="D8" s="141" t="s">
         <v>102</v>
       </c>
-      <c r="E8" s="229"/>
-      <c r="F8" s="226"/>
-      <c r="G8" s="226"/>
-      <c r="H8" s="226"/>
-      <c r="I8" s="224"/>
-      <c r="J8" s="217"/>
-      <c r="K8" s="225"/>
-      <c r="L8" s="224"/>
+      <c r="E8" s="226"/>
+      <c r="F8" s="223"/>
+      <c r="G8" s="223"/>
+      <c r="H8" s="223"/>
+      <c r="I8" s="227"/>
+      <c r="J8" s="220"/>
+      <c r="K8" s="228"/>
+      <c r="L8" s="227"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="227"/>
-      <c r="B9" s="228"/>
-      <c r="C9" s="227"/>
+      <c r="A9" s="224"/>
+      <c r="B9" s="225"/>
+      <c r="C9" s="224"/>
       <c r="D9" s="141" t="s">
         <v>103</v>
       </c>
-      <c r="E9" s="229"/>
-      <c r="F9" s="226"/>
-      <c r="G9" s="226"/>
-      <c r="H9" s="226"/>
-      <c r="I9" s="224"/>
-      <c r="J9" s="217"/>
-      <c r="K9" s="225"/>
-      <c r="L9" s="224"/>
+      <c r="E9" s="226"/>
+      <c r="F9" s="223"/>
+      <c r="G9" s="223"/>
+      <c r="H9" s="223"/>
+      <c r="I9" s="227"/>
+      <c r="J9" s="220"/>
+      <c r="K9" s="228"/>
+      <c r="L9" s="227"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="227"/>
-      <c r="B10" s="228"/>
-      <c r="C10" s="227"/>
+      <c r="A10" s="224"/>
+      <c r="B10" s="225"/>
+      <c r="C10" s="224"/>
       <c r="D10" s="141" t="s">
         <v>104</v>
       </c>
-      <c r="E10" s="229"/>
-      <c r="F10" s="226"/>
-      <c r="G10" s="226"/>
-      <c r="H10" s="226"/>
-      <c r="I10" s="224"/>
-      <c r="J10" s="217"/>
-      <c r="K10" s="225"/>
-      <c r="L10" s="224"/>
+      <c r="E10" s="226"/>
+      <c r="F10" s="223"/>
+      <c r="G10" s="223"/>
+      <c r="H10" s="223"/>
+      <c r="I10" s="227"/>
+      <c r="J10" s="220"/>
+      <c r="K10" s="228"/>
+      <c r="L10" s="227"/>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="122" t="s">
@@ -16704,17 +16657,17 @@
   </sheetData>
   <autoFilter ref="A1:L15" xr:uid="{FBE7E653-2382-46E4-9C76-9C694EDC9195}"/>
   <mergeCells count="11">
+    <mergeCell ref="L6:L10"/>
+    <mergeCell ref="K6:K10"/>
+    <mergeCell ref="H6:H10"/>
+    <mergeCell ref="I6:I10"/>
+    <mergeCell ref="J6:J10"/>
     <mergeCell ref="G6:G10"/>
     <mergeCell ref="A6:A10"/>
     <mergeCell ref="B6:B10"/>
     <mergeCell ref="C6:C10"/>
     <mergeCell ref="E6:E10"/>
     <mergeCell ref="F6:F10"/>
-    <mergeCell ref="L6:L10"/>
-    <mergeCell ref="K6:K10"/>
-    <mergeCell ref="H6:H10"/>
-    <mergeCell ref="I6:I10"/>
-    <mergeCell ref="J6:J10"/>
   </mergeCells>
   <conditionalFormatting sqref="F2:F6 F11:F15">
     <cfRule type="cellIs" dxfId="127" priority="7" operator="equal">
@@ -16806,9 +16759,9 @@
   </sheetPr>
   <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -17103,7 +17056,7 @@
       </c>
       <c r="L8" s="107"/>
     </row>
-    <row r="9" spans="1:12" ht="57.6">
+    <row r="9" spans="1:12" ht="43.2">
       <c r="A9" s="126" t="s">
         <v>488</v>
       </c>
@@ -17116,44 +17069,44 @@
       <c r="D9" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="207" t="s">
-        <v>491</v>
+      <c r="E9" s="229" t="s">
+        <v>606</v>
       </c>
       <c r="F9" s="128" t="s">
         <v>17</v>
       </c>
       <c r="G9" s="128" t="s">
-        <v>75</v>
+        <v>346</v>
       </c>
       <c r="H9" s="128">
         <v>1</v>
       </c>
       <c r="I9" s="130" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="J9" s="107" t="s">
         <v>62</v>
       </c>
       <c r="K9" s="106" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="L9" s="130"/>
     </row>
     <row r="10" spans="1:12" ht="43.2">
       <c r="A10" s="122" t="s">
+        <v>492</v>
+      </c>
+      <c r="B10" s="35" t="s">
         <v>493</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="C10" s="122" t="s">
         <v>494</v>
-      </c>
-      <c r="C10" s="122" t="s">
-        <v>495</v>
       </c>
       <c r="D10" s="133" t="s">
         <v>25</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F10" s="125" t="s">
         <v>17</v>
@@ -17171,7 +17124,7 @@
         <v>62</v>
       </c>
       <c r="K10" s="106" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="L10" s="107"/>
     </row>
@@ -17209,13 +17162,13 @@
     </row>
     <row r="12" spans="1:12" ht="28.8">
       <c r="A12" s="122" t="s">
+        <v>497</v>
+      </c>
+      <c r="B12" s="35" t="s">
         <v>498</v>
       </c>
-      <c r="B12" s="35" t="s">
+      <c r="C12" s="122" t="s">
         <v>499</v>
-      </c>
-      <c r="C12" s="122" t="s">
-        <v>500</v>
       </c>
       <c r="D12" s="133" t="s">
         <v>25</v>
@@ -17253,7 +17206,7 @@
         <v>25</v>
       </c>
       <c r="E13" s="127" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F13" s="128" t="s">
         <v>17</v>
@@ -17307,19 +17260,19 @@
     </row>
     <row r="15" spans="1:12" ht="57.6">
       <c r="A15" s="126" t="s">
+        <v>501</v>
+      </c>
+      <c r="B15" s="74" t="s">
         <v>502</v>
       </c>
-      <c r="B15" s="74" t="s">
+      <c r="C15" s="126" t="s">
         <v>503</v>
-      </c>
-      <c r="C15" s="126" t="s">
-        <v>504</v>
       </c>
       <c r="D15" s="127" t="s">
         <v>25</v>
       </c>
       <c r="E15" s="127" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F15" s="128" t="s">
         <v>27</v>
@@ -17353,7 +17306,7 @@
         <v>140</v>
       </c>
       <c r="E16" s="35" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F16" s="125" t="s">
         <v>27</v>
@@ -17387,7 +17340,7 @@
         <v>320</v>
       </c>
       <c r="E17" s="80" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F17" s="128" t="s">
         <v>17</v>
@@ -17405,7 +17358,7 @@
         <v>62</v>
       </c>
       <c r="K17" s="107" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="L17" s="130"/>
     </row>
@@ -17423,7 +17376,7 @@
         <v>25</v>
       </c>
       <c r="E18" s="35" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F18" s="125" t="s">
         <v>27</v>
@@ -17489,7 +17442,7 @@
         <v>25</v>
       </c>
       <c r="E20" s="35" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F20" s="125" t="s">
         <v>17</v>
@@ -17511,19 +17464,19 @@
     </row>
     <row r="21" spans="1:12" ht="57.6">
       <c r="A21" s="126" t="s">
+        <v>510</v>
+      </c>
+      <c r="B21" s="74" t="s">
         <v>511</v>
       </c>
-      <c r="B21" s="74" t="s">
+      <c r="C21" s="126" t="s">
         <v>512</v>
-      </c>
-      <c r="C21" s="126" t="s">
-        <v>513</v>
       </c>
       <c r="D21" s="127" t="s">
         <v>25</v>
       </c>
       <c r="E21" s="127" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F21" s="128" t="s">
         <v>27</v>
@@ -17541,7 +17494,7 @@
         <v>76</v>
       </c>
       <c r="K21" s="107" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="L21" s="130"/>
     </row>
@@ -17559,7 +17512,7 @@
         <v>266</v>
       </c>
       <c r="E22" s="35" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F22" s="125" t="s">
         <v>17</v>
@@ -17593,7 +17546,7 @@
         <v>25</v>
       </c>
       <c r="E23" s="127" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F23" s="128" t="s">
         <v>17</v>
@@ -17611,7 +17564,7 @@
         <v>76</v>
       </c>
       <c r="K23" s="106" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="L23" s="198"/>
     </row>
@@ -18091,12 +18044,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Status xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">Draft</Status>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="221af607-abea-4d5e-830c-567dcc03c0ec" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18343,21 +18299,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Status xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">Draft</Status>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="221af607-abea-4d5e-830c-567dcc03c0ec" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1A00443-9B7C-473F-A198-CBEB23A0BCC5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16D2CAB5-B21B-4A93-9D82-49FE3E36CF14}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cfc87205-1831-4b6c-a7b4-76d40079a43e"/>
+    <ds:schemaRef ds:uri="221af607-abea-4d5e-830c-567dcc03c0ec"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -18382,12 +18338,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16D2CAB5-B21B-4A93-9D82-49FE3E36CF14}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1A00443-9B7C-473F-A198-CBEB23A0BCC5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cfc87205-1831-4b6c-a7b4-76d40079a43e"/>
-    <ds:schemaRef ds:uri="221af607-abea-4d5e-830c-567dcc03c0ec"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix: URLs to spatial EU vocabs
</commit_message>
<xml_diff>
--- a/Documents/Metadata_CoreGenericHealth_v2.xlsx
+++ b/Documents/Metadata_CoreGenericHealth_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://healthri-my.sharepoint.com/personal/hannah_neikes_health-ri_nl/Documents/Documenten/GitHub/health-ri-metadata/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3216" documentId="13_ncr:1_{F400FBA4-788C-A049-BCFC-7AF7AD8163AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B34781B7-C461-4DB0-AF31-0C0F180972E1}"/>
+  <xr:revisionPtr revIDLastSave="3225" documentId="13_ncr:1_{F400FBA4-788C-A049-BCFC-7AF7AD8163AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC6F41C7-8696-4345-9896-16B847EC9B3E}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-12765" windowWidth="38640" windowHeight="21120" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4680" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="14" r:id="rId1"/>
@@ -2566,7 +2566,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="230">
+  <cellXfs count="232">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2980,9 +2980,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3020,9 +3017,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3195,28 +3189,37 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="50" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3228,14 +3231,17 @@
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6817,7 +6823,7 @@
     <col min="11" max="11" width="22.33203125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="206" customFormat="1" ht="43.2">
+    <row r="1" spans="1:12" s="204" customFormat="1" ht="43.2">
       <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
@@ -6848,7 +6854,7 @@
       <c r="J1" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="203" t="s">
+      <c r="K1" s="201" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="108" t="s">
@@ -6856,7 +6862,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="72">
-      <c r="A2" s="199" t="s">
+      <c r="A2" s="197" t="s">
         <v>518</v>
       </c>
       <c r="B2" s="45" t="s">
@@ -6865,29 +6871,29 @@
       <c r="C2" s="76" t="s">
         <v>520</v>
       </c>
-      <c r="D2" s="199" t="s">
+      <c r="D2" s="197" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="200" t="s">
+      <c r="E2" s="198" t="s">
         <v>521</v>
       </c>
-      <c r="F2" s="201" t="s">
+      <c r="F2" s="199" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="162" t="s">
+      <c r="G2" s="160" t="s">
         <v>75</v>
       </c>
-      <c r="H2" s="201" t="s">
+      <c r="H2" s="199" t="s">
         <v>522</v>
       </c>
-      <c r="I2" s="163" t="s">
+      <c r="I2" s="161" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="163" t="s">
+      <c r="J2" s="161" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="159"/>
-      <c r="L2" s="189"/>
+      <c r="K2" s="157"/>
+      <c r="L2" s="187"/>
     </row>
     <row r="3" spans="1:12" ht="28.8">
       <c r="A3" s="68" t="s">
@@ -6902,24 +6908,24 @@
       <c r="D3" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="165"/>
-      <c r="F3" s="166" t="s">
+      <c r="E3" s="163"/>
+      <c r="F3" s="164" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="166" t="s">
+      <c r="G3" s="164" t="s">
         <v>75</v>
       </c>
-      <c r="H3" s="166" t="s">
+      <c r="H3" s="164" t="s">
         <v>93</v>
       </c>
-      <c r="I3" s="167" t="s">
+      <c r="I3" s="165" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="163" t="s">
+      <c r="J3" s="161" t="s">
         <v>76</v>
       </c>
-      <c r="K3" s="170"/>
-      <c r="L3" s="198"/>
+      <c r="K3" s="168"/>
+      <c r="L3" s="196"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F3">
@@ -8999,13 +9005,13 @@
       <c r="D2" s="78" t="s">
         <v>599</v>
       </c>
-      <c r="E2" s="200" t="s">
+      <c r="E2" s="198" t="s">
         <v>600</v>
       </c>
       <c r="F2" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="207" t="s">
+      <c r="G2" s="205" t="s">
         <v>601</v>
       </c>
       <c r="H2" s="47">
@@ -9669,8 +9675,8 @@
   <dimension ref="A1:L53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -9690,7 +9696,7 @@
     <col min="13" max="16384" width="9.109375" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="202" customFormat="1" ht="41.4">
+    <row r="1" spans="1:12" s="200" customFormat="1" ht="41.4">
       <c r="A1" s="91" t="s">
         <v>0</v>
       </c>
@@ -10047,12 +10053,12 @@
       <c r="J10" s="107" t="s">
         <v>76</v>
       </c>
-      <c r="K10" s="209" t="s">
+      <c r="K10" s="207" t="s">
         <v>77</v>
       </c>
       <c r="L10" s="107"/>
     </row>
-    <row r="11" spans="1:12" s="210" customFormat="1">
+    <row r="11" spans="1:12" s="208" customFormat="1">
       <c r="A11" s="126" t="s">
         <v>78</v>
       </c>
@@ -10065,7 +10071,7 @@
       <c r="D11" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="142" t="s">
+      <c r="E11" s="141" t="s">
         <v>81</v>
       </c>
       <c r="F11" s="128" t="s">
@@ -10132,7 +10138,7 @@
       <c r="C13" s="126" t="s">
         <v>90</v>
       </c>
-      <c r="D13" s="144" t="s">
+      <c r="D13" s="143" t="s">
         <v>91</v>
       </c>
       <c r="E13" s="80" t="s">
@@ -10159,102 +10165,102 @@
       <c r="L13" s="130"/>
     </row>
     <row r="14" spans="1:12" ht="43.2">
-      <c r="A14" s="216" t="s">
+      <c r="A14" s="218" t="s">
         <v>95</v>
       </c>
-      <c r="B14" s="217" t="s">
+      <c r="B14" s="219" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="216" t="s">
+      <c r="C14" s="218" t="s">
         <v>97</v>
       </c>
-      <c r="D14" s="154" t="s">
+      <c r="D14" s="228" t="s">
         <v>98</v>
       </c>
-      <c r="E14" s="219" t="s">
+      <c r="E14" s="220" t="s">
         <v>99</v>
       </c>
-      <c r="F14" s="218" t="s">
+      <c r="F14" s="217" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="218" t="s">
+      <c r="G14" s="217" t="s">
         <v>100</v>
       </c>
-      <c r="H14" s="218" t="s">
+      <c r="H14" s="217" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="220" t="s">
+      <c r="I14" s="215" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="220" t="s">
+      <c r="J14" s="215" t="s">
         <v>30</v>
       </c>
-      <c r="K14" s="221"/>
-      <c r="L14" s="220"/>
+      <c r="K14" s="216"/>
+      <c r="L14" s="215"/>
     </row>
     <row r="15" spans="1:12" ht="43.2">
-      <c r="A15" s="216"/>
-      <c r="B15" s="217"/>
-      <c r="C15" s="216"/>
-      <c r="D15" s="155" t="s">
+      <c r="A15" s="218"/>
+      <c r="B15" s="219"/>
+      <c r="C15" s="218"/>
+      <c r="D15" s="229" t="s">
         <v>101</v>
       </c>
-      <c r="E15" s="219"/>
-      <c r="F15" s="218"/>
-      <c r="G15" s="218"/>
-      <c r="H15" s="218"/>
-      <c r="I15" s="220"/>
-      <c r="J15" s="220"/>
-      <c r="K15" s="221"/>
-      <c r="L15" s="220"/>
+      <c r="E15" s="220"/>
+      <c r="F15" s="217"/>
+      <c r="G15" s="217"/>
+      <c r="H15" s="217"/>
+      <c r="I15" s="215"/>
+      <c r="J15" s="215"/>
+      <c r="K15" s="216"/>
+      <c r="L15" s="215"/>
     </row>
     <row r="16" spans="1:12" ht="28.8">
-      <c r="A16" s="216"/>
-      <c r="B16" s="217"/>
-      <c r="C16" s="216"/>
-      <c r="D16" s="155" t="s">
+      <c r="A16" s="218"/>
+      <c r="B16" s="219"/>
+      <c r="C16" s="218"/>
+      <c r="D16" s="229" t="s">
         <v>102</v>
       </c>
-      <c r="E16" s="219"/>
-      <c r="F16" s="218"/>
-      <c r="G16" s="218"/>
-      <c r="H16" s="218"/>
-      <c r="I16" s="220"/>
-      <c r="J16" s="220"/>
-      <c r="K16" s="221"/>
-      <c r="L16" s="220"/>
+      <c r="E16" s="220"/>
+      <c r="F16" s="217"/>
+      <c r="G16" s="217"/>
+      <c r="H16" s="217"/>
+      <c r="I16" s="215"/>
+      <c r="J16" s="215"/>
+      <c r="K16" s="216"/>
+      <c r="L16" s="215"/>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="216"/>
-      <c r="B17" s="217"/>
-      <c r="C17" s="216"/>
-      <c r="D17" s="155" t="s">
+      <c r="A17" s="218"/>
+      <c r="B17" s="219"/>
+      <c r="C17" s="218"/>
+      <c r="D17" s="153" t="s">
         <v>103</v>
       </c>
-      <c r="E17" s="219"/>
-      <c r="F17" s="218"/>
-      <c r="G17" s="218"/>
-      <c r="H17" s="218"/>
-      <c r="I17" s="220"/>
-      <c r="J17" s="220"/>
-      <c r="K17" s="221"/>
-      <c r="L17" s="220"/>
+      <c r="E17" s="220"/>
+      <c r="F17" s="217"/>
+      <c r="G17" s="217"/>
+      <c r="H17" s="217"/>
+      <c r="I17" s="215"/>
+      <c r="J17" s="215"/>
+      <c r="K17" s="216"/>
+      <c r="L17" s="215"/>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="216"/>
-      <c r="B18" s="217"/>
-      <c r="C18" s="216"/>
-      <c r="D18" s="155" t="s">
+      <c r="A18" s="218"/>
+      <c r="B18" s="219"/>
+      <c r="C18" s="218"/>
+      <c r="D18" s="153" t="s">
         <v>104</v>
       </c>
-      <c r="E18" s="219"/>
-      <c r="F18" s="218"/>
-      <c r="G18" s="218"/>
-      <c r="H18" s="218"/>
-      <c r="I18" s="220"/>
-      <c r="J18" s="220"/>
-      <c r="K18" s="221"/>
-      <c r="L18" s="220"/>
+      <c r="E18" s="220"/>
+      <c r="F18" s="217"/>
+      <c r="G18" s="217"/>
+      <c r="H18" s="217"/>
+      <c r="I18" s="215"/>
+      <c r="J18" s="215"/>
+      <c r="K18" s="216"/>
+      <c r="L18" s="215"/>
     </row>
     <row r="19" spans="1:12" ht="28.8">
       <c r="A19" s="126" t="s">
@@ -10287,7 +10293,7 @@
       <c r="J19" s="130" t="s">
         <v>76</v>
       </c>
-      <c r="K19" s="211" t="s">
+      <c r="K19" s="209" t="s">
         <v>110</v>
       </c>
       <c r="L19" s="130"/>
@@ -10341,7 +10347,7 @@
       <c r="D21" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="212" t="s">
+      <c r="E21" s="210" t="s">
         <v>119</v>
       </c>
       <c r="F21" s="128" t="s">
@@ -10429,7 +10435,7 @@
       <c r="J23" s="130" t="s">
         <v>76</v>
       </c>
-      <c r="K23" s="211" t="s">
+      <c r="K23" s="209" t="s">
         <v>131</v>
       </c>
       <c r="L23" s="130"/>
@@ -10441,7 +10447,7 @@
       <c r="B24" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="C24" s="143" t="s">
+      <c r="C24" s="142" t="s">
         <v>134</v>
       </c>
       <c r="D24" s="133" t="s">
@@ -10480,7 +10486,7 @@
       <c r="C25" s="135" t="s">
         <v>139</v>
       </c>
-      <c r="D25" s="144" t="s">
+      <c r="D25" s="143" t="s">
         <v>140</v>
       </c>
       <c r="E25" s="127" t="s">
@@ -10501,7 +10507,7 @@
       <c r="J25" s="130" t="s">
         <v>76</v>
       </c>
-      <c r="K25" s="213" t="s">
+      <c r="K25" s="211" t="s">
         <v>143</v>
       </c>
       <c r="L25" s="130"/>
@@ -10513,7 +10519,7 @@
       <c r="B26" s="35" t="s">
         <v>145</v>
       </c>
-      <c r="C26" s="143" t="s">
+      <c r="C26" s="142" t="s">
         <v>146</v>
       </c>
       <c r="D26" s="123" t="s">
@@ -10585,7 +10591,7 @@
       <c r="B28" s="35" t="s">
         <v>158</v>
       </c>
-      <c r="C28" s="143" t="s">
+      <c r="C28" s="142" t="s">
         <v>159</v>
       </c>
       <c r="D28" s="133" t="s">
@@ -10768,7 +10774,7 @@
       <c r="C33" s="126" t="s">
         <v>187</v>
       </c>
-      <c r="D33" s="144" t="s">
+      <c r="D33" s="143" t="s">
         <v>188</v>
       </c>
       <c r="E33" s="80" t="s">
@@ -10843,7 +10849,7 @@
       <c r="D35" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="E35" s="208" t="s">
+      <c r="E35" s="206" t="s">
         <v>200</v>
       </c>
       <c r="F35" s="128" t="s">
@@ -11160,7 +11166,7 @@
       <c r="C44" s="122" t="s">
         <v>248</v>
       </c>
-      <c r="D44" s="184" t="s">
+      <c r="D44" s="182" t="s">
         <v>249</v>
       </c>
       <c r="E44" s="133" t="s">
@@ -11229,7 +11235,7 @@
       <c r="B46" s="35" t="s">
         <v>258</v>
       </c>
-      <c r="C46" s="143" t="s">
+      <c r="C46" s="142" t="s">
         <v>259</v>
       </c>
       <c r="D46" s="133" t="s">
@@ -11268,7 +11274,7 @@
       <c r="C47" s="126" t="s">
         <v>265</v>
       </c>
-      <c r="D47" s="144" t="s">
+      <c r="D47" s="143" t="s">
         <v>266</v>
       </c>
       <c r="E47" s="74" t="s">
@@ -11340,7 +11346,7 @@
       <c r="C49" s="126" t="s">
         <v>275</v>
       </c>
-      <c r="D49" s="188" t="s">
+      <c r="D49" s="186" t="s">
         <v>276</v>
       </c>
       <c r="E49" s="83" t="s">
@@ -11471,18 +11477,18 @@
       <c r="L52" s="107"/>
     </row>
     <row r="53" spans="1:12" s="119" customFormat="1">
-      <c r="A53" s="147"/>
-      <c r="B53" s="148"/>
-      <c r="C53" s="147"/>
-      <c r="D53" s="149"/>
-      <c r="E53" s="149"/>
-      <c r="F53" s="150"/>
-      <c r="G53" s="150"/>
-      <c r="H53" s="150"/>
-      <c r="I53" s="151"/>
-      <c r="J53" s="151"/>
-      <c r="K53" s="152"/>
-      <c r="L53" s="151"/>
+      <c r="A53" s="146"/>
+      <c r="B53" s="147"/>
+      <c r="C53" s="146"/>
+      <c r="D53" s="148"/>
+      <c r="E53" s="148"/>
+      <c r="F53" s="149"/>
+      <c r="G53" s="149"/>
+      <c r="H53" s="149"/>
+      <c r="I53" s="150"/>
+      <c r="J53" s="150"/>
+      <c r="K53" s="151"/>
+      <c r="L53" s="150"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J53" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
@@ -11490,17 +11496,17 @@
     <sortCondition ref="A2:A53"/>
   </sortState>
   <mergeCells count="11">
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="C14:C18"/>
+    <mergeCell ref="F14:F18"/>
+    <mergeCell ref="E14:E18"/>
     <mergeCell ref="L14:L18"/>
     <mergeCell ref="K14:K18"/>
     <mergeCell ref="G14:G18"/>
     <mergeCell ref="H14:H18"/>
     <mergeCell ref="I14:I18"/>
     <mergeCell ref="J14:J18"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="C14:C18"/>
-    <mergeCell ref="F14:F18"/>
-    <mergeCell ref="E14:E18"/>
   </mergeCells>
   <conditionalFormatting sqref="F2:F14 F19:F53">
     <cfRule type="cellIs" dxfId="190" priority="8" operator="equal">
@@ -11605,7 +11611,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N16" sqref="N16"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -11625,7 +11631,7 @@
     <col min="13" max="16384" width="9.109375" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="202" customFormat="1" ht="57.6">
+    <row r="1" spans="1:12" s="200" customFormat="1" ht="57.6">
       <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
@@ -11670,7 +11676,7 @@
       <c r="B2" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="143" t="s">
+      <c r="C2" s="142" t="s">
         <v>34</v>
       </c>
       <c r="D2" s="133" t="s">
@@ -11872,102 +11878,102 @@
       <c r="L7" s="130"/>
     </row>
     <row r="8" spans="1:12" ht="28.8">
-      <c r="A8" s="216" t="s">
+      <c r="A8" s="218" t="s">
         <v>95</v>
       </c>
-      <c r="B8" s="222" t="s">
+      <c r="B8" s="221" t="s">
         <v>96</v>
       </c>
-      <c r="C8" s="216" t="s">
+      <c r="C8" s="218" t="s">
         <v>97</v>
       </c>
-      <c r="D8" s="154" t="s">
+      <c r="D8" s="228" t="s">
         <v>98</v>
       </c>
-      <c r="E8" s="219" t="s">
+      <c r="E8" s="220" t="s">
         <v>307</v>
       </c>
-      <c r="F8" s="218" t="s">
+      <c r="F8" s="217" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="218" t="s">
+      <c r="G8" s="217" t="s">
         <v>100</v>
       </c>
-      <c r="H8" s="218" t="s">
+      <c r="H8" s="217" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="220" t="s">
+      <c r="I8" s="215" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="220" t="s">
+      <c r="J8" s="215" t="s">
         <v>30</v>
       </c>
       <c r="K8" s="138"/>
-      <c r="L8" s="220"/>
+      <c r="L8" s="215"/>
     </row>
     <row r="9" spans="1:12" ht="28.8">
-      <c r="A9" s="216"/>
-      <c r="B9" s="222"/>
-      <c r="C9" s="216"/>
-      <c r="D9" s="155" t="s">
+      <c r="A9" s="218"/>
+      <c r="B9" s="221"/>
+      <c r="C9" s="218"/>
+      <c r="D9" s="229" t="s">
         <v>101</v>
       </c>
-      <c r="E9" s="219"/>
-      <c r="F9" s="218"/>
-      <c r="G9" s="218"/>
-      <c r="H9" s="218"/>
-      <c r="I9" s="220"/>
-      <c r="J9" s="220"/>
+      <c r="E9" s="220"/>
+      <c r="F9" s="217"/>
+      <c r="G9" s="217"/>
+      <c r="H9" s="217"/>
+      <c r="I9" s="215"/>
+      <c r="J9" s="215"/>
       <c r="K9" s="138"/>
-      <c r="L9" s="220"/>
+      <c r="L9" s="215"/>
     </row>
     <row r="10" spans="1:12" ht="28.8">
-      <c r="A10" s="216"/>
-      <c r="B10" s="222"/>
-      <c r="C10" s="216"/>
-      <c r="D10" s="155" t="s">
+      <c r="A10" s="218"/>
+      <c r="B10" s="221"/>
+      <c r="C10" s="218"/>
+      <c r="D10" s="229" t="s">
         <v>102</v>
       </c>
-      <c r="E10" s="219"/>
-      <c r="F10" s="218"/>
-      <c r="G10" s="218"/>
-      <c r="H10" s="218"/>
-      <c r="I10" s="220"/>
-      <c r="J10" s="220"/>
+      <c r="E10" s="220"/>
+      <c r="F10" s="217"/>
+      <c r="G10" s="217"/>
+      <c r="H10" s="217"/>
+      <c r="I10" s="215"/>
+      <c r="J10" s="215"/>
       <c r="K10" s="138"/>
-      <c r="L10" s="220"/>
+      <c r="L10" s="215"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="216"/>
-      <c r="B11" s="222"/>
-      <c r="C11" s="216"/>
-      <c r="D11" s="155" t="s">
+      <c r="A11" s="218"/>
+      <c r="B11" s="221"/>
+      <c r="C11" s="218"/>
+      <c r="D11" s="153" t="s">
         <v>103</v>
       </c>
-      <c r="E11" s="219"/>
-      <c r="F11" s="218"/>
-      <c r="G11" s="218"/>
-      <c r="H11" s="218"/>
-      <c r="I11" s="220"/>
-      <c r="J11" s="220"/>
-      <c r="K11" s="156"/>
-      <c r="L11" s="220"/>
+      <c r="E11" s="220"/>
+      <c r="F11" s="217"/>
+      <c r="G11" s="217"/>
+      <c r="H11" s="217"/>
+      <c r="I11" s="215"/>
+      <c r="J11" s="215"/>
+      <c r="K11" s="154"/>
+      <c r="L11" s="215"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="216"/>
-      <c r="B12" s="222"/>
-      <c r="C12" s="216"/>
-      <c r="D12" s="155" t="s">
+      <c r="A12" s="218"/>
+      <c r="B12" s="221"/>
+      <c r="C12" s="218"/>
+      <c r="D12" s="153" t="s">
         <v>104</v>
       </c>
-      <c r="E12" s="219"/>
-      <c r="F12" s="218"/>
-      <c r="G12" s="218"/>
-      <c r="H12" s="218"/>
-      <c r="I12" s="220"/>
-      <c r="J12" s="220"/>
+      <c r="E12" s="220"/>
+      <c r="F12" s="217"/>
+      <c r="G12" s="217"/>
+      <c r="H12" s="217"/>
+      <c r="I12" s="215"/>
+      <c r="J12" s="215"/>
       <c r="K12" s="138"/>
-      <c r="L12" s="220"/>
+      <c r="L12" s="215"/>
     </row>
     <row r="13" spans="1:12" ht="43.2">
       <c r="A13" s="126" t="s">
@@ -12016,7 +12022,7 @@
       <c r="D14" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="143" t="s">
+      <c r="E14" s="142" t="s">
         <v>315</v>
       </c>
       <c r="F14" s="125" t="s">
@@ -12047,7 +12053,7 @@
       <c r="C15" s="126" t="s">
         <v>139</v>
       </c>
-      <c r="D15" s="157" t="s">
+      <c r="D15" s="155" t="s">
         <v>140</v>
       </c>
       <c r="E15" s="74" t="s">
@@ -12068,7 +12074,7 @@
       <c r="J15" s="107" t="s">
         <v>76</v>
       </c>
-      <c r="K15" s="158" t="s">
+      <c r="K15" s="156" t="s">
         <v>143</v>
       </c>
       <c r="L15" s="130"/>
@@ -12080,10 +12086,10 @@
       <c r="B16" s="35" t="s">
         <v>318</v>
       </c>
-      <c r="C16" s="143" t="s">
+      <c r="C16" s="142" t="s">
         <v>319</v>
       </c>
-      <c r="D16" s="145" t="s">
+      <c r="D16" s="144" t="s">
         <v>320</v>
       </c>
       <c r="E16" s="35" t="s">
@@ -12104,7 +12110,7 @@
       <c r="J16" s="107" t="s">
         <v>76</v>
       </c>
-      <c r="K16" s="158" t="s">
+      <c r="K16" s="156" t="s">
         <v>323</v>
       </c>
       <c r="L16" s="107"/>
@@ -12138,7 +12144,7 @@
       <c r="J17" s="107" t="s">
         <v>76</v>
       </c>
-      <c r="K17" s="158" t="s">
+      <c r="K17" s="156" t="s">
         <v>167</v>
       </c>
       <c r="L17" s="130"/>
@@ -12150,7 +12156,7 @@
       <c r="B18" s="35" t="s">
         <v>198</v>
       </c>
-      <c r="C18" s="143" t="s">
+      <c r="C18" s="142" t="s">
         <v>199</v>
       </c>
       <c r="D18" s="133" t="s">
@@ -12174,7 +12180,7 @@
       <c r="J18" s="107" t="s">
         <v>76</v>
       </c>
-      <c r="K18" s="158" t="s">
+      <c r="K18" s="156" t="s">
         <v>201</v>
       </c>
       <c r="L18" s="107"/>
@@ -12208,7 +12214,7 @@
       <c r="J19" s="130" t="s">
         <v>76</v>
       </c>
-      <c r="K19" s="211" t="s">
+      <c r="K19" s="209" t="s">
         <v>229</v>
       </c>
       <c r="L19" s="130"/>
@@ -12226,7 +12232,7 @@
       <c r="D20" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="214" t="s">
+      <c r="E20" s="212" t="s">
         <v>328</v>
       </c>
       <c r="F20" s="125" t="s">
@@ -12346,7 +12352,7 @@
       <c r="J23" s="130" t="s">
         <v>76</v>
       </c>
-      <c r="K23" s="211"/>
+      <c r="K23" s="209"/>
       <c r="L23" s="130"/>
     </row>
     <row r="24" spans="1:12" ht="28.8">
@@ -12362,7 +12368,7 @@
       <c r="D24" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="215" t="s">
+      <c r="E24" s="213" t="s">
         <v>338</v>
       </c>
       <c r="F24" s="125" t="s">
@@ -12890,28 +12896,28 @@
   <dimension ref="A1:L57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18" style="181" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38" style="181" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" style="181" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.44140625" style="178" customWidth="1"/>
-    <col min="5" max="5" width="65.88671875" style="181" customWidth="1"/>
+    <col min="1" max="1" width="18" style="179" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38" style="179" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" style="179" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.44140625" style="176" customWidth="1"/>
+    <col min="5" max="5" width="65.88671875" style="179" customWidth="1"/>
     <col min="6" max="6" width="18.6640625" style="137" customWidth="1"/>
     <col min="7" max="7" width="17.44140625" style="137" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" style="185" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" style="183" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.5546875" style="137" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19" style="137" customWidth="1"/>
-    <col min="11" max="11" width="39.33203125" style="159" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="39.33203125" style="157" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="26.6640625" style="137" customWidth="1"/>
     <col min="13" max="16384" width="8.88671875" style="137"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="204" customFormat="1" ht="43.2">
+    <row r="1" spans="1:12" s="202" customFormat="1" ht="43.2">
       <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
@@ -12942,7 +12948,7 @@
       <c r="J1" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="203" t="s">
+      <c r="K1" s="201" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="108" t="s">
@@ -12953,32 +12959,32 @@
       <c r="A2" s="64" t="s">
         <v>339</v>
       </c>
-      <c r="B2" s="160" t="s">
+      <c r="B2" s="158" t="s">
         <v>96</v>
       </c>
       <c r="C2" s="64" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="155" t="s">
+      <c r="D2" s="153" t="s">
         <v>340</v>
       </c>
-      <c r="E2" s="161" t="s">
+      <c r="E2" s="159" t="s">
         <v>341</v>
       </c>
-      <c r="F2" s="162" t="s">
+      <c r="F2" s="160" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="162" t="s">
+      <c r="G2" s="160" t="s">
         <v>100</v>
       </c>
-      <c r="H2" s="162" t="s">
+      <c r="H2" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="163" t="s">
+      <c r="I2" s="161" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="163"/>
-      <c r="K2" s="164"/>
+      <c r="J2" s="161"/>
+      <c r="K2" s="162"/>
       <c r="L2" s="107"/>
     </row>
     <row r="3" spans="1:12" ht="100.8">
@@ -12991,25 +12997,25 @@
       <c r="C3" s="68" t="s">
         <v>344</v>
       </c>
-      <c r="D3" s="165" t="s">
+      <c r="D3" s="163" t="s">
         <v>25</v>
       </c>
       <c r="E3" s="61" t="s">
         <v>345</v>
       </c>
-      <c r="F3" s="166" t="s">
+      <c r="F3" s="164" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="166" t="s">
+      <c r="G3" s="164" t="s">
         <v>346</v>
       </c>
-      <c r="H3" s="166">
+      <c r="H3" s="164">
         <v>1</v>
       </c>
-      <c r="I3" s="167" t="s">
+      <c r="I3" s="165" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="163" t="s">
+      <c r="J3" s="161" t="s">
         <v>30</v>
       </c>
       <c r="K3" s="137" t="s">
@@ -13021,7 +13027,7 @@
       <c r="A4" s="64" t="s">
         <v>116</v>
       </c>
-      <c r="B4" s="160" t="s">
+      <c r="B4" s="158" t="s">
         <v>117</v>
       </c>
       <c r="C4" s="64" t="s">
@@ -13030,22 +13036,22 @@
       <c r="D4" s="71" t="s">
         <v>348</v>
       </c>
-      <c r="E4" s="161" t="s">
+      <c r="E4" s="159" t="s">
         <v>349</v>
       </c>
-      <c r="F4" s="162" t="s">
+      <c r="F4" s="160" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="162" t="s">
+      <c r="G4" s="160" t="s">
         <v>75</v>
       </c>
-      <c r="H4" s="162" t="s">
+      <c r="H4" s="160" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="163" t="s">
+      <c r="I4" s="161" t="s">
         <v>69</v>
       </c>
-      <c r="J4" s="163" t="s">
+      <c r="J4" s="161" t="s">
         <v>350</v>
       </c>
       <c r="K4" s="137" t="s">
@@ -13054,13 +13060,13 @@
       <c r="L4" s="107"/>
     </row>
     <row r="5" spans="1:12" ht="43.2">
-      <c r="A5" s="168" t="s">
+      <c r="A5" s="166" t="s">
         <v>352</v>
       </c>
       <c r="B5" s="75" t="s">
         <v>353</v>
       </c>
-      <c r="C5" s="168" t="s">
+      <c r="C5" s="166" t="s">
         <v>354</v>
       </c>
       <c r="D5" s="127" t="s">
@@ -13069,19 +13075,19 @@
       <c r="E5" s="75" t="s">
         <v>355</v>
       </c>
-      <c r="F5" s="169" t="s">
+      <c r="F5" s="167" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="169" t="s">
+      <c r="G5" s="167" t="s">
         <v>75</v>
       </c>
-      <c r="H5" s="169" t="s">
+      <c r="H5" s="167" t="s">
         <v>37</v>
       </c>
-      <c r="I5" s="170" t="s">
+      <c r="I5" s="168" t="s">
         <v>69</v>
       </c>
-      <c r="J5" s="163" t="s">
+      <c r="J5" s="161" t="s">
         <v>76</v>
       </c>
       <c r="K5" s="137" t="s">
@@ -13090,19 +13096,19 @@
       <c r="L5" s="130"/>
     </row>
     <row r="6" spans="1:12" ht="72">
-      <c r="A6" s="171" t="s">
+      <c r="A6" s="169" t="s">
         <v>357</v>
       </c>
-      <c r="B6" s="153" t="s">
+      <c r="B6" s="152" t="s">
         <v>358</v>
       </c>
-      <c r="C6" s="171" t="s">
+      <c r="C6" s="169" t="s">
         <v>359</v>
       </c>
-      <c r="D6" s="172" t="s">
+      <c r="D6" s="170" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="153" t="s">
+      <c r="E6" s="152" t="s">
         <v>360</v>
       </c>
       <c r="F6" s="134" t="s">
@@ -13114,13 +13120,13 @@
       <c r="H6" s="134" t="s">
         <v>93</v>
       </c>
-      <c r="I6" s="146" t="s">
+      <c r="I6" s="145" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="173" t="s">
+      <c r="J6" s="171" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="164"/>
+      <c r="K6" s="162"/>
       <c r="L6" s="107"/>
     </row>
     <row r="7" spans="1:12" ht="115.2">
@@ -13133,7 +13139,7 @@
       <c r="C7" s="126" t="s">
         <v>363</v>
       </c>
-      <c r="D7" s="174" t="s">
+      <c r="D7" s="172" t="s">
         <v>364</v>
       </c>
       <c r="E7" s="81" t="s">
@@ -13151,41 +13157,41 @@
       <c r="I7" s="130" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="173" t="s">
+      <c r="J7" s="171" t="s">
         <v>30</v>
       </c>
-      <c r="K7" s="164"/>
+      <c r="K7" s="162"/>
       <c r="L7" s="130"/>
     </row>
     <row r="8" spans="1:12" ht="28.8">
       <c r="A8" s="64" t="s">
         <v>273</v>
       </c>
-      <c r="B8" s="160" t="s">
+      <c r="B8" s="158" t="s">
         <v>274</v>
       </c>
-      <c r="C8" s="175" t="s">
+      <c r="C8" s="173" t="s">
         <v>275</v>
       </c>
-      <c r="D8" s="145" t="s">
+      <c r="D8" s="144" t="s">
         <v>364</v>
       </c>
       <c r="E8" s="136" t="s">
         <v>366</v>
       </c>
-      <c r="F8" s="162" t="s">
+      <c r="F8" s="160" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="162" t="s">
+      <c r="G8" s="160" t="s">
         <v>43</v>
       </c>
-      <c r="H8" s="162" t="s">
+      <c r="H8" s="160" t="s">
         <v>93</v>
       </c>
-      <c r="I8" s="163" t="s">
+      <c r="I8" s="161" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="163" t="s">
+      <c r="J8" s="161" t="s">
         <v>76</v>
       </c>
       <c r="K8" s="137" t="s">
@@ -13194,34 +13200,34 @@
       <c r="L8" s="107"/>
     </row>
     <row r="9" spans="1:12" ht="43.2">
-      <c r="A9" s="168" t="s">
+      <c r="A9" s="166" t="s">
         <v>368</v>
       </c>
       <c r="B9" s="75" t="s">
         <v>313</v>
       </c>
-      <c r="C9" s="168" t="s">
+      <c r="C9" s="166" t="s">
         <v>314</v>
       </c>
-      <c r="D9" s="176" t="s">
+      <c r="D9" s="174" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="176" t="s">
+      <c r="E9" s="174" t="s">
         <v>369</v>
       </c>
-      <c r="F9" s="169" t="s">
+      <c r="F9" s="167" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="169" t="s">
+      <c r="G9" s="167" t="s">
         <v>130</v>
       </c>
-      <c r="H9" s="169">
+      <c r="H9" s="167">
         <v>1</v>
       </c>
-      <c r="I9" s="170" t="s">
+      <c r="I9" s="168" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="163" t="s">
+      <c r="J9" s="161" t="s">
         <v>30</v>
       </c>
       <c r="K9" s="137" t="s">
@@ -13230,594 +13236,594 @@
       <c r="L9" s="130"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="177"/>
-      <c r="B10" s="178"/>
-      <c r="C10" s="177"/>
-      <c r="D10" s="179"/>
+      <c r="A10" s="175"/>
+      <c r="B10" s="176"/>
+      <c r="C10" s="175"/>
+      <c r="D10" s="177"/>
       <c r="E10" s="10"/>
-      <c r="F10" s="180"/>
-      <c r="G10" s="180"/>
-      <c r="H10" s="180"/>
-      <c r="I10" s="159"/>
-      <c r="J10" s="159"/>
+      <c r="F10" s="178"/>
+      <c r="G10" s="178"/>
+      <c r="H10" s="178"/>
+      <c r="I10" s="157"/>
+      <c r="J10" s="157"/>
       <c r="K10" s="98"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="177"/>
-      <c r="B11" s="178"/>
-      <c r="D11" s="179"/>
-      <c r="E11" s="179"/>
-      <c r="F11" s="180"/>
-      <c r="G11" s="180"/>
-      <c r="H11" s="180"/>
-      <c r="I11" s="159"/>
-      <c r="J11" s="159"/>
+      <c r="A11" s="175"/>
+      <c r="B11" s="176"/>
+      <c r="D11" s="177"/>
+      <c r="E11" s="177"/>
+      <c r="F11" s="178"/>
+      <c r="G11" s="178"/>
+      <c r="H11" s="178"/>
+      <c r="I11" s="157"/>
+      <c r="J11" s="157"/>
       <c r="K11" s="99"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="177"/>
-      <c r="B12" s="178"/>
-      <c r="C12" s="177"/>
-      <c r="D12" s="179"/>
-      <c r="E12" s="179"/>
-      <c r="F12" s="180"/>
-      <c r="G12" s="180"/>
-      <c r="H12" s="180"/>
-      <c r="I12" s="159"/>
-      <c r="J12" s="159"/>
+      <c r="A12" s="175"/>
+      <c r="B12" s="176"/>
+      <c r="C12" s="175"/>
+      <c r="D12" s="177"/>
+      <c r="E12" s="177"/>
+      <c r="F12" s="178"/>
+      <c r="G12" s="178"/>
+      <c r="H12" s="178"/>
+      <c r="I12" s="157"/>
+      <c r="J12" s="157"/>
       <c r="K12" s="98"/>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="177"/>
-      <c r="B13" s="178"/>
-      <c r="C13" s="177"/>
-      <c r="D13" s="179"/>
-      <c r="E13" s="178"/>
-      <c r="F13" s="180"/>
-      <c r="G13" s="180"/>
-      <c r="H13" s="180"/>
-      <c r="I13" s="159"/>
-      <c r="J13" s="159"/>
+      <c r="A13" s="175"/>
+      <c r="B13" s="176"/>
+      <c r="C13" s="175"/>
+      <c r="D13" s="177"/>
+      <c r="E13" s="176"/>
+      <c r="F13" s="178"/>
+      <c r="G13" s="178"/>
+      <c r="H13" s="178"/>
+      <c r="I13" s="157"/>
+      <c r="J13" s="157"/>
       <c r="K13" s="98"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="177"/>
-      <c r="B14" s="178"/>
-      <c r="C14" s="177"/>
-      <c r="D14" s="179"/>
-      <c r="E14" s="179"/>
-      <c r="F14" s="180"/>
-      <c r="G14" s="180"/>
-      <c r="H14" s="180"/>
-      <c r="I14" s="159"/>
-      <c r="J14" s="159"/>
+      <c r="A14" s="175"/>
+      <c r="B14" s="176"/>
+      <c r="C14" s="175"/>
+      <c r="D14" s="177"/>
+      <c r="E14" s="177"/>
+      <c r="F14" s="178"/>
+      <c r="G14" s="178"/>
+      <c r="H14" s="178"/>
+      <c r="I14" s="157"/>
+      <c r="J14" s="157"/>
       <c r="K14" s="98"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="177"/>
-      <c r="B15" s="178"/>
-      <c r="C15" s="182"/>
-      <c r="D15" s="179"/>
-      <c r="E15" s="183"/>
-      <c r="F15" s="180"/>
-      <c r="G15" s="180"/>
-      <c r="H15" s="180"/>
-      <c r="I15" s="159"/>
-      <c r="J15" s="159"/>
+      <c r="A15" s="175"/>
+      <c r="B15" s="176"/>
+      <c r="C15" s="180"/>
+      <c r="D15" s="177"/>
+      <c r="E15" s="181"/>
+      <c r="F15" s="178"/>
+      <c r="G15" s="178"/>
+      <c r="H15" s="178"/>
+      <c r="I15" s="157"/>
+      <c r="J15" s="157"/>
       <c r="K15" s="98"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="177"/>
-      <c r="B16" s="178"/>
-      <c r="C16" s="177"/>
-      <c r="D16" s="179"/>
+      <c r="A16" s="175"/>
+      <c r="B16" s="176"/>
+      <c r="C16" s="175"/>
+      <c r="D16" s="177"/>
       <c r="E16" s="10"/>
-      <c r="F16" s="180"/>
-      <c r="G16" s="180"/>
-      <c r="H16" s="180"/>
-      <c r="I16" s="159"/>
-      <c r="J16" s="159"/>
+      <c r="F16" s="178"/>
+      <c r="G16" s="178"/>
+      <c r="H16" s="178"/>
+      <c r="I16" s="157"/>
+      <c r="J16" s="157"/>
       <c r="K16" s="98"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="177"/>
-      <c r="B17" s="178"/>
-      <c r="D17" s="179"/>
-      <c r="E17" s="179"/>
-      <c r="F17" s="180"/>
-      <c r="G17" s="180"/>
-      <c r="H17" s="180"/>
-      <c r="I17" s="159"/>
-      <c r="J17" s="159"/>
+      <c r="A17" s="175"/>
+      <c r="B17" s="176"/>
+      <c r="D17" s="177"/>
+      <c r="E17" s="177"/>
+      <c r="F17" s="178"/>
+      <c r="G17" s="178"/>
+      <c r="H17" s="178"/>
+      <c r="I17" s="157"/>
+      <c r="J17" s="157"/>
       <c r="K17" s="98"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="177"/>
-      <c r="B18" s="178"/>
-      <c r="C18" s="177"/>
+      <c r="A18" s="175"/>
+      <c r="B18" s="176"/>
+      <c r="C18" s="175"/>
       <c r="D18" s="123"/>
-      <c r="E18" s="179"/>
-      <c r="F18" s="180"/>
-      <c r="G18" s="180"/>
-      <c r="H18" s="180"/>
-      <c r="I18" s="159"/>
-      <c r="J18" s="159"/>
+      <c r="E18" s="177"/>
+      <c r="F18" s="178"/>
+      <c r="G18" s="178"/>
+      <c r="H18" s="178"/>
+      <c r="I18" s="157"/>
+      <c r="J18" s="157"/>
       <c r="K18" s="98"/>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="177"/>
-      <c r="B19" s="178"/>
-      <c r="C19" s="177"/>
-      <c r="D19" s="179"/>
-      <c r="E19" s="178"/>
-      <c r="F19" s="180"/>
-      <c r="G19" s="180"/>
-      <c r="H19" s="180"/>
-      <c r="I19" s="159"/>
-      <c r="J19" s="159"/>
+      <c r="A19" s="175"/>
+      <c r="B19" s="176"/>
+      <c r="C19" s="175"/>
+      <c r="D19" s="177"/>
+      <c r="E19" s="176"/>
+      <c r="F19" s="178"/>
+      <c r="G19" s="178"/>
+      <c r="H19" s="178"/>
+      <c r="I19" s="157"/>
+      <c r="J19" s="157"/>
       <c r="K19" s="101"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="177"/>
-      <c r="B20" s="178"/>
-      <c r="C20" s="177"/>
-      <c r="D20" s="179"/>
-      <c r="E20" s="179"/>
-      <c r="F20" s="180"/>
-      <c r="G20" s="180"/>
-      <c r="H20" s="180"/>
-      <c r="I20" s="159"/>
-      <c r="J20" s="159"/>
+      <c r="A20" s="175"/>
+      <c r="B20" s="176"/>
+      <c r="C20" s="175"/>
+      <c r="D20" s="177"/>
+      <c r="E20" s="177"/>
+      <c r="F20" s="178"/>
+      <c r="G20" s="178"/>
+      <c r="H20" s="178"/>
+      <c r="I20" s="157"/>
+      <c r="J20" s="157"/>
       <c r="K20" s="99"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="177"/>
-      <c r="B21" s="178"/>
-      <c r="C21" s="182"/>
-      <c r="D21" s="179"/>
-      <c r="E21" s="183"/>
-      <c r="F21" s="180"/>
-      <c r="G21" s="180"/>
-      <c r="H21" s="180"/>
-      <c r="I21" s="159"/>
-      <c r="J21" s="159"/>
+      <c r="A21" s="175"/>
+      <c r="B21" s="176"/>
+      <c r="C21" s="180"/>
+      <c r="D21" s="177"/>
+      <c r="E21" s="181"/>
+      <c r="F21" s="178"/>
+      <c r="G21" s="178"/>
+      <c r="H21" s="178"/>
+      <c r="I21" s="157"/>
+      <c r="J21" s="157"/>
       <c r="K21" s="98"/>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="177"/>
-      <c r="B22" s="178"/>
-      <c r="C22" s="177"/>
-      <c r="D22" s="179"/>
+      <c r="A22" s="175"/>
+      <c r="B22" s="176"/>
+      <c r="C22" s="175"/>
+      <c r="D22" s="177"/>
       <c r="E22" s="10"/>
-      <c r="F22" s="180"/>
-      <c r="G22" s="180"/>
-      <c r="H22" s="180"/>
-      <c r="I22" s="159"/>
-      <c r="J22" s="159"/>
+      <c r="F22" s="178"/>
+      <c r="G22" s="178"/>
+      <c r="H22" s="178"/>
+      <c r="I22" s="157"/>
+      <c r="J22" s="157"/>
       <c r="K22" s="98"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="177"/>
-      <c r="B23" s="178"/>
+      <c r="A23" s="175"/>
+      <c r="B23" s="176"/>
       <c r="D23" s="123"/>
-      <c r="E23" s="179"/>
-      <c r="F23" s="180"/>
-      <c r="G23" s="180"/>
-      <c r="H23" s="180"/>
-      <c r="I23" s="159"/>
-      <c r="J23" s="159"/>
+      <c r="E23" s="177"/>
+      <c r="F23" s="178"/>
+      <c r="G23" s="178"/>
+      <c r="H23" s="178"/>
+      <c r="I23" s="157"/>
+      <c r="J23" s="157"/>
       <c r="K23" s="98"/>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="177"/>
-      <c r="B24" s="178"/>
-      <c r="C24" s="177"/>
-      <c r="D24" s="179"/>
-      <c r="E24" s="179"/>
-      <c r="F24" s="180"/>
-      <c r="G24" s="180"/>
-      <c r="H24" s="180"/>
-      <c r="I24" s="159"/>
-      <c r="J24" s="159"/>
+      <c r="A24" s="175"/>
+      <c r="B24" s="176"/>
+      <c r="C24" s="175"/>
+      <c r="D24" s="177"/>
+      <c r="E24" s="177"/>
+      <c r="F24" s="178"/>
+      <c r="G24" s="178"/>
+      <c r="H24" s="178"/>
+      <c r="I24" s="157"/>
+      <c r="J24" s="157"/>
       <c r="K24" s="100"/>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="177"/>
-      <c r="B25" s="178"/>
-      <c r="C25" s="177"/>
-      <c r="D25" s="179"/>
-      <c r="E25" s="178"/>
-      <c r="F25" s="180"/>
-      <c r="G25" s="180"/>
-      <c r="H25" s="180"/>
-      <c r="I25" s="159"/>
-      <c r="J25" s="159"/>
+      <c r="A25" s="175"/>
+      <c r="B25" s="176"/>
+      <c r="C25" s="175"/>
+      <c r="D25" s="177"/>
+      <c r="E25" s="176"/>
+      <c r="F25" s="178"/>
+      <c r="G25" s="178"/>
+      <c r="H25" s="178"/>
+      <c r="I25" s="157"/>
+      <c r="J25" s="157"/>
       <c r="K25" s="98"/>
     </row>
     <row r="26" spans="1:11">
-      <c r="A26" s="177"/>
-      <c r="B26" s="178"/>
-      <c r="C26" s="177"/>
-      <c r="D26" s="179"/>
-      <c r="E26" s="179"/>
-      <c r="F26" s="180"/>
-      <c r="G26" s="180"/>
-      <c r="H26" s="180"/>
-      <c r="I26" s="159"/>
-      <c r="J26" s="159"/>
+      <c r="A26" s="175"/>
+      <c r="B26" s="176"/>
+      <c r="C26" s="175"/>
+      <c r="D26" s="177"/>
+      <c r="E26" s="177"/>
+      <c r="F26" s="178"/>
+      <c r="G26" s="178"/>
+      <c r="H26" s="178"/>
+      <c r="I26" s="157"/>
+      <c r="J26" s="157"/>
       <c r="K26" s="100"/>
     </row>
     <row r="27" spans="1:11">
-      <c r="A27" s="177"/>
-      <c r="B27" s="178"/>
-      <c r="C27" s="182"/>
-      <c r="D27" s="179"/>
-      <c r="E27" s="183"/>
-      <c r="F27" s="180"/>
-      <c r="G27" s="180"/>
-      <c r="H27" s="180"/>
-      <c r="I27" s="159"/>
-      <c r="J27" s="159"/>
+      <c r="A27" s="175"/>
+      <c r="B27" s="176"/>
+      <c r="C27" s="180"/>
+      <c r="D27" s="177"/>
+      <c r="E27" s="181"/>
+      <c r="F27" s="178"/>
+      <c r="G27" s="178"/>
+      <c r="H27" s="178"/>
+      <c r="I27" s="157"/>
+      <c r="J27" s="157"/>
       <c r="K27" s="98"/>
     </row>
     <row r="28" spans="1:11">
-      <c r="A28" s="177"/>
-      <c r="B28" s="178"/>
-      <c r="C28" s="177"/>
-      <c r="D28" s="179"/>
+      <c r="A28" s="175"/>
+      <c r="B28" s="176"/>
+      <c r="C28" s="175"/>
+      <c r="D28" s="177"/>
       <c r="E28" s="10"/>
-      <c r="F28" s="180"/>
-      <c r="G28" s="180"/>
-      <c r="H28" s="180"/>
-      <c r="I28" s="159"/>
-      <c r="J28" s="159"/>
+      <c r="F28" s="178"/>
+      <c r="G28" s="178"/>
+      <c r="H28" s="178"/>
+      <c r="I28" s="157"/>
+      <c r="J28" s="157"/>
       <c r="K28" s="98"/>
     </row>
     <row r="29" spans="1:11">
-      <c r="A29" s="177"/>
-      <c r="B29" s="178"/>
-      <c r="D29" s="179"/>
-      <c r="E29" s="179"/>
-      <c r="F29" s="180"/>
-      <c r="G29" s="180"/>
-      <c r="H29" s="180"/>
-      <c r="I29" s="159"/>
-      <c r="J29" s="159"/>
+      <c r="A29" s="175"/>
+      <c r="B29" s="176"/>
+      <c r="D29" s="177"/>
+      <c r="E29" s="177"/>
+      <c r="F29" s="178"/>
+      <c r="G29" s="178"/>
+      <c r="H29" s="178"/>
+      <c r="I29" s="157"/>
+      <c r="J29" s="157"/>
       <c r="K29" s="98"/>
     </row>
     <row r="30" spans="1:11">
-      <c r="A30" s="177"/>
-      <c r="B30" s="178"/>
-      <c r="C30" s="177"/>
-      <c r="D30" s="179"/>
-      <c r="E30" s="179"/>
-      <c r="F30" s="180"/>
-      <c r="G30" s="180"/>
-      <c r="H30" s="180"/>
-      <c r="I30" s="159"/>
-      <c r="J30" s="159"/>
+      <c r="A30" s="175"/>
+      <c r="B30" s="176"/>
+      <c r="C30" s="175"/>
+      <c r="D30" s="177"/>
+      <c r="E30" s="177"/>
+      <c r="F30" s="178"/>
+      <c r="G30" s="178"/>
+      <c r="H30" s="178"/>
+      <c r="I30" s="157"/>
+      <c r="J30" s="157"/>
       <c r="K30" s="98"/>
     </row>
     <row r="31" spans="1:11">
-      <c r="A31" s="177"/>
-      <c r="B31" s="178"/>
-      <c r="C31" s="177"/>
-      <c r="D31" s="179"/>
-      <c r="E31" s="178"/>
-      <c r="F31" s="180"/>
-      <c r="G31" s="180"/>
-      <c r="H31" s="180"/>
-      <c r="I31" s="159"/>
-      <c r="J31" s="159"/>
+      <c r="A31" s="175"/>
+      <c r="B31" s="176"/>
+      <c r="C31" s="175"/>
+      <c r="D31" s="177"/>
+      <c r="E31" s="176"/>
+      <c r="F31" s="178"/>
+      <c r="G31" s="178"/>
+      <c r="H31" s="178"/>
+      <c r="I31" s="157"/>
+      <c r="J31" s="157"/>
       <c r="K31" s="98"/>
     </row>
     <row r="32" spans="1:11">
-      <c r="A32" s="177"/>
-      <c r="B32" s="178"/>
-      <c r="C32" s="177"/>
+      <c r="A32" s="175"/>
+      <c r="B32" s="176"/>
+      <c r="C32" s="175"/>
       <c r="D32" s="123"/>
-      <c r="E32" s="179"/>
-      <c r="F32" s="180"/>
-      <c r="G32" s="180"/>
-      <c r="H32" s="180"/>
-      <c r="I32" s="159"/>
-      <c r="J32" s="159"/>
+      <c r="E32" s="177"/>
+      <c r="F32" s="178"/>
+      <c r="G32" s="178"/>
+      <c r="H32" s="178"/>
+      <c r="I32" s="157"/>
+      <c r="J32" s="157"/>
       <c r="K32" s="98"/>
     </row>
     <row r="33" spans="1:11">
-      <c r="A33" s="177"/>
-      <c r="B33" s="178"/>
-      <c r="C33" s="182"/>
-      <c r="D33" s="179"/>
-      <c r="E33" s="183"/>
-      <c r="F33" s="180"/>
-      <c r="G33" s="180"/>
-      <c r="H33" s="180"/>
-      <c r="I33" s="159"/>
-      <c r="J33" s="159"/>
+      <c r="A33" s="175"/>
+      <c r="B33" s="176"/>
+      <c r="C33" s="180"/>
+      <c r="D33" s="177"/>
+      <c r="E33" s="181"/>
+      <c r="F33" s="178"/>
+      <c r="G33" s="178"/>
+      <c r="H33" s="178"/>
+      <c r="I33" s="157"/>
+      <c r="J33" s="157"/>
       <c r="K33" s="98"/>
     </row>
     <row r="34" spans="1:11">
-      <c r="A34" s="177"/>
-      <c r="B34" s="178"/>
-      <c r="C34" s="177"/>
-      <c r="D34" s="179"/>
+      <c r="A34" s="175"/>
+      <c r="B34" s="176"/>
+      <c r="C34" s="175"/>
+      <c r="D34" s="177"/>
       <c r="E34" s="10"/>
-      <c r="F34" s="180"/>
-      <c r="G34" s="180"/>
-      <c r="H34" s="180"/>
-      <c r="I34" s="159"/>
-      <c r="J34" s="159"/>
+      <c r="F34" s="178"/>
+      <c r="G34" s="178"/>
+      <c r="H34" s="178"/>
+      <c r="I34" s="157"/>
+      <c r="J34" s="157"/>
       <c r="K34" s="98"/>
     </row>
     <row r="35" spans="1:11">
-      <c r="A35" s="177"/>
-      <c r="B35" s="178"/>
-      <c r="D35" s="179"/>
-      <c r="E35" s="179"/>
-      <c r="F35" s="180"/>
-      <c r="G35" s="180"/>
-      <c r="H35" s="180"/>
-      <c r="I35" s="159"/>
-      <c r="J35" s="159"/>
+      <c r="A35" s="175"/>
+      <c r="B35" s="176"/>
+      <c r="D35" s="177"/>
+      <c r="E35" s="177"/>
+      <c r="F35" s="178"/>
+      <c r="G35" s="178"/>
+      <c r="H35" s="178"/>
+      <c r="I35" s="157"/>
+      <c r="J35" s="157"/>
       <c r="K35" s="98"/>
     </row>
     <row r="36" spans="1:11">
-      <c r="A36" s="177"/>
-      <c r="B36" s="178"/>
-      <c r="C36" s="177"/>
-      <c r="D36" s="179"/>
-      <c r="E36" s="179"/>
-      <c r="F36" s="180"/>
-      <c r="G36" s="180"/>
-      <c r="H36" s="180"/>
-      <c r="I36" s="159"/>
-      <c r="J36" s="159"/>
+      <c r="A36" s="175"/>
+      <c r="B36" s="176"/>
+      <c r="C36" s="175"/>
+      <c r="D36" s="177"/>
+      <c r="E36" s="177"/>
+      <c r="F36" s="178"/>
+      <c r="G36" s="178"/>
+      <c r="H36" s="178"/>
+      <c r="I36" s="157"/>
+      <c r="J36" s="157"/>
       <c r="K36" s="98"/>
     </row>
     <row r="37" spans="1:11">
-      <c r="A37" s="177"/>
-      <c r="B37" s="178"/>
-      <c r="C37" s="177"/>
-      <c r="D37" s="179"/>
-      <c r="E37" s="178"/>
-      <c r="F37" s="180"/>
-      <c r="G37" s="180"/>
-      <c r="H37" s="180"/>
-      <c r="I37" s="159"/>
-      <c r="J37" s="159"/>
+      <c r="A37" s="175"/>
+      <c r="B37" s="176"/>
+      <c r="C37" s="175"/>
+      <c r="D37" s="177"/>
+      <c r="E37" s="176"/>
+      <c r="F37" s="178"/>
+      <c r="G37" s="178"/>
+      <c r="H37" s="178"/>
+      <c r="I37" s="157"/>
+      <c r="J37" s="157"/>
       <c r="K37" s="98"/>
     </row>
     <row r="38" spans="1:11">
-      <c r="A38" s="177"/>
-      <c r="B38" s="178"/>
-      <c r="C38" s="177"/>
-      <c r="D38" s="179"/>
-      <c r="E38" s="179"/>
-      <c r="F38" s="180"/>
-      <c r="G38" s="180"/>
-      <c r="H38" s="180"/>
-      <c r="I38" s="159"/>
-      <c r="J38" s="159"/>
+      <c r="A38" s="175"/>
+      <c r="B38" s="176"/>
+      <c r="C38" s="175"/>
+      <c r="D38" s="177"/>
+      <c r="E38" s="177"/>
+      <c r="F38" s="178"/>
+      <c r="G38" s="178"/>
+      <c r="H38" s="178"/>
+      <c r="I38" s="157"/>
+      <c r="J38" s="157"/>
       <c r="K38" s="98"/>
     </row>
     <row r="39" spans="1:11">
-      <c r="A39" s="177"/>
-      <c r="B39" s="178"/>
-      <c r="C39" s="182"/>
+      <c r="A39" s="175"/>
+      <c r="B39" s="176"/>
+      <c r="C39" s="180"/>
       <c r="D39" s="123"/>
-      <c r="E39" s="183"/>
-      <c r="F39" s="180"/>
-      <c r="G39" s="180"/>
-      <c r="H39" s="180"/>
-      <c r="I39" s="159"/>
-      <c r="J39" s="159"/>
+      <c r="E39" s="181"/>
+      <c r="F39" s="178"/>
+      <c r="G39" s="178"/>
+      <c r="H39" s="178"/>
+      <c r="I39" s="157"/>
+      <c r="J39" s="157"/>
       <c r="K39" s="98"/>
     </row>
     <row r="40" spans="1:11">
-      <c r="A40" s="177"/>
-      <c r="B40" s="178"/>
-      <c r="C40" s="177"/>
-      <c r="D40" s="179"/>
-      <c r="E40" s="179"/>
-      <c r="F40" s="180"/>
-      <c r="G40" s="180"/>
-      <c r="H40" s="180"/>
-      <c r="I40" s="159"/>
-      <c r="J40" s="159"/>
+      <c r="A40" s="175"/>
+      <c r="B40" s="176"/>
+      <c r="C40" s="175"/>
+      <c r="D40" s="177"/>
+      <c r="E40" s="177"/>
+      <c r="F40" s="178"/>
+      <c r="G40" s="178"/>
+      <c r="H40" s="178"/>
+      <c r="I40" s="157"/>
+      <c r="J40" s="157"/>
       <c r="K40" s="98"/>
     </row>
     <row r="41" spans="1:11">
-      <c r="A41" s="177"/>
-      <c r="B41" s="178"/>
-      <c r="C41" s="177"/>
-      <c r="D41" s="179"/>
-      <c r="E41" s="178"/>
-      <c r="F41" s="180"/>
-      <c r="G41" s="180"/>
-      <c r="H41" s="180"/>
-      <c r="I41" s="159"/>
-      <c r="J41" s="159"/>
+      <c r="A41" s="175"/>
+      <c r="B41" s="176"/>
+      <c r="C41" s="175"/>
+      <c r="D41" s="177"/>
+      <c r="E41" s="176"/>
+      <c r="F41" s="178"/>
+      <c r="G41" s="178"/>
+      <c r="H41" s="178"/>
+      <c r="I41" s="157"/>
+      <c r="J41" s="157"/>
       <c r="K41" s="98"/>
     </row>
     <row r="42" spans="1:11">
-      <c r="A42" s="177"/>
-      <c r="B42" s="178"/>
-      <c r="C42" s="177"/>
-      <c r="D42" s="179"/>
-      <c r="E42" s="179"/>
-      <c r="F42" s="180"/>
-      <c r="G42" s="180"/>
-      <c r="H42" s="180"/>
-      <c r="I42" s="159"/>
-      <c r="J42" s="159"/>
+      <c r="A42" s="175"/>
+      <c r="B42" s="176"/>
+      <c r="C42" s="175"/>
+      <c r="D42" s="177"/>
+      <c r="E42" s="177"/>
+      <c r="F42" s="178"/>
+      <c r="G42" s="178"/>
+      <c r="H42" s="178"/>
+      <c r="I42" s="157"/>
+      <c r="J42" s="157"/>
       <c r="K42" s="98"/>
     </row>
     <row r="43" spans="1:11">
-      <c r="A43" s="177"/>
-      <c r="B43" s="178"/>
-      <c r="C43" s="182"/>
+      <c r="A43" s="175"/>
+      <c r="B43" s="176"/>
+      <c r="C43" s="180"/>
       <c r="D43" s="123"/>
-      <c r="E43" s="183"/>
-      <c r="F43" s="180"/>
-      <c r="G43" s="180"/>
-      <c r="H43" s="180"/>
-      <c r="I43" s="159"/>
-      <c r="J43" s="159"/>
+      <c r="E43" s="181"/>
+      <c r="F43" s="178"/>
+      <c r="G43" s="178"/>
+      <c r="H43" s="178"/>
+      <c r="I43" s="157"/>
+      <c r="J43" s="157"/>
       <c r="K43" s="98"/>
     </row>
     <row r="44" spans="1:11">
-      <c r="A44" s="177"/>
-      <c r="B44" s="178"/>
-      <c r="C44" s="177"/>
-      <c r="D44" s="179"/>
+      <c r="A44" s="175"/>
+      <c r="B44" s="176"/>
+      <c r="C44" s="175"/>
+      <c r="D44" s="177"/>
       <c r="E44" s="10"/>
-      <c r="F44" s="180"/>
-      <c r="G44" s="180"/>
-      <c r="H44" s="180"/>
-      <c r="I44" s="159"/>
-      <c r="J44" s="159"/>
+      <c r="F44" s="178"/>
+      <c r="G44" s="178"/>
+      <c r="H44" s="178"/>
+      <c r="I44" s="157"/>
+      <c r="J44" s="157"/>
       <c r="K44" s="98"/>
     </row>
     <row r="45" spans="1:11">
-      <c r="A45" s="177"/>
-      <c r="B45" s="178"/>
-      <c r="D45" s="179"/>
-      <c r="E45" s="179"/>
-      <c r="F45" s="180"/>
-      <c r="G45" s="180"/>
-      <c r="H45" s="180"/>
-      <c r="I45" s="159"/>
-      <c r="J45" s="159"/>
+      <c r="A45" s="175"/>
+      <c r="B45" s="176"/>
+      <c r="D45" s="177"/>
+      <c r="E45" s="177"/>
+      <c r="F45" s="178"/>
+      <c r="G45" s="178"/>
+      <c r="H45" s="178"/>
+      <c r="I45" s="157"/>
+      <c r="J45" s="157"/>
       <c r="K45" s="98"/>
     </row>
     <row r="46" spans="1:11">
-      <c r="A46" s="177"/>
-      <c r="B46" s="178"/>
-      <c r="C46" s="177"/>
-      <c r="D46" s="179"/>
-      <c r="E46" s="179"/>
-      <c r="F46" s="180"/>
-      <c r="G46" s="180"/>
-      <c r="H46" s="180"/>
-      <c r="I46" s="159"/>
-      <c r="J46" s="159"/>
+      <c r="A46" s="175"/>
+      <c r="B46" s="176"/>
+      <c r="C46" s="175"/>
+      <c r="D46" s="177"/>
+      <c r="E46" s="177"/>
+      <c r="F46" s="178"/>
+      <c r="G46" s="178"/>
+      <c r="H46" s="178"/>
+      <c r="I46" s="157"/>
+      <c r="J46" s="157"/>
       <c r="K46" s="98"/>
     </row>
     <row r="47" spans="1:11">
-      <c r="A47" s="177"/>
-      <c r="B47" s="178"/>
-      <c r="C47" s="177"/>
-      <c r="D47" s="179"/>
-      <c r="E47" s="178"/>
-      <c r="F47" s="180"/>
-      <c r="G47" s="180"/>
-      <c r="H47" s="180"/>
-      <c r="I47" s="159"/>
-      <c r="J47" s="159"/>
+      <c r="A47" s="175"/>
+      <c r="B47" s="176"/>
+      <c r="C47" s="175"/>
+      <c r="D47" s="177"/>
+      <c r="E47" s="176"/>
+      <c r="F47" s="178"/>
+      <c r="G47" s="178"/>
+      <c r="H47" s="178"/>
+      <c r="I47" s="157"/>
+      <c r="J47" s="157"/>
       <c r="K47" s="98"/>
     </row>
     <row r="48" spans="1:11">
-      <c r="A48" s="177"/>
-      <c r="B48" s="178"/>
-      <c r="C48" s="177"/>
-      <c r="D48" s="179"/>
-      <c r="E48" s="179"/>
-      <c r="F48" s="180"/>
-      <c r="G48" s="180"/>
-      <c r="H48" s="180"/>
-      <c r="I48" s="159"/>
-      <c r="J48" s="159"/>
+      <c r="A48" s="175"/>
+      <c r="B48" s="176"/>
+      <c r="C48" s="175"/>
+      <c r="D48" s="177"/>
+      <c r="E48" s="177"/>
+      <c r="F48" s="178"/>
+      <c r="G48" s="178"/>
+      <c r="H48" s="178"/>
+      <c r="I48" s="157"/>
+      <c r="J48" s="157"/>
       <c r="K48" s="98"/>
     </row>
     <row r="49" spans="1:11">
-      <c r="A49" s="177"/>
-      <c r="B49" s="178"/>
-      <c r="C49" s="182"/>
-      <c r="D49" s="179"/>
-      <c r="E49" s="183"/>
-      <c r="F49" s="180"/>
-      <c r="G49" s="180"/>
-      <c r="H49" s="180"/>
-      <c r="I49" s="159"/>
-      <c r="J49" s="159"/>
+      <c r="A49" s="175"/>
+      <c r="B49" s="176"/>
+      <c r="C49" s="180"/>
+      <c r="D49" s="177"/>
+      <c r="E49" s="181"/>
+      <c r="F49" s="178"/>
+      <c r="G49" s="178"/>
+      <c r="H49" s="178"/>
+      <c r="I49" s="157"/>
+      <c r="J49" s="157"/>
       <c r="K49" s="98"/>
     </row>
     <row r="50" spans="1:11">
-      <c r="A50" s="177"/>
-      <c r="B50" s="178"/>
-      <c r="C50" s="177"/>
-      <c r="D50" s="179"/>
-      <c r="E50" s="178"/>
-      <c r="F50" s="180"/>
-      <c r="G50" s="180"/>
-      <c r="H50" s="180"/>
-      <c r="I50" s="159"/>
-      <c r="J50" s="159"/>
+      <c r="A50" s="175"/>
+      <c r="B50" s="176"/>
+      <c r="C50" s="175"/>
+      <c r="D50" s="177"/>
+      <c r="E50" s="176"/>
+      <c r="F50" s="178"/>
+      <c r="G50" s="178"/>
+      <c r="H50" s="178"/>
+      <c r="I50" s="157"/>
+      <c r="J50" s="157"/>
       <c r="K50" s="98"/>
     </row>
     <row r="51" spans="1:11">
-      <c r="A51" s="177"/>
-      <c r="B51" s="178"/>
-      <c r="C51" s="177"/>
-      <c r="D51" s="179"/>
-      <c r="E51" s="178"/>
-      <c r="F51" s="180"/>
-      <c r="G51" s="180"/>
-      <c r="H51" s="180"/>
-      <c r="I51" s="159"/>
-      <c r="J51" s="159"/>
+      <c r="A51" s="175"/>
+      <c r="B51" s="176"/>
+      <c r="C51" s="175"/>
+      <c r="D51" s="177"/>
+      <c r="E51" s="176"/>
+      <c r="F51" s="178"/>
+      <c r="G51" s="178"/>
+      <c r="H51" s="178"/>
+      <c r="I51" s="157"/>
+      <c r="J51" s="157"/>
       <c r="K51" s="98"/>
     </row>
     <row r="52" spans="1:11">
-      <c r="A52" s="177"/>
-      <c r="B52" s="178"/>
-      <c r="C52" s="177"/>
-      <c r="D52" s="184"/>
-      <c r="E52" s="179"/>
-      <c r="F52" s="180"/>
-      <c r="G52" s="180"/>
-      <c r="H52" s="180"/>
-      <c r="I52" s="159"/>
-      <c r="J52" s="159"/>
+      <c r="A52" s="175"/>
+      <c r="B52" s="176"/>
+      <c r="C52" s="175"/>
+      <c r="D52" s="182"/>
+      <c r="E52" s="177"/>
+      <c r="F52" s="178"/>
+      <c r="G52" s="178"/>
+      <c r="H52" s="178"/>
+      <c r="I52" s="157"/>
+      <c r="J52" s="157"/>
       <c r="K52" s="98"/>
     </row>
     <row r="53" spans="1:11">
-      <c r="A53" s="177"/>
-      <c r="B53" s="178"/>
-      <c r="D53" s="179"/>
-      <c r="E53" s="179"/>
-      <c r="F53" s="180"/>
-      <c r="G53" s="180"/>
-      <c r="H53" s="180"/>
-      <c r="I53" s="159"/>
-      <c r="J53" s="159"/>
+      <c r="A53" s="175"/>
+      <c r="B53" s="176"/>
+      <c r="D53" s="177"/>
+      <c r="E53" s="177"/>
+      <c r="F53" s="178"/>
+      <c r="G53" s="178"/>
+      <c r="H53" s="178"/>
+      <c r="I53" s="157"/>
+      <c r="J53" s="157"/>
       <c r="K53" s="98"/>
     </row>
     <row r="54" spans="1:11">
-      <c r="A54" s="177"/>
-      <c r="B54" s="178"/>
-      <c r="C54" s="177"/>
-      <c r="D54" s="179"/>
-      <c r="E54" s="179"/>
-      <c r="F54" s="180"/>
-      <c r="G54" s="180"/>
-      <c r="H54" s="180"/>
-      <c r="I54" s="159"/>
-      <c r="J54" s="159"/>
+      <c r="A54" s="175"/>
+      <c r="B54" s="176"/>
+      <c r="C54" s="175"/>
+      <c r="D54" s="177"/>
+      <c r="E54" s="177"/>
+      <c r="F54" s="178"/>
+      <c r="G54" s="178"/>
+      <c r="H54" s="178"/>
+      <c r="I54" s="157"/>
+      <c r="J54" s="157"/>
       <c r="K54" s="98"/>
     </row>
     <row r="55" spans="1:11">
-      <c r="A55" s="177"/>
-      <c r="B55" s="178"/>
-      <c r="C55" s="177"/>
-      <c r="D55" s="179"/>
-      <c r="E55" s="179"/>
-      <c r="F55" s="180"/>
-      <c r="G55" s="180"/>
-      <c r="H55" s="180"/>
-      <c r="I55" s="159"/>
-      <c r="J55" s="159"/>
+      <c r="A55" s="175"/>
+      <c r="B55" s="176"/>
+      <c r="C55" s="175"/>
+      <c r="D55" s="177"/>
+      <c r="E55" s="177"/>
+      <c r="F55" s="178"/>
+      <c r="G55" s="178"/>
+      <c r="H55" s="178"/>
+      <c r="I55" s="157"/>
+      <c r="J55" s="157"/>
       <c r="K55" s="98"/>
     </row>
     <row r="56" spans="1:11">
@@ -13927,7 +13933,7 @@
     <col min="13" max="16384" width="8.88671875" style="84"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="204" customFormat="1" ht="57.6">
+    <row r="1" spans="1:12" s="202" customFormat="1" ht="57.6">
       <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
@@ -13958,7 +13964,7 @@
       <c r="J1" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="203" t="s">
+      <c r="K1" s="201" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="108" t="s">
@@ -13972,7 +13978,7 @@
       <c r="B2" s="45" t="s">
         <v>372</v>
       </c>
-      <c r="C2" s="175" t="s">
+      <c r="C2" s="173" t="s">
         <v>373</v>
       </c>
       <c r="D2" s="64" t="s">
@@ -13981,22 +13987,22 @@
       <c r="E2" s="88" t="s">
         <v>374</v>
       </c>
-      <c r="F2" s="162" t="s">
+      <c r="F2" s="160" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="162" t="s">
+      <c r="G2" s="160" t="s">
         <v>346</v>
       </c>
-      <c r="H2" s="162" t="s">
+      <c r="H2" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="163" t="s">
+      <c r="I2" s="161" t="s">
         <v>69</v>
       </c>
-      <c r="J2" s="163" t="s">
+      <c r="J2" s="161" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="159" t="s">
+      <c r="K2" s="157" t="s">
         <v>375</v>
       </c>
       <c r="L2" s="137"/>
@@ -14011,28 +14017,28 @@
       <c r="C3" s="68" t="s">
         <v>378</v>
       </c>
-      <c r="D3" s="186" t="s">
+      <c r="D3" s="184" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="187" t="s">
+      <c r="E3" s="185" t="s">
         <v>379</v>
       </c>
-      <c r="F3" s="166" t="s">
+      <c r="F3" s="164" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="166" t="s">
+      <c r="G3" s="164" t="s">
         <v>346</v>
       </c>
-      <c r="H3" s="166">
+      <c r="H3" s="164">
         <v>1</v>
       </c>
-      <c r="I3" s="167" t="s">
+      <c r="I3" s="165" t="s">
         <v>69</v>
       </c>
-      <c r="J3" s="163" t="s">
+      <c r="J3" s="161" t="s">
         <v>76</v>
       </c>
-      <c r="K3" s="159" t="s">
+      <c r="K3" s="157" t="s">
         <v>380</v>
       </c>
       <c r="L3" s="137"/>
@@ -14053,22 +14059,22 @@
       <c r="E4" s="88" t="s">
         <v>384</v>
       </c>
-      <c r="F4" s="162" t="s">
+      <c r="F4" s="160" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="162" t="s">
+      <c r="G4" s="160" t="s">
         <v>385</v>
       </c>
-      <c r="H4" s="162">
+      <c r="H4" s="160">
         <v>1</v>
       </c>
-      <c r="I4" s="163" t="s">
+      <c r="I4" s="161" t="s">
         <v>69</v>
       </c>
-      <c r="J4" s="163" t="s">
+      <c r="J4" s="161" t="s">
         <v>76</v>
       </c>
-      <c r="K4" s="159" t="s">
+      <c r="K4" s="157" t="s">
         <v>386</v>
       </c>
       <c r="L4" s="137"/>
@@ -14786,8 +14792,8 @@
   </sheetPr>
   <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
@@ -14808,7 +14814,7 @@
     <col min="13" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="204" customFormat="1" ht="57.6">
+    <row r="1" spans="1:12" s="202" customFormat="1" ht="57.6">
       <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
@@ -14839,7 +14845,7 @@
       <c r="J1" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="203" t="s">
+      <c r="K1" s="201" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="108" t="s">
@@ -15036,7 +15042,7 @@
       <c r="C7" s="135" t="s">
         <v>412</v>
       </c>
-      <c r="D7" s="188" t="s">
+      <c r="D7" s="186" t="s">
         <v>413</v>
       </c>
       <c r="E7" s="127" t="s">
@@ -15045,7 +15051,7 @@
       <c r="F7" s="128" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="159" t="s">
+      <c r="G7" s="157" t="s">
         <v>415</v>
       </c>
       <c r="H7" s="128" t="s">
@@ -15108,7 +15114,7 @@
       <c r="C9" s="126" t="s">
         <v>84</v>
       </c>
-      <c r="D9" s="190" t="s">
+      <c r="D9" s="188" t="s">
         <v>25</v>
       </c>
       <c r="E9" s="127" t="s">
@@ -15141,7 +15147,7 @@
       <c r="B10" s="35" t="s">
         <v>422</v>
       </c>
-      <c r="C10" s="143" t="s">
+      <c r="C10" s="142" t="s">
         <v>423</v>
       </c>
       <c r="D10" s="133" t="s">
@@ -15180,7 +15186,7 @@
       <c r="C11" s="126" t="s">
         <v>428</v>
       </c>
-      <c r="D11" s="157" t="s">
+      <c r="D11" s="155" t="s">
         <v>429</v>
       </c>
       <c r="E11" s="127" t="s">
@@ -15216,7 +15222,7 @@
       <c r="C12" s="122" t="s">
         <v>139</v>
       </c>
-      <c r="D12" s="191" t="s">
+      <c r="D12" s="189" t="s">
         <v>140</v>
       </c>
       <c r="E12" s="139" t="s">
@@ -15252,7 +15258,7 @@
       <c r="C13" s="126" t="s">
         <v>319</v>
       </c>
-      <c r="D13" s="144" t="s">
+      <c r="D13" s="143" t="s">
         <v>320</v>
       </c>
       <c r="E13" s="80" t="s">
@@ -15324,7 +15330,7 @@
       <c r="C15" s="126" t="s">
         <v>444</v>
       </c>
-      <c r="D15" s="188" t="s">
+      <c r="D15" s="186" t="s">
         <v>413</v>
       </c>
       <c r="E15" s="80" t="s">
@@ -15357,10 +15363,10 @@
       <c r="B16" s="35" t="s">
         <v>163</v>
       </c>
-      <c r="C16" s="143" t="s">
+      <c r="C16" s="142" t="s">
         <v>164</v>
       </c>
-      <c r="D16" s="192" t="s">
+      <c r="D16" s="190" t="s">
         <v>25</v>
       </c>
       <c r="E16" s="133"/>
@@ -15394,7 +15400,7 @@
       <c r="C17" s="126" t="s">
         <v>450</v>
       </c>
-      <c r="D17" s="188" t="s">
+      <c r="D17" s="186" t="s">
         <v>413</v>
       </c>
       <c r="E17" s="74" t="s">
@@ -15504,7 +15510,7 @@
       <c r="E20" s="79" t="s">
         <v>456</v>
       </c>
-      <c r="F20" s="193" t="s">
+      <c r="F20" s="191" t="s">
         <v>17</v>
       </c>
       <c r="G20" s="125" t="s">
@@ -15534,7 +15540,7 @@
       <c r="C21" s="126" t="s">
         <v>248</v>
       </c>
-      <c r="D21" s="157" t="s">
+      <c r="D21" s="155" t="s">
         <v>458</v>
       </c>
       <c r="E21" s="81" t="s">
@@ -16054,7 +16060,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -16074,7 +16080,7 @@
     <col min="13" max="16384" width="9.109375" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="202" customFormat="1" ht="43.2">
+    <row r="1" spans="1:12" s="200" customFormat="1" ht="43.2">
       <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
@@ -16105,7 +16111,7 @@
       <c r="J1" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="203" t="s">
+      <c r="K1" s="201" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="108" t="s">
@@ -16113,7 +16119,7 @@
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="194" t="s">
+      <c r="A2" s="192" t="s">
         <v>32</v>
       </c>
       <c r="B2" s="74" t="s">
@@ -16134,10 +16140,10 @@
       <c r="G2" s="128" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="195" t="s">
+      <c r="H2" s="193" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="195" t="s">
+      <c r="I2" s="193" t="s">
         <v>19</v>
       </c>
       <c r="J2" s="107" t="s">
@@ -16255,104 +16261,104 @@
       <c r="L5" s="107"/>
     </row>
     <row r="6" spans="1:12" ht="28.8">
-      <c r="A6" s="224" t="s">
+      <c r="A6" s="225" t="s">
         <v>95</v>
       </c>
-      <c r="B6" s="225" t="s">
+      <c r="B6" s="226" t="s">
         <v>96</v>
       </c>
-      <c r="C6" s="224" t="s">
+      <c r="C6" s="225" t="s">
         <v>97</v>
       </c>
-      <c r="D6" s="140" t="s">
+      <c r="D6" s="230" t="s">
         <v>98</v>
       </c>
-      <c r="E6" s="226" t="s">
+      <c r="E6" s="227" t="s">
         <v>99</v>
       </c>
-      <c r="F6" s="223" t="s">
+      <c r="F6" s="224" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="223" t="s">
+      <c r="G6" s="224" t="s">
         <v>100</v>
       </c>
-      <c r="H6" s="223" t="s">
+      <c r="H6" s="224" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="227" t="s">
+      <c r="I6" s="222" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="220" t="s">
+      <c r="J6" s="215" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="228" t="s">
+      <c r="K6" s="223" t="s">
         <v>471</v>
       </c>
-      <c r="L6" s="227"/>
+      <c r="L6" s="222"/>
     </row>
     <row r="7" spans="1:12" ht="28.8">
-      <c r="A7" s="224"/>
-      <c r="B7" s="225"/>
-      <c r="C7" s="224"/>
-      <c r="D7" s="141" t="s">
+      <c r="A7" s="225"/>
+      <c r="B7" s="226"/>
+      <c r="C7" s="225"/>
+      <c r="D7" s="231" t="s">
         <v>101</v>
       </c>
-      <c r="E7" s="226"/>
-      <c r="F7" s="223"/>
-      <c r="G7" s="223"/>
-      <c r="H7" s="223"/>
-      <c r="I7" s="227"/>
-      <c r="J7" s="220"/>
-      <c r="K7" s="228"/>
-      <c r="L7" s="227"/>
+      <c r="E7" s="227"/>
+      <c r="F7" s="224"/>
+      <c r="G7" s="224"/>
+      <c r="H7" s="224"/>
+      <c r="I7" s="222"/>
+      <c r="J7" s="215"/>
+      <c r="K7" s="223"/>
+      <c r="L7" s="222"/>
     </row>
     <row r="8" spans="1:12" ht="28.8">
-      <c r="A8" s="224"/>
-      <c r="B8" s="225"/>
-      <c r="C8" s="224"/>
-      <c r="D8" s="141" t="s">
+      <c r="A8" s="225"/>
+      <c r="B8" s="226"/>
+      <c r="C8" s="225"/>
+      <c r="D8" s="231" t="s">
         <v>102</v>
       </c>
-      <c r="E8" s="226"/>
-      <c r="F8" s="223"/>
-      <c r="G8" s="223"/>
-      <c r="H8" s="223"/>
-      <c r="I8" s="227"/>
-      <c r="J8" s="220"/>
-      <c r="K8" s="228"/>
-      <c r="L8" s="227"/>
+      <c r="E8" s="227"/>
+      <c r="F8" s="224"/>
+      <c r="G8" s="224"/>
+      <c r="H8" s="224"/>
+      <c r="I8" s="222"/>
+      <c r="J8" s="215"/>
+      <c r="K8" s="223"/>
+      <c r="L8" s="222"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="224"/>
-      <c r="B9" s="225"/>
-      <c r="C9" s="224"/>
-      <c r="D9" s="141" t="s">
+      <c r="A9" s="225"/>
+      <c r="B9" s="226"/>
+      <c r="C9" s="225"/>
+      <c r="D9" s="140" t="s">
         <v>103</v>
       </c>
-      <c r="E9" s="226"/>
-      <c r="F9" s="223"/>
-      <c r="G9" s="223"/>
-      <c r="H9" s="223"/>
-      <c r="I9" s="227"/>
-      <c r="J9" s="220"/>
-      <c r="K9" s="228"/>
-      <c r="L9" s="227"/>
+      <c r="E9" s="227"/>
+      <c r="F9" s="224"/>
+      <c r="G9" s="224"/>
+      <c r="H9" s="224"/>
+      <c r="I9" s="222"/>
+      <c r="J9" s="215"/>
+      <c r="K9" s="223"/>
+      <c r="L9" s="222"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="224"/>
-      <c r="B10" s="225"/>
-      <c r="C10" s="224"/>
-      <c r="D10" s="141" t="s">
+      <c r="A10" s="225"/>
+      <c r="B10" s="226"/>
+      <c r="C10" s="225"/>
+      <c r="D10" s="140" t="s">
         <v>104</v>
       </c>
-      <c r="E10" s="226"/>
-      <c r="F10" s="223"/>
-      <c r="G10" s="223"/>
-      <c r="H10" s="223"/>
-      <c r="I10" s="227"/>
-      <c r="J10" s="220"/>
-      <c r="K10" s="228"/>
-      <c r="L10" s="227"/>
+      <c r="E10" s="227"/>
+      <c r="F10" s="224"/>
+      <c r="G10" s="224"/>
+      <c r="H10" s="224"/>
+      <c r="I10" s="222"/>
+      <c r="J10" s="215"/>
+      <c r="K10" s="223"/>
+      <c r="L10" s="222"/>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="122" t="s">
@@ -16484,10 +16490,10 @@
       <c r="G14" s="129" t="s">
         <v>234</v>
       </c>
-      <c r="H14" s="196" t="s">
+      <c r="H14" s="194" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="196" t="s">
+      <c r="I14" s="194" t="s">
         <v>19</v>
       </c>
       <c r="J14" s="107" t="s">
@@ -16657,17 +16663,17 @@
   </sheetData>
   <autoFilter ref="A1:L15" xr:uid="{FBE7E653-2382-46E4-9C76-9C694EDC9195}"/>
   <mergeCells count="11">
-    <mergeCell ref="L6:L10"/>
-    <mergeCell ref="K6:K10"/>
-    <mergeCell ref="H6:H10"/>
-    <mergeCell ref="I6:I10"/>
-    <mergeCell ref="J6:J10"/>
     <mergeCell ref="G6:G10"/>
     <mergeCell ref="A6:A10"/>
     <mergeCell ref="B6:B10"/>
     <mergeCell ref="C6:C10"/>
     <mergeCell ref="E6:E10"/>
     <mergeCell ref="F6:F10"/>
+    <mergeCell ref="L6:L10"/>
+    <mergeCell ref="K6:K10"/>
+    <mergeCell ref="H6:H10"/>
+    <mergeCell ref="I6:I10"/>
+    <mergeCell ref="J6:J10"/>
   </mergeCells>
   <conditionalFormatting sqref="F2:F6 F11:F15">
     <cfRule type="cellIs" dxfId="127" priority="7" operator="equal">
@@ -16759,7 +16765,7 @@
   </sheetPr>
   <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
@@ -16780,7 +16786,7 @@
     <col min="12" max="12" width="25.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="205" customFormat="1" ht="43.2">
+    <row r="1" spans="1:12" s="203" customFormat="1" ht="43.2">
       <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
@@ -16811,7 +16817,7 @@
       <c r="J1" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="203" t="s">
+      <c r="K1" s="201" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="108" t="s">
@@ -16828,7 +16834,7 @@
       <c r="C2" s="122" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="145" t="s">
+      <c r="D2" s="144" t="s">
         <v>15</v>
       </c>
       <c r="E2" s="82" t="s">
@@ -16852,7 +16858,7 @@
       <c r="K2" s="107" t="s">
         <v>481</v>
       </c>
-      <c r="L2" s="189"/>
+      <c r="L2" s="187"/>
     </row>
     <row r="3" spans="1:12" ht="28.8">
       <c r="A3" s="126" t="s">
@@ -16899,7 +16905,7 @@
       <c r="D4" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="197" t="s">
+      <c r="E4" s="195" t="s">
         <v>483</v>
       </c>
       <c r="F4" s="125" t="s">
@@ -16921,7 +16927,7 @@
       <c r="L4" s="107"/>
     </row>
     <row r="5" spans="1:12" ht="72">
-      <c r="A5" s="194" t="s">
+      <c r="A5" s="192" t="s">
         <v>56</v>
       </c>
       <c r="B5" s="74" t="s">
@@ -16933,7 +16939,7 @@
       <c r="D5" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="142" t="s">
+      <c r="E5" s="141" t="s">
         <v>484</v>
       </c>
       <c r="F5" s="128" t="s">
@@ -17069,7 +17075,7 @@
       <c r="D9" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="229" t="s">
+      <c r="E9" s="214" t="s">
         <v>606</v>
       </c>
       <c r="F9" s="128" t="s">
@@ -17138,7 +17144,7 @@
       <c r="C11" s="135" t="s">
         <v>428</v>
       </c>
-      <c r="D11" s="157" t="s">
+      <c r="D11" s="155" t="s">
         <v>429</v>
       </c>
       <c r="E11" s="127"/>
@@ -17193,7 +17199,7 @@
       <c r="L12" s="107"/>
     </row>
     <row r="13" spans="1:12" ht="57.6">
-      <c r="A13" s="194" t="s">
+      <c r="A13" s="192" t="s">
         <v>116</v>
       </c>
       <c r="B13" s="74" t="s">
@@ -17302,7 +17308,7 @@
       <c r="C16" s="122" t="s">
         <v>139</v>
       </c>
-      <c r="D16" s="191" t="s">
+      <c r="D16" s="189" t="s">
         <v>140</v>
       </c>
       <c r="E16" s="35" t="s">
@@ -17336,7 +17342,7 @@
       <c r="C17" s="126" t="s">
         <v>319</v>
       </c>
-      <c r="D17" s="144" t="s">
+      <c r="D17" s="143" t="s">
         <v>320</v>
       </c>
       <c r="E17" s="80" t="s">
@@ -17508,7 +17514,7 @@
       <c r="C22" s="122" t="s">
         <v>265</v>
       </c>
-      <c r="D22" s="145" t="s">
+      <c r="D22" s="144" t="s">
         <v>266</v>
       </c>
       <c r="E22" s="35" t="s">
@@ -17566,7 +17572,7 @@
       <c r="K23" s="106" t="s">
         <v>517</v>
       </c>
-      <c r="L23" s="198"/>
+      <c r="L23" s="196"/>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="23"/>
@@ -18044,15 +18050,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Status xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">Draft</Status>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="221af607-abea-4d5e-830c-567dcc03c0ec" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18299,21 +18302,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Status xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">Draft</Status>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="221af607-abea-4d5e-830c-567dcc03c0ec" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16D2CAB5-B21B-4A93-9D82-49FE3E36CF14}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1A00443-9B7C-473F-A198-CBEB23A0BCC5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cfc87205-1831-4b6c-a7b4-76d40079a43e"/>
-    <ds:schemaRef ds:uri="221af607-abea-4d5e-830c-567dcc03c0ec"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -18338,9 +18341,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1A00443-9B7C-473F-A198-CBEB23A0BCC5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16D2CAB5-B21B-4A93-9D82-49FE3E36CF14}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cfc87205-1831-4b6c-a7b4-76d40079a43e"/>
+    <ds:schemaRef ds:uri="221af607-abea-4d5e-830c-567dcc03c0ec"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fix: remove xsd:string and add uniqueLang (#244)
* fix: remove xsd:string and add uniqueLang

* fix: URLs to spatial EU vocabs

* docs: update changelog

* fix: remove unused prefix and correct property description
</commit_message>
<xml_diff>
--- a/Documents/Metadata_CoreGenericHealth_v2.xlsx
+++ b/Documents/Metadata_CoreGenericHealth_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://healthri-my.sharepoint.com/personal/hannah_neikes_health-ri_nl/Documents/Documenten/GitHub/health-ri-metadata/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3216" documentId="13_ncr:1_{F400FBA4-788C-A049-BCFC-7AF7AD8163AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B34781B7-C461-4DB0-AF31-0C0F180972E1}"/>
+  <xr:revisionPtr revIDLastSave="3225" documentId="13_ncr:1_{F400FBA4-788C-A049-BCFC-7AF7AD8163AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC6F41C7-8696-4345-9896-16B847EC9B3E}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-12765" windowWidth="38640" windowHeight="21120" firstSheet="2" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4680" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="14" r:id="rId1"/>
@@ -2566,7 +2566,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="230">
+  <cellXfs count="232">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2980,9 +2980,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3020,9 +3017,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -3195,28 +3189,37 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="50" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3228,14 +3231,17 @@
     <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -6817,7 +6823,7 @@
     <col min="11" max="11" width="22.33203125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="206" customFormat="1" ht="43.2">
+    <row r="1" spans="1:12" s="204" customFormat="1" ht="43.2">
       <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
@@ -6848,7 +6854,7 @@
       <c r="J1" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="203" t="s">
+      <c r="K1" s="201" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="108" t="s">
@@ -6856,7 +6862,7 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="72">
-      <c r="A2" s="199" t="s">
+      <c r="A2" s="197" t="s">
         <v>518</v>
       </c>
       <c r="B2" s="45" t="s">
@@ -6865,29 +6871,29 @@
       <c r="C2" s="76" t="s">
         <v>520</v>
       </c>
-      <c r="D2" s="199" t="s">
+      <c r="D2" s="197" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="200" t="s">
+      <c r="E2" s="198" t="s">
         <v>521</v>
       </c>
-      <c r="F2" s="201" t="s">
+      <c r="F2" s="199" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="162" t="s">
+      <c r="G2" s="160" t="s">
         <v>75</v>
       </c>
-      <c r="H2" s="201" t="s">
+      <c r="H2" s="199" t="s">
         <v>522</v>
       </c>
-      <c r="I2" s="163" t="s">
+      <c r="I2" s="161" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="163" t="s">
+      <c r="J2" s="161" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="159"/>
-      <c r="L2" s="189"/>
+      <c r="K2" s="157"/>
+      <c r="L2" s="187"/>
     </row>
     <row r="3" spans="1:12" ht="28.8">
       <c r="A3" s="68" t="s">
@@ -6902,24 +6908,24 @@
       <c r="D3" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="165"/>
-      <c r="F3" s="166" t="s">
+      <c r="E3" s="163"/>
+      <c r="F3" s="164" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="166" t="s">
+      <c r="G3" s="164" t="s">
         <v>75</v>
       </c>
-      <c r="H3" s="166" t="s">
+      <c r="H3" s="164" t="s">
         <v>93</v>
       </c>
-      <c r="I3" s="167" t="s">
+      <c r="I3" s="165" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="163" t="s">
+      <c r="J3" s="161" t="s">
         <v>76</v>
       </c>
-      <c r="K3" s="170"/>
-      <c r="L3" s="198"/>
+      <c r="K3" s="168"/>
+      <c r="L3" s="196"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2:F3">
@@ -8999,13 +9005,13 @@
       <c r="D2" s="78" t="s">
         <v>599</v>
       </c>
-      <c r="E2" s="200" t="s">
+      <c r="E2" s="198" t="s">
         <v>600</v>
       </c>
       <c r="F2" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="207" t="s">
+      <c r="G2" s="205" t="s">
         <v>601</v>
       </c>
       <c r="H2" s="47">
@@ -9669,8 +9675,8 @@
   <dimension ref="A1:L53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -9690,7 +9696,7 @@
     <col min="13" max="16384" width="9.109375" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="202" customFormat="1" ht="41.4">
+    <row r="1" spans="1:12" s="200" customFormat="1" ht="41.4">
       <c r="A1" s="91" t="s">
         <v>0</v>
       </c>
@@ -10047,12 +10053,12 @@
       <c r="J10" s="107" t="s">
         <v>76</v>
       </c>
-      <c r="K10" s="209" t="s">
+      <c r="K10" s="207" t="s">
         <v>77</v>
       </c>
       <c r="L10" s="107"/>
     </row>
-    <row r="11" spans="1:12" s="210" customFormat="1">
+    <row r="11" spans="1:12" s="208" customFormat="1">
       <c r="A11" s="126" t="s">
         <v>78</v>
       </c>
@@ -10065,7 +10071,7 @@
       <c r="D11" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="E11" s="142" t="s">
+      <c r="E11" s="141" t="s">
         <v>81</v>
       </c>
       <c r="F11" s="128" t="s">
@@ -10132,7 +10138,7 @@
       <c r="C13" s="126" t="s">
         <v>90</v>
       </c>
-      <c r="D13" s="144" t="s">
+      <c r="D13" s="143" t="s">
         <v>91</v>
       </c>
       <c r="E13" s="80" t="s">
@@ -10159,102 +10165,102 @@
       <c r="L13" s="130"/>
     </row>
     <row r="14" spans="1:12" ht="43.2">
-      <c r="A14" s="216" t="s">
+      <c r="A14" s="218" t="s">
         <v>95</v>
       </c>
-      <c r="B14" s="217" t="s">
+      <c r="B14" s="219" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="216" t="s">
+      <c r="C14" s="218" t="s">
         <v>97</v>
       </c>
-      <c r="D14" s="154" t="s">
+      <c r="D14" s="228" t="s">
         <v>98</v>
       </c>
-      <c r="E14" s="219" t="s">
+      <c r="E14" s="220" t="s">
         <v>99</v>
       </c>
-      <c r="F14" s="218" t="s">
+      <c r="F14" s="217" t="s">
         <v>27</v>
       </c>
-      <c r="G14" s="218" t="s">
+      <c r="G14" s="217" t="s">
         <v>100</v>
       </c>
-      <c r="H14" s="218" t="s">
+      <c r="H14" s="217" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="220" t="s">
+      <c r="I14" s="215" t="s">
         <v>19</v>
       </c>
-      <c r="J14" s="220" t="s">
+      <c r="J14" s="215" t="s">
         <v>30</v>
       </c>
-      <c r="K14" s="221"/>
-      <c r="L14" s="220"/>
+      <c r="K14" s="216"/>
+      <c r="L14" s="215"/>
     </row>
     <row r="15" spans="1:12" ht="43.2">
-      <c r="A15" s="216"/>
-      <c r="B15" s="217"/>
-      <c r="C15" s="216"/>
-      <c r="D15" s="155" t="s">
+      <c r="A15" s="218"/>
+      <c r="B15" s="219"/>
+      <c r="C15" s="218"/>
+      <c r="D15" s="229" t="s">
         <v>101</v>
       </c>
-      <c r="E15" s="219"/>
-      <c r="F15" s="218"/>
-      <c r="G15" s="218"/>
-      <c r="H15" s="218"/>
-      <c r="I15" s="220"/>
-      <c r="J15" s="220"/>
-      <c r="K15" s="221"/>
-      <c r="L15" s="220"/>
+      <c r="E15" s="220"/>
+      <c r="F15" s="217"/>
+      <c r="G15" s="217"/>
+      <c r="H15" s="217"/>
+      <c r="I15" s="215"/>
+      <c r="J15" s="215"/>
+      <c r="K15" s="216"/>
+      <c r="L15" s="215"/>
     </row>
     <row r="16" spans="1:12" ht="28.8">
-      <c r="A16" s="216"/>
-      <c r="B16" s="217"/>
-      <c r="C16" s="216"/>
-      <c r="D16" s="155" t="s">
+      <c r="A16" s="218"/>
+      <c r="B16" s="219"/>
+      <c r="C16" s="218"/>
+      <c r="D16" s="229" t="s">
         <v>102</v>
       </c>
-      <c r="E16" s="219"/>
-      <c r="F16" s="218"/>
-      <c r="G16" s="218"/>
-      <c r="H16" s="218"/>
-      <c r="I16" s="220"/>
-      <c r="J16" s="220"/>
-      <c r="K16" s="221"/>
-      <c r="L16" s="220"/>
+      <c r="E16" s="220"/>
+      <c r="F16" s="217"/>
+      <c r="G16" s="217"/>
+      <c r="H16" s="217"/>
+      <c r="I16" s="215"/>
+      <c r="J16" s="215"/>
+      <c r="K16" s="216"/>
+      <c r="L16" s="215"/>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="216"/>
-      <c r="B17" s="217"/>
-      <c r="C17" s="216"/>
-      <c r="D17" s="155" t="s">
+      <c r="A17" s="218"/>
+      <c r="B17" s="219"/>
+      <c r="C17" s="218"/>
+      <c r="D17" s="153" t="s">
         <v>103</v>
       </c>
-      <c r="E17" s="219"/>
-      <c r="F17" s="218"/>
-      <c r="G17" s="218"/>
-      <c r="H17" s="218"/>
-      <c r="I17" s="220"/>
-      <c r="J17" s="220"/>
-      <c r="K17" s="221"/>
-      <c r="L17" s="220"/>
+      <c r="E17" s="220"/>
+      <c r="F17" s="217"/>
+      <c r="G17" s="217"/>
+      <c r="H17" s="217"/>
+      <c r="I17" s="215"/>
+      <c r="J17" s="215"/>
+      <c r="K17" s="216"/>
+      <c r="L17" s="215"/>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="216"/>
-      <c r="B18" s="217"/>
-      <c r="C18" s="216"/>
-      <c r="D18" s="155" t="s">
+      <c r="A18" s="218"/>
+      <c r="B18" s="219"/>
+      <c r="C18" s="218"/>
+      <c r="D18" s="153" t="s">
         <v>104</v>
       </c>
-      <c r="E18" s="219"/>
-      <c r="F18" s="218"/>
-      <c r="G18" s="218"/>
-      <c r="H18" s="218"/>
-      <c r="I18" s="220"/>
-      <c r="J18" s="220"/>
-      <c r="K18" s="221"/>
-      <c r="L18" s="220"/>
+      <c r="E18" s="220"/>
+      <c r="F18" s="217"/>
+      <c r="G18" s="217"/>
+      <c r="H18" s="217"/>
+      <c r="I18" s="215"/>
+      <c r="J18" s="215"/>
+      <c r="K18" s="216"/>
+      <c r="L18" s="215"/>
     </row>
     <row r="19" spans="1:12" ht="28.8">
       <c r="A19" s="126" t="s">
@@ -10287,7 +10293,7 @@
       <c r="J19" s="130" t="s">
         <v>76</v>
       </c>
-      <c r="K19" s="211" t="s">
+      <c r="K19" s="209" t="s">
         <v>110</v>
       </c>
       <c r="L19" s="130"/>
@@ -10341,7 +10347,7 @@
       <c r="D21" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="212" t="s">
+      <c r="E21" s="210" t="s">
         <v>119</v>
       </c>
       <c r="F21" s="128" t="s">
@@ -10429,7 +10435,7 @@
       <c r="J23" s="130" t="s">
         <v>76</v>
       </c>
-      <c r="K23" s="211" t="s">
+      <c r="K23" s="209" t="s">
         <v>131</v>
       </c>
       <c r="L23" s="130"/>
@@ -10441,7 +10447,7 @@
       <c r="B24" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="C24" s="143" t="s">
+      <c r="C24" s="142" t="s">
         <v>134</v>
       </c>
       <c r="D24" s="133" t="s">
@@ -10480,7 +10486,7 @@
       <c r="C25" s="135" t="s">
         <v>139</v>
       </c>
-      <c r="D25" s="144" t="s">
+      <c r="D25" s="143" t="s">
         <v>140</v>
       </c>
       <c r="E25" s="127" t="s">
@@ -10501,7 +10507,7 @@
       <c r="J25" s="130" t="s">
         <v>76</v>
       </c>
-      <c r="K25" s="213" t="s">
+      <c r="K25" s="211" t="s">
         <v>143</v>
       </c>
       <c r="L25" s="130"/>
@@ -10513,7 +10519,7 @@
       <c r="B26" s="35" t="s">
         <v>145</v>
       </c>
-      <c r="C26" s="143" t="s">
+      <c r="C26" s="142" t="s">
         <v>146</v>
       </c>
       <c r="D26" s="123" t="s">
@@ -10585,7 +10591,7 @@
       <c r="B28" s="35" t="s">
         <v>158</v>
       </c>
-      <c r="C28" s="143" t="s">
+      <c r="C28" s="142" t="s">
         <v>159</v>
       </c>
       <c r="D28" s="133" t="s">
@@ -10768,7 +10774,7 @@
       <c r="C33" s="126" t="s">
         <v>187</v>
       </c>
-      <c r="D33" s="144" t="s">
+      <c r="D33" s="143" t="s">
         <v>188</v>
       </c>
       <c r="E33" s="80" t="s">
@@ -10843,7 +10849,7 @@
       <c r="D35" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="E35" s="208" t="s">
+      <c r="E35" s="206" t="s">
         <v>200</v>
       </c>
       <c r="F35" s="128" t="s">
@@ -11160,7 +11166,7 @@
       <c r="C44" s="122" t="s">
         <v>248</v>
       </c>
-      <c r="D44" s="184" t="s">
+      <c r="D44" s="182" t="s">
         <v>249</v>
       </c>
       <c r="E44" s="133" t="s">
@@ -11229,7 +11235,7 @@
       <c r="B46" s="35" t="s">
         <v>258</v>
       </c>
-      <c r="C46" s="143" t="s">
+      <c r="C46" s="142" t="s">
         <v>259</v>
       </c>
       <c r="D46" s="133" t="s">
@@ -11268,7 +11274,7 @@
       <c r="C47" s="126" t="s">
         <v>265</v>
       </c>
-      <c r="D47" s="144" t="s">
+      <c r="D47" s="143" t="s">
         <v>266</v>
       </c>
       <c r="E47" s="74" t="s">
@@ -11340,7 +11346,7 @@
       <c r="C49" s="126" t="s">
         <v>275</v>
       </c>
-      <c r="D49" s="188" t="s">
+      <c r="D49" s="186" t="s">
         <v>276</v>
       </c>
       <c r="E49" s="83" t="s">
@@ -11471,18 +11477,18 @@
       <c r="L52" s="107"/>
     </row>
     <row r="53" spans="1:12" s="119" customFormat="1">
-      <c r="A53" s="147"/>
-      <c r="B53" s="148"/>
-      <c r="C53" s="147"/>
-      <c r="D53" s="149"/>
-      <c r="E53" s="149"/>
-      <c r="F53" s="150"/>
-      <c r="G53" s="150"/>
-      <c r="H53" s="150"/>
-      <c r="I53" s="151"/>
-      <c r="J53" s="151"/>
-      <c r="K53" s="152"/>
-      <c r="L53" s="151"/>
+      <c r="A53" s="146"/>
+      <c r="B53" s="147"/>
+      <c r="C53" s="146"/>
+      <c r="D53" s="148"/>
+      <c r="E53" s="148"/>
+      <c r="F53" s="149"/>
+      <c r="G53" s="149"/>
+      <c r="H53" s="149"/>
+      <c r="I53" s="150"/>
+      <c r="J53" s="150"/>
+      <c r="K53" s="151"/>
+      <c r="L53" s="150"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J53" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
@@ -11490,17 +11496,17 @@
     <sortCondition ref="A2:A53"/>
   </sortState>
   <mergeCells count="11">
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="C14:C18"/>
+    <mergeCell ref="F14:F18"/>
+    <mergeCell ref="E14:E18"/>
     <mergeCell ref="L14:L18"/>
     <mergeCell ref="K14:K18"/>
     <mergeCell ref="G14:G18"/>
     <mergeCell ref="H14:H18"/>
     <mergeCell ref="I14:I18"/>
     <mergeCell ref="J14:J18"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="C14:C18"/>
-    <mergeCell ref="F14:F18"/>
-    <mergeCell ref="E14:E18"/>
   </mergeCells>
   <conditionalFormatting sqref="F2:F14 F19:F53">
     <cfRule type="cellIs" dxfId="190" priority="8" operator="equal">
@@ -11605,7 +11611,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N16" sqref="N16"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -11625,7 +11631,7 @@
     <col min="13" max="16384" width="9.109375" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="202" customFormat="1" ht="57.6">
+    <row r="1" spans="1:12" s="200" customFormat="1" ht="57.6">
       <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
@@ -11670,7 +11676,7 @@
       <c r="B2" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="143" t="s">
+      <c r="C2" s="142" t="s">
         <v>34</v>
       </c>
       <c r="D2" s="133" t="s">
@@ -11872,102 +11878,102 @@
       <c r="L7" s="130"/>
     </row>
     <row r="8" spans="1:12" ht="28.8">
-      <c r="A8" s="216" t="s">
+      <c r="A8" s="218" t="s">
         <v>95</v>
       </c>
-      <c r="B8" s="222" t="s">
+      <c r="B8" s="221" t="s">
         <v>96</v>
       </c>
-      <c r="C8" s="216" t="s">
+      <c r="C8" s="218" t="s">
         <v>97</v>
       </c>
-      <c r="D8" s="154" t="s">
+      <c r="D8" s="228" t="s">
         <v>98</v>
       </c>
-      <c r="E8" s="219" t="s">
+      <c r="E8" s="220" t="s">
         <v>307</v>
       </c>
-      <c r="F8" s="218" t="s">
+      <c r="F8" s="217" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="218" t="s">
+      <c r="G8" s="217" t="s">
         <v>100</v>
       </c>
-      <c r="H8" s="218" t="s">
+      <c r="H8" s="217" t="s">
         <v>29</v>
       </c>
-      <c r="I8" s="220" t="s">
+      <c r="I8" s="215" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="220" t="s">
+      <c r="J8" s="215" t="s">
         <v>30</v>
       </c>
       <c r="K8" s="138"/>
-      <c r="L8" s="220"/>
+      <c r="L8" s="215"/>
     </row>
     <row r="9" spans="1:12" ht="28.8">
-      <c r="A9" s="216"/>
-      <c r="B9" s="222"/>
-      <c r="C9" s="216"/>
-      <c r="D9" s="155" t="s">
+      <c r="A9" s="218"/>
+      <c r="B9" s="221"/>
+      <c r="C9" s="218"/>
+      <c r="D9" s="229" t="s">
         <v>101</v>
       </c>
-      <c r="E9" s="219"/>
-      <c r="F9" s="218"/>
-      <c r="G9" s="218"/>
-      <c r="H9" s="218"/>
-      <c r="I9" s="220"/>
-      <c r="J9" s="220"/>
+      <c r="E9" s="220"/>
+      <c r="F9" s="217"/>
+      <c r="G9" s="217"/>
+      <c r="H9" s="217"/>
+      <c r="I9" s="215"/>
+      <c r="J9" s="215"/>
       <c r="K9" s="138"/>
-      <c r="L9" s="220"/>
+      <c r="L9" s="215"/>
     </row>
     <row r="10" spans="1:12" ht="28.8">
-      <c r="A10" s="216"/>
-      <c r="B10" s="222"/>
-      <c r="C10" s="216"/>
-      <c r="D10" s="155" t="s">
+      <c r="A10" s="218"/>
+      <c r="B10" s="221"/>
+      <c r="C10" s="218"/>
+      <c r="D10" s="229" t="s">
         <v>102</v>
       </c>
-      <c r="E10" s="219"/>
-      <c r="F10" s="218"/>
-      <c r="G10" s="218"/>
-      <c r="H10" s="218"/>
-      <c r="I10" s="220"/>
-      <c r="J10" s="220"/>
+      <c r="E10" s="220"/>
+      <c r="F10" s="217"/>
+      <c r="G10" s="217"/>
+      <c r="H10" s="217"/>
+      <c r="I10" s="215"/>
+      <c r="J10" s="215"/>
       <c r="K10" s="138"/>
-      <c r="L10" s="220"/>
+      <c r="L10" s="215"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="216"/>
-      <c r="B11" s="222"/>
-      <c r="C11" s="216"/>
-      <c r="D11" s="155" t="s">
+      <c r="A11" s="218"/>
+      <c r="B11" s="221"/>
+      <c r="C11" s="218"/>
+      <c r="D11" s="153" t="s">
         <v>103</v>
       </c>
-      <c r="E11" s="219"/>
-      <c r="F11" s="218"/>
-      <c r="G11" s="218"/>
-      <c r="H11" s="218"/>
-      <c r="I11" s="220"/>
-      <c r="J11" s="220"/>
-      <c r="K11" s="156"/>
-      <c r="L11" s="220"/>
+      <c r="E11" s="220"/>
+      <c r="F11" s="217"/>
+      <c r="G11" s="217"/>
+      <c r="H11" s="217"/>
+      <c r="I11" s="215"/>
+      <c r="J11" s="215"/>
+      <c r="K11" s="154"/>
+      <c r="L11" s="215"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="216"/>
-      <c r="B12" s="222"/>
-      <c r="C12" s="216"/>
-      <c r="D12" s="155" t="s">
+      <c r="A12" s="218"/>
+      <c r="B12" s="221"/>
+      <c r="C12" s="218"/>
+      <c r="D12" s="153" t="s">
         <v>104</v>
       </c>
-      <c r="E12" s="219"/>
-      <c r="F12" s="218"/>
-      <c r="G12" s="218"/>
-      <c r="H12" s="218"/>
-      <c r="I12" s="220"/>
-      <c r="J12" s="220"/>
+      <c r="E12" s="220"/>
+      <c r="F12" s="217"/>
+      <c r="G12" s="217"/>
+      <c r="H12" s="217"/>
+      <c r="I12" s="215"/>
+      <c r="J12" s="215"/>
       <c r="K12" s="138"/>
-      <c r="L12" s="220"/>
+      <c r="L12" s="215"/>
     </row>
     <row r="13" spans="1:12" ht="43.2">
       <c r="A13" s="126" t="s">
@@ -12016,7 +12022,7 @@
       <c r="D14" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="143" t="s">
+      <c r="E14" s="142" t="s">
         <v>315</v>
       </c>
       <c r="F14" s="125" t="s">
@@ -12047,7 +12053,7 @@
       <c r="C15" s="126" t="s">
         <v>139</v>
       </c>
-      <c r="D15" s="157" t="s">
+      <c r="D15" s="155" t="s">
         <v>140</v>
       </c>
       <c r="E15" s="74" t="s">
@@ -12068,7 +12074,7 @@
       <c r="J15" s="107" t="s">
         <v>76</v>
       </c>
-      <c r="K15" s="158" t="s">
+      <c r="K15" s="156" t="s">
         <v>143</v>
       </c>
       <c r="L15" s="130"/>
@@ -12080,10 +12086,10 @@
       <c r="B16" s="35" t="s">
         <v>318</v>
       </c>
-      <c r="C16" s="143" t="s">
+      <c r="C16" s="142" t="s">
         <v>319</v>
       </c>
-      <c r="D16" s="145" t="s">
+      <c r="D16" s="144" t="s">
         <v>320</v>
       </c>
       <c r="E16" s="35" t="s">
@@ -12104,7 +12110,7 @@
       <c r="J16" s="107" t="s">
         <v>76</v>
       </c>
-      <c r="K16" s="158" t="s">
+      <c r="K16" s="156" t="s">
         <v>323</v>
       </c>
       <c r="L16" s="107"/>
@@ -12138,7 +12144,7 @@
       <c r="J17" s="107" t="s">
         <v>76</v>
       </c>
-      <c r="K17" s="158" t="s">
+      <c r="K17" s="156" t="s">
         <v>167</v>
       </c>
       <c r="L17" s="130"/>
@@ -12150,7 +12156,7 @@
       <c r="B18" s="35" t="s">
         <v>198</v>
       </c>
-      <c r="C18" s="143" t="s">
+      <c r="C18" s="142" t="s">
         <v>199</v>
       </c>
       <c r="D18" s="133" t="s">
@@ -12174,7 +12180,7 @@
       <c r="J18" s="107" t="s">
         <v>76</v>
       </c>
-      <c r="K18" s="158" t="s">
+      <c r="K18" s="156" t="s">
         <v>201</v>
       </c>
       <c r="L18" s="107"/>
@@ -12208,7 +12214,7 @@
       <c r="J19" s="130" t="s">
         <v>76</v>
       </c>
-      <c r="K19" s="211" t="s">
+      <c r="K19" s="209" t="s">
         <v>229</v>
       </c>
       <c r="L19" s="130"/>
@@ -12226,7 +12232,7 @@
       <c r="D20" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="214" t="s">
+      <c r="E20" s="212" t="s">
         <v>328</v>
       </c>
       <c r="F20" s="125" t="s">
@@ -12346,7 +12352,7 @@
       <c r="J23" s="130" t="s">
         <v>76</v>
       </c>
-      <c r="K23" s="211"/>
+      <c r="K23" s="209"/>
       <c r="L23" s="130"/>
     </row>
     <row r="24" spans="1:12" ht="28.8">
@@ -12362,7 +12368,7 @@
       <c r="D24" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="E24" s="215" t="s">
+      <c r="E24" s="213" t="s">
         <v>338</v>
       </c>
       <c r="F24" s="125" t="s">
@@ -12890,28 +12896,28 @@
   <dimension ref="A1:L57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="18" style="181" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38" style="181" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" style="181" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.44140625" style="178" customWidth="1"/>
-    <col min="5" max="5" width="65.88671875" style="181" customWidth="1"/>
+    <col min="1" max="1" width="18" style="179" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38" style="179" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" style="179" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.44140625" style="176" customWidth="1"/>
+    <col min="5" max="5" width="65.88671875" style="179" customWidth="1"/>
     <col min="6" max="6" width="18.6640625" style="137" customWidth="1"/>
     <col min="7" max="7" width="17.44140625" style="137" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" style="185" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" style="183" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.5546875" style="137" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19" style="137" customWidth="1"/>
-    <col min="11" max="11" width="39.33203125" style="159" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="39.33203125" style="157" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="26.6640625" style="137" customWidth="1"/>
     <col min="13" max="16384" width="8.88671875" style="137"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="204" customFormat="1" ht="43.2">
+    <row r="1" spans="1:12" s="202" customFormat="1" ht="43.2">
       <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
@@ -12942,7 +12948,7 @@
       <c r="J1" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="203" t="s">
+      <c r="K1" s="201" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="108" t="s">
@@ -12953,32 +12959,32 @@
       <c r="A2" s="64" t="s">
         <v>339</v>
       </c>
-      <c r="B2" s="160" t="s">
+      <c r="B2" s="158" t="s">
         <v>96</v>
       </c>
       <c r="C2" s="64" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="155" t="s">
+      <c r="D2" s="153" t="s">
         <v>340</v>
       </c>
-      <c r="E2" s="161" t="s">
+      <c r="E2" s="159" t="s">
         <v>341</v>
       </c>
-      <c r="F2" s="162" t="s">
+      <c r="F2" s="160" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="162" t="s">
+      <c r="G2" s="160" t="s">
         <v>100</v>
       </c>
-      <c r="H2" s="162" t="s">
+      <c r="H2" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="163" t="s">
+      <c r="I2" s="161" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="163"/>
-      <c r="K2" s="164"/>
+      <c r="J2" s="161"/>
+      <c r="K2" s="162"/>
       <c r="L2" s="107"/>
     </row>
     <row r="3" spans="1:12" ht="100.8">
@@ -12991,25 +12997,25 @@
       <c r="C3" s="68" t="s">
         <v>344</v>
       </c>
-      <c r="D3" s="165" t="s">
+      <c r="D3" s="163" t="s">
         <v>25</v>
       </c>
       <c r="E3" s="61" t="s">
         <v>345</v>
       </c>
-      <c r="F3" s="166" t="s">
+      <c r="F3" s="164" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="166" t="s">
+      <c r="G3" s="164" t="s">
         <v>346</v>
       </c>
-      <c r="H3" s="166">
+      <c r="H3" s="164">
         <v>1</v>
       </c>
-      <c r="I3" s="167" t="s">
+      <c r="I3" s="165" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="163" t="s">
+      <c r="J3" s="161" t="s">
         <v>30</v>
       </c>
       <c r="K3" s="137" t="s">
@@ -13021,7 +13027,7 @@
       <c r="A4" s="64" t="s">
         <v>116</v>
       </c>
-      <c r="B4" s="160" t="s">
+      <c r="B4" s="158" t="s">
         <v>117</v>
       </c>
       <c r="C4" s="64" t="s">
@@ -13030,22 +13036,22 @@
       <c r="D4" s="71" t="s">
         <v>348</v>
       </c>
-      <c r="E4" s="161" t="s">
+      <c r="E4" s="159" t="s">
         <v>349</v>
       </c>
-      <c r="F4" s="162" t="s">
+      <c r="F4" s="160" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="162" t="s">
+      <c r="G4" s="160" t="s">
         <v>75</v>
       </c>
-      <c r="H4" s="162" t="s">
+      <c r="H4" s="160" t="s">
         <v>37</v>
       </c>
-      <c r="I4" s="163" t="s">
+      <c r="I4" s="161" t="s">
         <v>69</v>
       </c>
-      <c r="J4" s="163" t="s">
+      <c r="J4" s="161" t="s">
         <v>350</v>
       </c>
       <c r="K4" s="137" t="s">
@@ -13054,13 +13060,13 @@
       <c r="L4" s="107"/>
     </row>
     <row r="5" spans="1:12" ht="43.2">
-      <c r="A5" s="168" t="s">
+      <c r="A5" s="166" t="s">
         <v>352</v>
       </c>
       <c r="B5" s="75" t="s">
         <v>353</v>
       </c>
-      <c r="C5" s="168" t="s">
+      <c r="C5" s="166" t="s">
         <v>354</v>
       </c>
       <c r="D5" s="127" t="s">
@@ -13069,19 +13075,19 @@
       <c r="E5" s="75" t="s">
         <v>355</v>
       </c>
-      <c r="F5" s="169" t="s">
+      <c r="F5" s="167" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="169" t="s">
+      <c r="G5" s="167" t="s">
         <v>75</v>
       </c>
-      <c r="H5" s="169" t="s">
+      <c r="H5" s="167" t="s">
         <v>37</v>
       </c>
-      <c r="I5" s="170" t="s">
+      <c r="I5" s="168" t="s">
         <v>69</v>
       </c>
-      <c r="J5" s="163" t="s">
+      <c r="J5" s="161" t="s">
         <v>76</v>
       </c>
       <c r="K5" s="137" t="s">
@@ -13090,19 +13096,19 @@
       <c r="L5" s="130"/>
     </row>
     <row r="6" spans="1:12" ht="72">
-      <c r="A6" s="171" t="s">
+      <c r="A6" s="169" t="s">
         <v>357</v>
       </c>
-      <c r="B6" s="153" t="s">
+      <c r="B6" s="152" t="s">
         <v>358</v>
       </c>
-      <c r="C6" s="171" t="s">
+      <c r="C6" s="169" t="s">
         <v>359</v>
       </c>
-      <c r="D6" s="172" t="s">
+      <c r="D6" s="170" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="153" t="s">
+      <c r="E6" s="152" t="s">
         <v>360</v>
       </c>
       <c r="F6" s="134" t="s">
@@ -13114,13 +13120,13 @@
       <c r="H6" s="134" t="s">
         <v>93</v>
       </c>
-      <c r="I6" s="146" t="s">
+      <c r="I6" s="145" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="173" t="s">
+      <c r="J6" s="171" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="164"/>
+      <c r="K6" s="162"/>
       <c r="L6" s="107"/>
     </row>
     <row r="7" spans="1:12" ht="115.2">
@@ -13133,7 +13139,7 @@
       <c r="C7" s="126" t="s">
         <v>363</v>
       </c>
-      <c r="D7" s="174" t="s">
+      <c r="D7" s="172" t="s">
         <v>364</v>
       </c>
       <c r="E7" s="81" t="s">
@@ -13151,41 +13157,41 @@
       <c r="I7" s="130" t="s">
         <v>19</v>
       </c>
-      <c r="J7" s="173" t="s">
+      <c r="J7" s="171" t="s">
         <v>30</v>
       </c>
-      <c r="K7" s="164"/>
+      <c r="K7" s="162"/>
       <c r="L7" s="130"/>
     </row>
     <row r="8" spans="1:12" ht="28.8">
       <c r="A8" s="64" t="s">
         <v>273</v>
       </c>
-      <c r="B8" s="160" t="s">
+      <c r="B8" s="158" t="s">
         <v>274</v>
       </c>
-      <c r="C8" s="175" t="s">
+      <c r="C8" s="173" t="s">
         <v>275</v>
       </c>
-      <c r="D8" s="145" t="s">
+      <c r="D8" s="144" t="s">
         <v>364</v>
       </c>
       <c r="E8" s="136" t="s">
         <v>366</v>
       </c>
-      <c r="F8" s="162" t="s">
+      <c r="F8" s="160" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="162" t="s">
+      <c r="G8" s="160" t="s">
         <v>43</v>
       </c>
-      <c r="H8" s="162" t="s">
+      <c r="H8" s="160" t="s">
         <v>93</v>
       </c>
-      <c r="I8" s="163" t="s">
+      <c r="I8" s="161" t="s">
         <v>19</v>
       </c>
-      <c r="J8" s="163" t="s">
+      <c r="J8" s="161" t="s">
         <v>76</v>
       </c>
       <c r="K8" s="137" t="s">
@@ -13194,34 +13200,34 @@
       <c r="L8" s="107"/>
     </row>
     <row r="9" spans="1:12" ht="43.2">
-      <c r="A9" s="168" t="s">
+      <c r="A9" s="166" t="s">
         <v>368</v>
       </c>
       <c r="B9" s="75" t="s">
         <v>313</v>
       </c>
-      <c r="C9" s="168" t="s">
+      <c r="C9" s="166" t="s">
         <v>314</v>
       </c>
-      <c r="D9" s="176" t="s">
+      <c r="D9" s="174" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="176" t="s">
+      <c r="E9" s="174" t="s">
         <v>369</v>
       </c>
-      <c r="F9" s="169" t="s">
+      <c r="F9" s="167" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="169" t="s">
+      <c r="G9" s="167" t="s">
         <v>130</v>
       </c>
-      <c r="H9" s="169">
+      <c r="H9" s="167">
         <v>1</v>
       </c>
-      <c r="I9" s="170" t="s">
+      <c r="I9" s="168" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="163" t="s">
+      <c r="J9" s="161" t="s">
         <v>30</v>
       </c>
       <c r="K9" s="137" t="s">
@@ -13230,594 +13236,594 @@
       <c r="L9" s="130"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="177"/>
-      <c r="B10" s="178"/>
-      <c r="C10" s="177"/>
-      <c r="D10" s="179"/>
+      <c r="A10" s="175"/>
+      <c r="B10" s="176"/>
+      <c r="C10" s="175"/>
+      <c r="D10" s="177"/>
       <c r="E10" s="10"/>
-      <c r="F10" s="180"/>
-      <c r="G10" s="180"/>
-      <c r="H10" s="180"/>
-      <c r="I10" s="159"/>
-      <c r="J10" s="159"/>
+      <c r="F10" s="178"/>
+      <c r="G10" s="178"/>
+      <c r="H10" s="178"/>
+      <c r="I10" s="157"/>
+      <c r="J10" s="157"/>
       <c r="K10" s="98"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="177"/>
-      <c r="B11" s="178"/>
-      <c r="D11" s="179"/>
-      <c r="E11" s="179"/>
-      <c r="F11" s="180"/>
-      <c r="G11" s="180"/>
-      <c r="H11" s="180"/>
-      <c r="I11" s="159"/>
-      <c r="J11" s="159"/>
+      <c r="A11" s="175"/>
+      <c r="B11" s="176"/>
+      <c r="D11" s="177"/>
+      <c r="E11" s="177"/>
+      <c r="F11" s="178"/>
+      <c r="G11" s="178"/>
+      <c r="H11" s="178"/>
+      <c r="I11" s="157"/>
+      <c r="J11" s="157"/>
       <c r="K11" s="99"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="177"/>
-      <c r="B12" s="178"/>
-      <c r="C12" s="177"/>
-      <c r="D12" s="179"/>
-      <c r="E12" s="179"/>
-      <c r="F12" s="180"/>
-      <c r="G12" s="180"/>
-      <c r="H12" s="180"/>
-      <c r="I12" s="159"/>
-      <c r="J12" s="159"/>
+      <c r="A12" s="175"/>
+      <c r="B12" s="176"/>
+      <c r="C12" s="175"/>
+      <c r="D12" s="177"/>
+      <c r="E12" s="177"/>
+      <c r="F12" s="178"/>
+      <c r="G12" s="178"/>
+      <c r="H12" s="178"/>
+      <c r="I12" s="157"/>
+      <c r="J12" s="157"/>
       <c r="K12" s="98"/>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="177"/>
-      <c r="B13" s="178"/>
-      <c r="C13" s="177"/>
-      <c r="D13" s="179"/>
-      <c r="E13" s="178"/>
-      <c r="F13" s="180"/>
-      <c r="G13" s="180"/>
-      <c r="H13" s="180"/>
-      <c r="I13" s="159"/>
-      <c r="J13" s="159"/>
+      <c r="A13" s="175"/>
+      <c r="B13" s="176"/>
+      <c r="C13" s="175"/>
+      <c r="D13" s="177"/>
+      <c r="E13" s="176"/>
+      <c r="F13" s="178"/>
+      <c r="G13" s="178"/>
+      <c r="H13" s="178"/>
+      <c r="I13" s="157"/>
+      <c r="J13" s="157"/>
       <c r="K13" s="98"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="177"/>
-      <c r="B14" s="178"/>
-      <c r="C14" s="177"/>
-      <c r="D14" s="179"/>
-      <c r="E14" s="179"/>
-      <c r="F14" s="180"/>
-      <c r="G14" s="180"/>
-      <c r="H14" s="180"/>
-      <c r="I14" s="159"/>
-      <c r="J14" s="159"/>
+      <c r="A14" s="175"/>
+      <c r="B14" s="176"/>
+      <c r="C14" s="175"/>
+      <c r="D14" s="177"/>
+      <c r="E14" s="177"/>
+      <c r="F14" s="178"/>
+      <c r="G14" s="178"/>
+      <c r="H14" s="178"/>
+      <c r="I14" s="157"/>
+      <c r="J14" s="157"/>
       <c r="K14" s="98"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="177"/>
-      <c r="B15" s="178"/>
-      <c r="C15" s="182"/>
-      <c r="D15" s="179"/>
-      <c r="E15" s="183"/>
-      <c r="F15" s="180"/>
-      <c r="G15" s="180"/>
-      <c r="H15" s="180"/>
-      <c r="I15" s="159"/>
-      <c r="J15" s="159"/>
+      <c r="A15" s="175"/>
+      <c r="B15" s="176"/>
+      <c r="C15" s="180"/>
+      <c r="D15" s="177"/>
+      <c r="E15" s="181"/>
+      <c r="F15" s="178"/>
+      <c r="G15" s="178"/>
+      <c r="H15" s="178"/>
+      <c r="I15" s="157"/>
+      <c r="J15" s="157"/>
       <c r="K15" s="98"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="177"/>
-      <c r="B16" s="178"/>
-      <c r="C16" s="177"/>
-      <c r="D16" s="179"/>
+      <c r="A16" s="175"/>
+      <c r="B16" s="176"/>
+      <c r="C16" s="175"/>
+      <c r="D16" s="177"/>
       <c r="E16" s="10"/>
-      <c r="F16" s="180"/>
-      <c r="G16" s="180"/>
-      <c r="H16" s="180"/>
-      <c r="I16" s="159"/>
-      <c r="J16" s="159"/>
+      <c r="F16" s="178"/>
+      <c r="G16" s="178"/>
+      <c r="H16" s="178"/>
+      <c r="I16" s="157"/>
+      <c r="J16" s="157"/>
       <c r="K16" s="98"/>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="177"/>
-      <c r="B17" s="178"/>
-      <c r="D17" s="179"/>
-      <c r="E17" s="179"/>
-      <c r="F17" s="180"/>
-      <c r="G17" s="180"/>
-      <c r="H17" s="180"/>
-      <c r="I17" s="159"/>
-      <c r="J17" s="159"/>
+      <c r="A17" s="175"/>
+      <c r="B17" s="176"/>
+      <c r="D17" s="177"/>
+      <c r="E17" s="177"/>
+      <c r="F17" s="178"/>
+      <c r="G17" s="178"/>
+      <c r="H17" s="178"/>
+      <c r="I17" s="157"/>
+      <c r="J17" s="157"/>
       <c r="K17" s="98"/>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="177"/>
-      <c r="B18" s="178"/>
-      <c r="C18" s="177"/>
+      <c r="A18" s="175"/>
+      <c r="B18" s="176"/>
+      <c r="C18" s="175"/>
       <c r="D18" s="123"/>
-      <c r="E18" s="179"/>
-      <c r="F18" s="180"/>
-      <c r="G18" s="180"/>
-      <c r="H18" s="180"/>
-      <c r="I18" s="159"/>
-      <c r="J18" s="159"/>
+      <c r="E18" s="177"/>
+      <c r="F18" s="178"/>
+      <c r="G18" s="178"/>
+      <c r="H18" s="178"/>
+      <c r="I18" s="157"/>
+      <c r="J18" s="157"/>
       <c r="K18" s="98"/>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="177"/>
-      <c r="B19" s="178"/>
-      <c r="C19" s="177"/>
-      <c r="D19" s="179"/>
-      <c r="E19" s="178"/>
-      <c r="F19" s="180"/>
-      <c r="G19" s="180"/>
-      <c r="H19" s="180"/>
-      <c r="I19" s="159"/>
-      <c r="J19" s="159"/>
+      <c r="A19" s="175"/>
+      <c r="B19" s="176"/>
+      <c r="C19" s="175"/>
+      <c r="D19" s="177"/>
+      <c r="E19" s="176"/>
+      <c r="F19" s="178"/>
+      <c r="G19" s="178"/>
+      <c r="H19" s="178"/>
+      <c r="I19" s="157"/>
+      <c r="J19" s="157"/>
       <c r="K19" s="101"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="177"/>
-      <c r="B20" s="178"/>
-      <c r="C20" s="177"/>
-      <c r="D20" s="179"/>
-      <c r="E20" s="179"/>
-      <c r="F20" s="180"/>
-      <c r="G20" s="180"/>
-      <c r="H20" s="180"/>
-      <c r="I20" s="159"/>
-      <c r="J20" s="159"/>
+      <c r="A20" s="175"/>
+      <c r="B20" s="176"/>
+      <c r="C20" s="175"/>
+      <c r="D20" s="177"/>
+      <c r="E20" s="177"/>
+      <c r="F20" s="178"/>
+      <c r="G20" s="178"/>
+      <c r="H20" s="178"/>
+      <c r="I20" s="157"/>
+      <c r="J20" s="157"/>
       <c r="K20" s="99"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="177"/>
-      <c r="B21" s="178"/>
-      <c r="C21" s="182"/>
-      <c r="D21" s="179"/>
-      <c r="E21" s="183"/>
-      <c r="F21" s="180"/>
-      <c r="G21" s="180"/>
-      <c r="H21" s="180"/>
-      <c r="I21" s="159"/>
-      <c r="J21" s="159"/>
+      <c r="A21" s="175"/>
+      <c r="B21" s="176"/>
+      <c r="C21" s="180"/>
+      <c r="D21" s="177"/>
+      <c r="E21" s="181"/>
+      <c r="F21" s="178"/>
+      <c r="G21" s="178"/>
+      <c r="H21" s="178"/>
+      <c r="I21" s="157"/>
+      <c r="J21" s="157"/>
       <c r="K21" s="98"/>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="177"/>
-      <c r="B22" s="178"/>
-      <c r="C22" s="177"/>
-      <c r="D22" s="179"/>
+      <c r="A22" s="175"/>
+      <c r="B22" s="176"/>
+      <c r="C22" s="175"/>
+      <c r="D22" s="177"/>
       <c r="E22" s="10"/>
-      <c r="F22" s="180"/>
-      <c r="G22" s="180"/>
-      <c r="H22" s="180"/>
-      <c r="I22" s="159"/>
-      <c r="J22" s="159"/>
+      <c r="F22" s="178"/>
+      <c r="G22" s="178"/>
+      <c r="H22" s="178"/>
+      <c r="I22" s="157"/>
+      <c r="J22" s="157"/>
       <c r="K22" s="98"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="177"/>
-      <c r="B23" s="178"/>
+      <c r="A23" s="175"/>
+      <c r="B23" s="176"/>
       <c r="D23" s="123"/>
-      <c r="E23" s="179"/>
-      <c r="F23" s="180"/>
-      <c r="G23" s="180"/>
-      <c r="H23" s="180"/>
-      <c r="I23" s="159"/>
-      <c r="J23" s="159"/>
+      <c r="E23" s="177"/>
+      <c r="F23" s="178"/>
+      <c r="G23" s="178"/>
+      <c r="H23" s="178"/>
+      <c r="I23" s="157"/>
+      <c r="J23" s="157"/>
       <c r="K23" s="98"/>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="177"/>
-      <c r="B24" s="178"/>
-      <c r="C24" s="177"/>
-      <c r="D24" s="179"/>
-      <c r="E24" s="179"/>
-      <c r="F24" s="180"/>
-      <c r="G24" s="180"/>
-      <c r="H24" s="180"/>
-      <c r="I24" s="159"/>
-      <c r="J24" s="159"/>
+      <c r="A24" s="175"/>
+      <c r="B24" s="176"/>
+      <c r="C24" s="175"/>
+      <c r="D24" s="177"/>
+      <c r="E24" s="177"/>
+      <c r="F24" s="178"/>
+      <c r="G24" s="178"/>
+      <c r="H24" s="178"/>
+      <c r="I24" s="157"/>
+      <c r="J24" s="157"/>
       <c r="K24" s="100"/>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="177"/>
-      <c r="B25" s="178"/>
-      <c r="C25" s="177"/>
-      <c r="D25" s="179"/>
-      <c r="E25" s="178"/>
-      <c r="F25" s="180"/>
-      <c r="G25" s="180"/>
-      <c r="H25" s="180"/>
-      <c r="I25" s="159"/>
-      <c r="J25" s="159"/>
+      <c r="A25" s="175"/>
+      <c r="B25" s="176"/>
+      <c r="C25" s="175"/>
+      <c r="D25" s="177"/>
+      <c r="E25" s="176"/>
+      <c r="F25" s="178"/>
+      <c r="G25" s="178"/>
+      <c r="H25" s="178"/>
+      <c r="I25" s="157"/>
+      <c r="J25" s="157"/>
       <c r="K25" s="98"/>
     </row>
     <row r="26" spans="1:11">
-      <c r="A26" s="177"/>
-      <c r="B26" s="178"/>
-      <c r="C26" s="177"/>
-      <c r="D26" s="179"/>
-      <c r="E26" s="179"/>
-      <c r="F26" s="180"/>
-      <c r="G26" s="180"/>
-      <c r="H26" s="180"/>
-      <c r="I26" s="159"/>
-      <c r="J26" s="159"/>
+      <c r="A26" s="175"/>
+      <c r="B26" s="176"/>
+      <c r="C26" s="175"/>
+      <c r="D26" s="177"/>
+      <c r="E26" s="177"/>
+      <c r="F26" s="178"/>
+      <c r="G26" s="178"/>
+      <c r="H26" s="178"/>
+      <c r="I26" s="157"/>
+      <c r="J26" s="157"/>
       <c r="K26" s="100"/>
     </row>
     <row r="27" spans="1:11">
-      <c r="A27" s="177"/>
-      <c r="B27" s="178"/>
-      <c r="C27" s="182"/>
-      <c r="D27" s="179"/>
-      <c r="E27" s="183"/>
-      <c r="F27" s="180"/>
-      <c r="G27" s="180"/>
-      <c r="H27" s="180"/>
-      <c r="I27" s="159"/>
-      <c r="J27" s="159"/>
+      <c r="A27" s="175"/>
+      <c r="B27" s="176"/>
+      <c r="C27" s="180"/>
+      <c r="D27" s="177"/>
+      <c r="E27" s="181"/>
+      <c r="F27" s="178"/>
+      <c r="G27" s="178"/>
+      <c r="H27" s="178"/>
+      <c r="I27" s="157"/>
+      <c r="J27" s="157"/>
       <c r="K27" s="98"/>
     </row>
     <row r="28" spans="1:11">
-      <c r="A28" s="177"/>
-      <c r="B28" s="178"/>
-      <c r="C28" s="177"/>
-      <c r="D28" s="179"/>
+      <c r="A28" s="175"/>
+      <c r="B28" s="176"/>
+      <c r="C28" s="175"/>
+      <c r="D28" s="177"/>
       <c r="E28" s="10"/>
-      <c r="F28" s="180"/>
-      <c r="G28" s="180"/>
-      <c r="H28" s="180"/>
-      <c r="I28" s="159"/>
-      <c r="J28" s="159"/>
+      <c r="F28" s="178"/>
+      <c r="G28" s="178"/>
+      <c r="H28" s="178"/>
+      <c r="I28" s="157"/>
+      <c r="J28" s="157"/>
       <c r="K28" s="98"/>
     </row>
     <row r="29" spans="1:11">
-      <c r="A29" s="177"/>
-      <c r="B29" s="178"/>
-      <c r="D29" s="179"/>
-      <c r="E29" s="179"/>
-      <c r="F29" s="180"/>
-      <c r="G29" s="180"/>
-      <c r="H29" s="180"/>
-      <c r="I29" s="159"/>
-      <c r="J29" s="159"/>
+      <c r="A29" s="175"/>
+      <c r="B29" s="176"/>
+      <c r="D29" s="177"/>
+      <c r="E29" s="177"/>
+      <c r="F29" s="178"/>
+      <c r="G29" s="178"/>
+      <c r="H29" s="178"/>
+      <c r="I29" s="157"/>
+      <c r="J29" s="157"/>
       <c r="K29" s="98"/>
     </row>
     <row r="30" spans="1:11">
-      <c r="A30" s="177"/>
-      <c r="B30" s="178"/>
-      <c r="C30" s="177"/>
-      <c r="D30" s="179"/>
-      <c r="E30" s="179"/>
-      <c r="F30" s="180"/>
-      <c r="G30" s="180"/>
-      <c r="H30" s="180"/>
-      <c r="I30" s="159"/>
-      <c r="J30" s="159"/>
+      <c r="A30" s="175"/>
+      <c r="B30" s="176"/>
+      <c r="C30" s="175"/>
+      <c r="D30" s="177"/>
+      <c r="E30" s="177"/>
+      <c r="F30" s="178"/>
+      <c r="G30" s="178"/>
+      <c r="H30" s="178"/>
+      <c r="I30" s="157"/>
+      <c r="J30" s="157"/>
       <c r="K30" s="98"/>
     </row>
     <row r="31" spans="1:11">
-      <c r="A31" s="177"/>
-      <c r="B31" s="178"/>
-      <c r="C31" s="177"/>
-      <c r="D31" s="179"/>
-      <c r="E31" s="178"/>
-      <c r="F31" s="180"/>
-      <c r="G31" s="180"/>
-      <c r="H31" s="180"/>
-      <c r="I31" s="159"/>
-      <c r="J31" s="159"/>
+      <c r="A31" s="175"/>
+      <c r="B31" s="176"/>
+      <c r="C31" s="175"/>
+      <c r="D31" s="177"/>
+      <c r="E31" s="176"/>
+      <c r="F31" s="178"/>
+      <c r="G31" s="178"/>
+      <c r="H31" s="178"/>
+      <c r="I31" s="157"/>
+      <c r="J31" s="157"/>
       <c r="K31" s="98"/>
     </row>
     <row r="32" spans="1:11">
-      <c r="A32" s="177"/>
-      <c r="B32" s="178"/>
-      <c r="C32" s="177"/>
+      <c r="A32" s="175"/>
+      <c r="B32" s="176"/>
+      <c r="C32" s="175"/>
       <c r="D32" s="123"/>
-      <c r="E32" s="179"/>
-      <c r="F32" s="180"/>
-      <c r="G32" s="180"/>
-      <c r="H32" s="180"/>
-      <c r="I32" s="159"/>
-      <c r="J32" s="159"/>
+      <c r="E32" s="177"/>
+      <c r="F32" s="178"/>
+      <c r="G32" s="178"/>
+      <c r="H32" s="178"/>
+      <c r="I32" s="157"/>
+      <c r="J32" s="157"/>
       <c r="K32" s="98"/>
     </row>
     <row r="33" spans="1:11">
-      <c r="A33" s="177"/>
-      <c r="B33" s="178"/>
-      <c r="C33" s="182"/>
-      <c r="D33" s="179"/>
-      <c r="E33" s="183"/>
-      <c r="F33" s="180"/>
-      <c r="G33" s="180"/>
-      <c r="H33" s="180"/>
-      <c r="I33" s="159"/>
-      <c r="J33" s="159"/>
+      <c r="A33" s="175"/>
+      <c r="B33" s="176"/>
+      <c r="C33" s="180"/>
+      <c r="D33" s="177"/>
+      <c r="E33" s="181"/>
+      <c r="F33" s="178"/>
+      <c r="G33" s="178"/>
+      <c r="H33" s="178"/>
+      <c r="I33" s="157"/>
+      <c r="J33" s="157"/>
       <c r="K33" s="98"/>
     </row>
     <row r="34" spans="1:11">
-      <c r="A34" s="177"/>
-      <c r="B34" s="178"/>
-      <c r="C34" s="177"/>
-      <c r="D34" s="179"/>
+      <c r="A34" s="175"/>
+      <c r="B34" s="176"/>
+      <c r="C34" s="175"/>
+      <c r="D34" s="177"/>
       <c r="E34" s="10"/>
-      <c r="F34" s="180"/>
-      <c r="G34" s="180"/>
-      <c r="H34" s="180"/>
-      <c r="I34" s="159"/>
-      <c r="J34" s="159"/>
+      <c r="F34" s="178"/>
+      <c r="G34" s="178"/>
+      <c r="H34" s="178"/>
+      <c r="I34" s="157"/>
+      <c r="J34" s="157"/>
       <c r="K34" s="98"/>
     </row>
     <row r="35" spans="1:11">
-      <c r="A35" s="177"/>
-      <c r="B35" s="178"/>
-      <c r="D35" s="179"/>
-      <c r="E35" s="179"/>
-      <c r="F35" s="180"/>
-      <c r="G35" s="180"/>
-      <c r="H35" s="180"/>
-      <c r="I35" s="159"/>
-      <c r="J35" s="159"/>
+      <c r="A35" s="175"/>
+      <c r="B35" s="176"/>
+      <c r="D35" s="177"/>
+      <c r="E35" s="177"/>
+      <c r="F35" s="178"/>
+      <c r="G35" s="178"/>
+      <c r="H35" s="178"/>
+      <c r="I35" s="157"/>
+      <c r="J35" s="157"/>
       <c r="K35" s="98"/>
     </row>
     <row r="36" spans="1:11">
-      <c r="A36" s="177"/>
-      <c r="B36" s="178"/>
-      <c r="C36" s="177"/>
-      <c r="D36" s="179"/>
-      <c r="E36" s="179"/>
-      <c r="F36" s="180"/>
-      <c r="G36" s="180"/>
-      <c r="H36" s="180"/>
-      <c r="I36" s="159"/>
-      <c r="J36" s="159"/>
+      <c r="A36" s="175"/>
+      <c r="B36" s="176"/>
+      <c r="C36" s="175"/>
+      <c r="D36" s="177"/>
+      <c r="E36" s="177"/>
+      <c r="F36" s="178"/>
+      <c r="G36" s="178"/>
+      <c r="H36" s="178"/>
+      <c r="I36" s="157"/>
+      <c r="J36" s="157"/>
       <c r="K36" s="98"/>
     </row>
     <row r="37" spans="1:11">
-      <c r="A37" s="177"/>
-      <c r="B37" s="178"/>
-      <c r="C37" s="177"/>
-      <c r="D37" s="179"/>
-      <c r="E37" s="178"/>
-      <c r="F37" s="180"/>
-      <c r="G37" s="180"/>
-      <c r="H37" s="180"/>
-      <c r="I37" s="159"/>
-      <c r="J37" s="159"/>
+      <c r="A37" s="175"/>
+      <c r="B37" s="176"/>
+      <c r="C37" s="175"/>
+      <c r="D37" s="177"/>
+      <c r="E37" s="176"/>
+      <c r="F37" s="178"/>
+      <c r="G37" s="178"/>
+      <c r="H37" s="178"/>
+      <c r="I37" s="157"/>
+      <c r="J37" s="157"/>
       <c r="K37" s="98"/>
     </row>
     <row r="38" spans="1:11">
-      <c r="A38" s="177"/>
-      <c r="B38" s="178"/>
-      <c r="C38" s="177"/>
-      <c r="D38" s="179"/>
-      <c r="E38" s="179"/>
-      <c r="F38" s="180"/>
-      <c r="G38" s="180"/>
-      <c r="H38" s="180"/>
-      <c r="I38" s="159"/>
-      <c r="J38" s="159"/>
+      <c r="A38" s="175"/>
+      <c r="B38" s="176"/>
+      <c r="C38" s="175"/>
+      <c r="D38" s="177"/>
+      <c r="E38" s="177"/>
+      <c r="F38" s="178"/>
+      <c r="G38" s="178"/>
+      <c r="H38" s="178"/>
+      <c r="I38" s="157"/>
+      <c r="J38" s="157"/>
       <c r="K38" s="98"/>
     </row>
     <row r="39" spans="1:11">
-      <c r="A39" s="177"/>
-      <c r="B39" s="178"/>
-      <c r="C39" s="182"/>
+      <c r="A39" s="175"/>
+      <c r="B39" s="176"/>
+      <c r="C39" s="180"/>
       <c r="D39" s="123"/>
-      <c r="E39" s="183"/>
-      <c r="F39" s="180"/>
-      <c r="G39" s="180"/>
-      <c r="H39" s="180"/>
-      <c r="I39" s="159"/>
-      <c r="J39" s="159"/>
+      <c r="E39" s="181"/>
+      <c r="F39" s="178"/>
+      <c r="G39" s="178"/>
+      <c r="H39" s="178"/>
+      <c r="I39" s="157"/>
+      <c r="J39" s="157"/>
       <c r="K39" s="98"/>
     </row>
     <row r="40" spans="1:11">
-      <c r="A40" s="177"/>
-      <c r="B40" s="178"/>
-      <c r="C40" s="177"/>
-      <c r="D40" s="179"/>
-      <c r="E40" s="179"/>
-      <c r="F40" s="180"/>
-      <c r="G40" s="180"/>
-      <c r="H40" s="180"/>
-      <c r="I40" s="159"/>
-      <c r="J40" s="159"/>
+      <c r="A40" s="175"/>
+      <c r="B40" s="176"/>
+      <c r="C40" s="175"/>
+      <c r="D40" s="177"/>
+      <c r="E40" s="177"/>
+      <c r="F40" s="178"/>
+      <c r="G40" s="178"/>
+      <c r="H40" s="178"/>
+      <c r="I40" s="157"/>
+      <c r="J40" s="157"/>
       <c r="K40" s="98"/>
     </row>
     <row r="41" spans="1:11">
-      <c r="A41" s="177"/>
-      <c r="B41" s="178"/>
-      <c r="C41" s="177"/>
-      <c r="D41" s="179"/>
-      <c r="E41" s="178"/>
-      <c r="F41" s="180"/>
-      <c r="G41" s="180"/>
-      <c r="H41" s="180"/>
-      <c r="I41" s="159"/>
-      <c r="J41" s="159"/>
+      <c r="A41" s="175"/>
+      <c r="B41" s="176"/>
+      <c r="C41" s="175"/>
+      <c r="D41" s="177"/>
+      <c r="E41" s="176"/>
+      <c r="F41" s="178"/>
+      <c r="G41" s="178"/>
+      <c r="H41" s="178"/>
+      <c r="I41" s="157"/>
+      <c r="J41" s="157"/>
       <c r="K41" s="98"/>
     </row>
     <row r="42" spans="1:11">
-      <c r="A42" s="177"/>
-      <c r="B42" s="178"/>
-      <c r="C42" s="177"/>
-      <c r="D42" s="179"/>
-      <c r="E42" s="179"/>
-      <c r="F42" s="180"/>
-      <c r="G42" s="180"/>
-      <c r="H42" s="180"/>
-      <c r="I42" s="159"/>
-      <c r="J42" s="159"/>
+      <c r="A42" s="175"/>
+      <c r="B42" s="176"/>
+      <c r="C42" s="175"/>
+      <c r="D42" s="177"/>
+      <c r="E42" s="177"/>
+      <c r="F42" s="178"/>
+      <c r="G42" s="178"/>
+      <c r="H42" s="178"/>
+      <c r="I42" s="157"/>
+      <c r="J42" s="157"/>
       <c r="K42" s="98"/>
     </row>
     <row r="43" spans="1:11">
-      <c r="A43" s="177"/>
-      <c r="B43" s="178"/>
-      <c r="C43" s="182"/>
+      <c r="A43" s="175"/>
+      <c r="B43" s="176"/>
+      <c r="C43" s="180"/>
       <c r="D43" s="123"/>
-      <c r="E43" s="183"/>
-      <c r="F43" s="180"/>
-      <c r="G43" s="180"/>
-      <c r="H43" s="180"/>
-      <c r="I43" s="159"/>
-      <c r="J43" s="159"/>
+      <c r="E43" s="181"/>
+      <c r="F43" s="178"/>
+      <c r="G43" s="178"/>
+      <c r="H43" s="178"/>
+      <c r="I43" s="157"/>
+      <c r="J43" s="157"/>
       <c r="K43" s="98"/>
     </row>
     <row r="44" spans="1:11">
-      <c r="A44" s="177"/>
-      <c r="B44" s="178"/>
-      <c r="C44" s="177"/>
-      <c r="D44" s="179"/>
+      <c r="A44" s="175"/>
+      <c r="B44" s="176"/>
+      <c r="C44" s="175"/>
+      <c r="D44" s="177"/>
       <c r="E44" s="10"/>
-      <c r="F44" s="180"/>
-      <c r="G44" s="180"/>
-      <c r="H44" s="180"/>
-      <c r="I44" s="159"/>
-      <c r="J44" s="159"/>
+      <c r="F44" s="178"/>
+      <c r="G44" s="178"/>
+      <c r="H44" s="178"/>
+      <c r="I44" s="157"/>
+      <c r="J44" s="157"/>
       <c r="K44" s="98"/>
     </row>
     <row r="45" spans="1:11">
-      <c r="A45" s="177"/>
-      <c r="B45" s="178"/>
-      <c r="D45" s="179"/>
-      <c r="E45" s="179"/>
-      <c r="F45" s="180"/>
-      <c r="G45" s="180"/>
-      <c r="H45" s="180"/>
-      <c r="I45" s="159"/>
-      <c r="J45" s="159"/>
+      <c r="A45" s="175"/>
+      <c r="B45" s="176"/>
+      <c r="D45" s="177"/>
+      <c r="E45" s="177"/>
+      <c r="F45" s="178"/>
+      <c r="G45" s="178"/>
+      <c r="H45" s="178"/>
+      <c r="I45" s="157"/>
+      <c r="J45" s="157"/>
       <c r="K45" s="98"/>
     </row>
     <row r="46" spans="1:11">
-      <c r="A46" s="177"/>
-      <c r="B46" s="178"/>
-      <c r="C46" s="177"/>
-      <c r="D46" s="179"/>
-      <c r="E46" s="179"/>
-      <c r="F46" s="180"/>
-      <c r="G46" s="180"/>
-      <c r="H46" s="180"/>
-      <c r="I46" s="159"/>
-      <c r="J46" s="159"/>
+      <c r="A46" s="175"/>
+      <c r="B46" s="176"/>
+      <c r="C46" s="175"/>
+      <c r="D46" s="177"/>
+      <c r="E46" s="177"/>
+      <c r="F46" s="178"/>
+      <c r="G46" s="178"/>
+      <c r="H46" s="178"/>
+      <c r="I46" s="157"/>
+      <c r="J46" s="157"/>
       <c r="K46" s="98"/>
     </row>
     <row r="47" spans="1:11">
-      <c r="A47" s="177"/>
-      <c r="B47" s="178"/>
-      <c r="C47" s="177"/>
-      <c r="D47" s="179"/>
-      <c r="E47" s="178"/>
-      <c r="F47" s="180"/>
-      <c r="G47" s="180"/>
-      <c r="H47" s="180"/>
-      <c r="I47" s="159"/>
-      <c r="J47" s="159"/>
+      <c r="A47" s="175"/>
+      <c r="B47" s="176"/>
+      <c r="C47" s="175"/>
+      <c r="D47" s="177"/>
+      <c r="E47" s="176"/>
+      <c r="F47" s="178"/>
+      <c r="G47" s="178"/>
+      <c r="H47" s="178"/>
+      <c r="I47" s="157"/>
+      <c r="J47" s="157"/>
       <c r="K47" s="98"/>
     </row>
     <row r="48" spans="1:11">
-      <c r="A48" s="177"/>
-      <c r="B48" s="178"/>
-      <c r="C48" s="177"/>
-      <c r="D48" s="179"/>
-      <c r="E48" s="179"/>
-      <c r="F48" s="180"/>
-      <c r="G48" s="180"/>
-      <c r="H48" s="180"/>
-      <c r="I48" s="159"/>
-      <c r="J48" s="159"/>
+      <c r="A48" s="175"/>
+      <c r="B48" s="176"/>
+      <c r="C48" s="175"/>
+      <c r="D48" s="177"/>
+      <c r="E48" s="177"/>
+      <c r="F48" s="178"/>
+      <c r="G48" s="178"/>
+      <c r="H48" s="178"/>
+      <c r="I48" s="157"/>
+      <c r="J48" s="157"/>
       <c r="K48" s="98"/>
     </row>
     <row r="49" spans="1:11">
-      <c r="A49" s="177"/>
-      <c r="B49" s="178"/>
-      <c r="C49" s="182"/>
-      <c r="D49" s="179"/>
-      <c r="E49" s="183"/>
-      <c r="F49" s="180"/>
-      <c r="G49" s="180"/>
-      <c r="H49" s="180"/>
-      <c r="I49" s="159"/>
-      <c r="J49" s="159"/>
+      <c r="A49" s="175"/>
+      <c r="B49" s="176"/>
+      <c r="C49" s="180"/>
+      <c r="D49" s="177"/>
+      <c r="E49" s="181"/>
+      <c r="F49" s="178"/>
+      <c r="G49" s="178"/>
+      <c r="H49" s="178"/>
+      <c r="I49" s="157"/>
+      <c r="J49" s="157"/>
       <c r="K49" s="98"/>
     </row>
     <row r="50" spans="1:11">
-      <c r="A50" s="177"/>
-      <c r="B50" s="178"/>
-      <c r="C50" s="177"/>
-      <c r="D50" s="179"/>
-      <c r="E50" s="178"/>
-      <c r="F50" s="180"/>
-      <c r="G50" s="180"/>
-      <c r="H50" s="180"/>
-      <c r="I50" s="159"/>
-      <c r="J50" s="159"/>
+      <c r="A50" s="175"/>
+      <c r="B50" s="176"/>
+      <c r="C50" s="175"/>
+      <c r="D50" s="177"/>
+      <c r="E50" s="176"/>
+      <c r="F50" s="178"/>
+      <c r="G50" s="178"/>
+      <c r="H50" s="178"/>
+      <c r="I50" s="157"/>
+      <c r="J50" s="157"/>
       <c r="K50" s="98"/>
     </row>
     <row r="51" spans="1:11">
-      <c r="A51" s="177"/>
-      <c r="B51" s="178"/>
-      <c r="C51" s="177"/>
-      <c r="D51" s="179"/>
-      <c r="E51" s="178"/>
-      <c r="F51" s="180"/>
-      <c r="G51" s="180"/>
-      <c r="H51" s="180"/>
-      <c r="I51" s="159"/>
-      <c r="J51" s="159"/>
+      <c r="A51" s="175"/>
+      <c r="B51" s="176"/>
+      <c r="C51" s="175"/>
+      <c r="D51" s="177"/>
+      <c r="E51" s="176"/>
+      <c r="F51" s="178"/>
+      <c r="G51" s="178"/>
+      <c r="H51" s="178"/>
+      <c r="I51" s="157"/>
+      <c r="J51" s="157"/>
       <c r="K51" s="98"/>
     </row>
     <row r="52" spans="1:11">
-      <c r="A52" s="177"/>
-      <c r="B52" s="178"/>
-      <c r="C52" s="177"/>
-      <c r="D52" s="184"/>
-      <c r="E52" s="179"/>
-      <c r="F52" s="180"/>
-      <c r="G52" s="180"/>
-      <c r="H52" s="180"/>
-      <c r="I52" s="159"/>
-      <c r="J52" s="159"/>
+      <c r="A52" s="175"/>
+      <c r="B52" s="176"/>
+      <c r="C52" s="175"/>
+      <c r="D52" s="182"/>
+      <c r="E52" s="177"/>
+      <c r="F52" s="178"/>
+      <c r="G52" s="178"/>
+      <c r="H52" s="178"/>
+      <c r="I52" s="157"/>
+      <c r="J52" s="157"/>
       <c r="K52" s="98"/>
     </row>
     <row r="53" spans="1:11">
-      <c r="A53" s="177"/>
-      <c r="B53" s="178"/>
-      <c r="D53" s="179"/>
-      <c r="E53" s="179"/>
-      <c r="F53" s="180"/>
-      <c r="G53" s="180"/>
-      <c r="H53" s="180"/>
-      <c r="I53" s="159"/>
-      <c r="J53" s="159"/>
+      <c r="A53" s="175"/>
+      <c r="B53" s="176"/>
+      <c r="D53" s="177"/>
+      <c r="E53" s="177"/>
+      <c r="F53" s="178"/>
+      <c r="G53" s="178"/>
+      <c r="H53" s="178"/>
+      <c r="I53" s="157"/>
+      <c r="J53" s="157"/>
       <c r="K53" s="98"/>
     </row>
     <row r="54" spans="1:11">
-      <c r="A54" s="177"/>
-      <c r="B54" s="178"/>
-      <c r="C54" s="177"/>
-      <c r="D54" s="179"/>
-      <c r="E54" s="179"/>
-      <c r="F54" s="180"/>
-      <c r="G54" s="180"/>
-      <c r="H54" s="180"/>
-      <c r="I54" s="159"/>
-      <c r="J54" s="159"/>
+      <c r="A54" s="175"/>
+      <c r="B54" s="176"/>
+      <c r="C54" s="175"/>
+      <c r="D54" s="177"/>
+      <c r="E54" s="177"/>
+      <c r="F54" s="178"/>
+      <c r="G54" s="178"/>
+      <c r="H54" s="178"/>
+      <c r="I54" s="157"/>
+      <c r="J54" s="157"/>
       <c r="K54" s="98"/>
     </row>
     <row r="55" spans="1:11">
-      <c r="A55" s="177"/>
-      <c r="B55" s="178"/>
-      <c r="C55" s="177"/>
-      <c r="D55" s="179"/>
-      <c r="E55" s="179"/>
-      <c r="F55" s="180"/>
-      <c r="G55" s="180"/>
-      <c r="H55" s="180"/>
-      <c r="I55" s="159"/>
-      <c r="J55" s="159"/>
+      <c r="A55" s="175"/>
+      <c r="B55" s="176"/>
+      <c r="C55" s="175"/>
+      <c r="D55" s="177"/>
+      <c r="E55" s="177"/>
+      <c r="F55" s="178"/>
+      <c r="G55" s="178"/>
+      <c r="H55" s="178"/>
+      <c r="I55" s="157"/>
+      <c r="J55" s="157"/>
       <c r="K55" s="98"/>
     </row>
     <row r="56" spans="1:11">
@@ -13927,7 +13933,7 @@
     <col min="13" max="16384" width="8.88671875" style="84"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="204" customFormat="1" ht="57.6">
+    <row r="1" spans="1:12" s="202" customFormat="1" ht="57.6">
       <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
@@ -13958,7 +13964,7 @@
       <c r="J1" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="203" t="s">
+      <c r="K1" s="201" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="108" t="s">
@@ -13972,7 +13978,7 @@
       <c r="B2" s="45" t="s">
         <v>372</v>
       </c>
-      <c r="C2" s="175" t="s">
+      <c r="C2" s="173" t="s">
         <v>373</v>
       </c>
       <c r="D2" s="64" t="s">
@@ -13981,22 +13987,22 @@
       <c r="E2" s="88" t="s">
         <v>374</v>
       </c>
-      <c r="F2" s="162" t="s">
+      <c r="F2" s="160" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="162" t="s">
+      <c r="G2" s="160" t="s">
         <v>346</v>
       </c>
-      <c r="H2" s="162" t="s">
+      <c r="H2" s="160" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="163" t="s">
+      <c r="I2" s="161" t="s">
         <v>69</v>
       </c>
-      <c r="J2" s="163" t="s">
+      <c r="J2" s="161" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="159" t="s">
+      <c r="K2" s="157" t="s">
         <v>375</v>
       </c>
       <c r="L2" s="137"/>
@@ -14011,28 +14017,28 @@
       <c r="C3" s="68" t="s">
         <v>378</v>
       </c>
-      <c r="D3" s="186" t="s">
+      <c r="D3" s="184" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="187" t="s">
+      <c r="E3" s="185" t="s">
         <v>379</v>
       </c>
-      <c r="F3" s="166" t="s">
+      <c r="F3" s="164" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="166" t="s">
+      <c r="G3" s="164" t="s">
         <v>346</v>
       </c>
-      <c r="H3" s="166">
+      <c r="H3" s="164">
         <v>1</v>
       </c>
-      <c r="I3" s="167" t="s">
+      <c r="I3" s="165" t="s">
         <v>69</v>
       </c>
-      <c r="J3" s="163" t="s">
+      <c r="J3" s="161" t="s">
         <v>76</v>
       </c>
-      <c r="K3" s="159" t="s">
+      <c r="K3" s="157" t="s">
         <v>380</v>
       </c>
       <c r="L3" s="137"/>
@@ -14053,22 +14059,22 @@
       <c r="E4" s="88" t="s">
         <v>384</v>
       </c>
-      <c r="F4" s="162" t="s">
+      <c r="F4" s="160" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="162" t="s">
+      <c r="G4" s="160" t="s">
         <v>385</v>
       </c>
-      <c r="H4" s="162">
+      <c r="H4" s="160">
         <v>1</v>
       </c>
-      <c r="I4" s="163" t="s">
+      <c r="I4" s="161" t="s">
         <v>69</v>
       </c>
-      <c r="J4" s="163" t="s">
+      <c r="J4" s="161" t="s">
         <v>76</v>
       </c>
-      <c r="K4" s="159" t="s">
+      <c r="K4" s="157" t="s">
         <v>386</v>
       </c>
       <c r="L4" s="137"/>
@@ -14786,8 +14792,8 @@
   </sheetPr>
   <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
@@ -14808,7 +14814,7 @@
     <col min="13" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="204" customFormat="1" ht="57.6">
+    <row r="1" spans="1:12" s="202" customFormat="1" ht="57.6">
       <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
@@ -14839,7 +14845,7 @@
       <c r="J1" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="203" t="s">
+      <c r="K1" s="201" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="108" t="s">
@@ -15036,7 +15042,7 @@
       <c r="C7" s="135" t="s">
         <v>412</v>
       </c>
-      <c r="D7" s="188" t="s">
+      <c r="D7" s="186" t="s">
         <v>413</v>
       </c>
       <c r="E7" s="127" t="s">
@@ -15045,7 +15051,7 @@
       <c r="F7" s="128" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="159" t="s">
+      <c r="G7" s="157" t="s">
         <v>415</v>
       </c>
       <c r="H7" s="128" t="s">
@@ -15108,7 +15114,7 @@
       <c r="C9" s="126" t="s">
         <v>84</v>
       </c>
-      <c r="D9" s="190" t="s">
+      <c r="D9" s="188" t="s">
         <v>25</v>
       </c>
       <c r="E9" s="127" t="s">
@@ -15141,7 +15147,7 @@
       <c r="B10" s="35" t="s">
         <v>422</v>
       </c>
-      <c r="C10" s="143" t="s">
+      <c r="C10" s="142" t="s">
         <v>423</v>
       </c>
       <c r="D10" s="133" t="s">
@@ -15180,7 +15186,7 @@
       <c r="C11" s="126" t="s">
         <v>428</v>
       </c>
-      <c r="D11" s="157" t="s">
+      <c r="D11" s="155" t="s">
         <v>429</v>
       </c>
       <c r="E11" s="127" t="s">
@@ -15216,7 +15222,7 @@
       <c r="C12" s="122" t="s">
         <v>139</v>
       </c>
-      <c r="D12" s="191" t="s">
+      <c r="D12" s="189" t="s">
         <v>140</v>
       </c>
       <c r="E12" s="139" t="s">
@@ -15252,7 +15258,7 @@
       <c r="C13" s="126" t="s">
         <v>319</v>
       </c>
-      <c r="D13" s="144" t="s">
+      <c r="D13" s="143" t="s">
         <v>320</v>
       </c>
       <c r="E13" s="80" t="s">
@@ -15324,7 +15330,7 @@
       <c r="C15" s="126" t="s">
         <v>444</v>
       </c>
-      <c r="D15" s="188" t="s">
+      <c r="D15" s="186" t="s">
         <v>413</v>
       </c>
       <c r="E15" s="80" t="s">
@@ -15357,10 +15363,10 @@
       <c r="B16" s="35" t="s">
         <v>163</v>
       </c>
-      <c r="C16" s="143" t="s">
+      <c r="C16" s="142" t="s">
         <v>164</v>
       </c>
-      <c r="D16" s="192" t="s">
+      <c r="D16" s="190" t="s">
         <v>25</v>
       </c>
       <c r="E16" s="133"/>
@@ -15394,7 +15400,7 @@
       <c r="C17" s="126" t="s">
         <v>450</v>
       </c>
-      <c r="D17" s="188" t="s">
+      <c r="D17" s="186" t="s">
         <v>413</v>
       </c>
       <c r="E17" s="74" t="s">
@@ -15504,7 +15510,7 @@
       <c r="E20" s="79" t="s">
         <v>456</v>
       </c>
-      <c r="F20" s="193" t="s">
+      <c r="F20" s="191" t="s">
         <v>17</v>
       </c>
       <c r="G20" s="125" t="s">
@@ -15534,7 +15540,7 @@
       <c r="C21" s="126" t="s">
         <v>248</v>
       </c>
-      <c r="D21" s="157" t="s">
+      <c r="D21" s="155" t="s">
         <v>458</v>
       </c>
       <c r="E21" s="81" t="s">
@@ -16054,7 +16060,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -16074,7 +16080,7 @@
     <col min="13" max="16384" width="9.109375" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="202" customFormat="1" ht="43.2">
+    <row r="1" spans="1:12" s="200" customFormat="1" ht="43.2">
       <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
@@ -16105,7 +16111,7 @@
       <c r="J1" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="203" t="s">
+      <c r="K1" s="201" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="108" t="s">
@@ -16113,7 +16119,7 @@
       </c>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="194" t="s">
+      <c r="A2" s="192" t="s">
         <v>32</v>
       </c>
       <c r="B2" s="74" t="s">
@@ -16134,10 +16140,10 @@
       <c r="G2" s="128" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="195" t="s">
+      <c r="H2" s="193" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="195" t="s">
+      <c r="I2" s="193" t="s">
         <v>19</v>
       </c>
       <c r="J2" s="107" t="s">
@@ -16255,104 +16261,104 @@
       <c r="L5" s="107"/>
     </row>
     <row r="6" spans="1:12" ht="28.8">
-      <c r="A6" s="224" t="s">
+      <c r="A6" s="225" t="s">
         <v>95</v>
       </c>
-      <c r="B6" s="225" t="s">
+      <c r="B6" s="226" t="s">
         <v>96</v>
       </c>
-      <c r="C6" s="224" t="s">
+      <c r="C6" s="225" t="s">
         <v>97</v>
       </c>
-      <c r="D6" s="140" t="s">
+      <c r="D6" s="230" t="s">
         <v>98</v>
       </c>
-      <c r="E6" s="226" t="s">
+      <c r="E6" s="227" t="s">
         <v>99</v>
       </c>
-      <c r="F6" s="223" t="s">
+      <c r="F6" s="224" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="223" t="s">
+      <c r="G6" s="224" t="s">
         <v>100</v>
       </c>
-      <c r="H6" s="223" t="s">
+      <c r="H6" s="224" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="227" t="s">
+      <c r="I6" s="222" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="220" t="s">
+      <c r="J6" s="215" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="228" t="s">
+      <c r="K6" s="223" t="s">
         <v>471</v>
       </c>
-      <c r="L6" s="227"/>
+      <c r="L6" s="222"/>
     </row>
     <row r="7" spans="1:12" ht="28.8">
-      <c r="A7" s="224"/>
-      <c r="B7" s="225"/>
-      <c r="C7" s="224"/>
-      <c r="D7" s="141" t="s">
+      <c r="A7" s="225"/>
+      <c r="B7" s="226"/>
+      <c r="C7" s="225"/>
+      <c r="D7" s="231" t="s">
         <v>101</v>
       </c>
-      <c r="E7" s="226"/>
-      <c r="F7" s="223"/>
-      <c r="G7" s="223"/>
-      <c r="H7" s="223"/>
-      <c r="I7" s="227"/>
-      <c r="J7" s="220"/>
-      <c r="K7" s="228"/>
-      <c r="L7" s="227"/>
+      <c r="E7" s="227"/>
+      <c r="F7" s="224"/>
+      <c r="G7" s="224"/>
+      <c r="H7" s="224"/>
+      <c r="I7" s="222"/>
+      <c r="J7" s="215"/>
+      <c r="K7" s="223"/>
+      <c r="L7" s="222"/>
     </row>
     <row r="8" spans="1:12" ht="28.8">
-      <c r="A8" s="224"/>
-      <c r="B8" s="225"/>
-      <c r="C8" s="224"/>
-      <c r="D8" s="141" t="s">
+      <c r="A8" s="225"/>
+      <c r="B8" s="226"/>
+      <c r="C8" s="225"/>
+      <c r="D8" s="231" t="s">
         <v>102</v>
       </c>
-      <c r="E8" s="226"/>
-      <c r="F8" s="223"/>
-      <c r="G8" s="223"/>
-      <c r="H8" s="223"/>
-      <c r="I8" s="227"/>
-      <c r="J8" s="220"/>
-      <c r="K8" s="228"/>
-      <c r="L8" s="227"/>
+      <c r="E8" s="227"/>
+      <c r="F8" s="224"/>
+      <c r="G8" s="224"/>
+      <c r="H8" s="224"/>
+      <c r="I8" s="222"/>
+      <c r="J8" s="215"/>
+      <c r="K8" s="223"/>
+      <c r="L8" s="222"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="224"/>
-      <c r="B9" s="225"/>
-      <c r="C9" s="224"/>
-      <c r="D9" s="141" t="s">
+      <c r="A9" s="225"/>
+      <c r="B9" s="226"/>
+      <c r="C9" s="225"/>
+      <c r="D9" s="140" t="s">
         <v>103</v>
       </c>
-      <c r="E9" s="226"/>
-      <c r="F9" s="223"/>
-      <c r="G9" s="223"/>
-      <c r="H9" s="223"/>
-      <c r="I9" s="227"/>
-      <c r="J9" s="220"/>
-      <c r="K9" s="228"/>
-      <c r="L9" s="227"/>
+      <c r="E9" s="227"/>
+      <c r="F9" s="224"/>
+      <c r="G9" s="224"/>
+      <c r="H9" s="224"/>
+      <c r="I9" s="222"/>
+      <c r="J9" s="215"/>
+      <c r="K9" s="223"/>
+      <c r="L9" s="222"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="224"/>
-      <c r="B10" s="225"/>
-      <c r="C10" s="224"/>
-      <c r="D10" s="141" t="s">
+      <c r="A10" s="225"/>
+      <c r="B10" s="226"/>
+      <c r="C10" s="225"/>
+      <c r="D10" s="140" t="s">
         <v>104</v>
       </c>
-      <c r="E10" s="226"/>
-      <c r="F10" s="223"/>
-      <c r="G10" s="223"/>
-      <c r="H10" s="223"/>
-      <c r="I10" s="227"/>
-      <c r="J10" s="220"/>
-      <c r="K10" s="228"/>
-      <c r="L10" s="227"/>
+      <c r="E10" s="227"/>
+      <c r="F10" s="224"/>
+      <c r="G10" s="224"/>
+      <c r="H10" s="224"/>
+      <c r="I10" s="222"/>
+      <c r="J10" s="215"/>
+      <c r="K10" s="223"/>
+      <c r="L10" s="222"/>
     </row>
     <row r="11" spans="1:12">
       <c r="A11" s="122" t="s">
@@ -16484,10 +16490,10 @@
       <c r="G14" s="129" t="s">
         <v>234</v>
       </c>
-      <c r="H14" s="196" t="s">
+      <c r="H14" s="194" t="s">
         <v>29</v>
       </c>
-      <c r="I14" s="196" t="s">
+      <c r="I14" s="194" t="s">
         <v>19</v>
       </c>
       <c r="J14" s="107" t="s">
@@ -16657,17 +16663,17 @@
   </sheetData>
   <autoFilter ref="A1:L15" xr:uid="{FBE7E653-2382-46E4-9C76-9C694EDC9195}"/>
   <mergeCells count="11">
-    <mergeCell ref="L6:L10"/>
-    <mergeCell ref="K6:K10"/>
-    <mergeCell ref="H6:H10"/>
-    <mergeCell ref="I6:I10"/>
-    <mergeCell ref="J6:J10"/>
     <mergeCell ref="G6:G10"/>
     <mergeCell ref="A6:A10"/>
     <mergeCell ref="B6:B10"/>
     <mergeCell ref="C6:C10"/>
     <mergeCell ref="E6:E10"/>
     <mergeCell ref="F6:F10"/>
+    <mergeCell ref="L6:L10"/>
+    <mergeCell ref="K6:K10"/>
+    <mergeCell ref="H6:H10"/>
+    <mergeCell ref="I6:I10"/>
+    <mergeCell ref="J6:J10"/>
   </mergeCells>
   <conditionalFormatting sqref="F2:F6 F11:F15">
     <cfRule type="cellIs" dxfId="127" priority="7" operator="equal">
@@ -16759,7 +16765,7 @@
   </sheetPr>
   <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
@@ -16780,7 +16786,7 @@
     <col min="12" max="12" width="25.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="205" customFormat="1" ht="43.2">
+    <row r="1" spans="1:12" s="203" customFormat="1" ht="43.2">
       <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
@@ -16811,7 +16817,7 @@
       <c r="J1" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="203" t="s">
+      <c r="K1" s="201" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="108" t="s">
@@ -16828,7 +16834,7 @@
       <c r="C2" s="122" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="145" t="s">
+      <c r="D2" s="144" t="s">
         <v>15</v>
       </c>
       <c r="E2" s="82" t="s">
@@ -16852,7 +16858,7 @@
       <c r="K2" s="107" t="s">
         <v>481</v>
       </c>
-      <c r="L2" s="189"/>
+      <c r="L2" s="187"/>
     </row>
     <row r="3" spans="1:12" ht="28.8">
       <c r="A3" s="126" t="s">
@@ -16899,7 +16905,7 @@
       <c r="D4" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="197" t="s">
+      <c r="E4" s="195" t="s">
         <v>483</v>
       </c>
       <c r="F4" s="125" t="s">
@@ -16921,7 +16927,7 @@
       <c r="L4" s="107"/>
     </row>
     <row r="5" spans="1:12" ht="72">
-      <c r="A5" s="194" t="s">
+      <c r="A5" s="192" t="s">
         <v>56</v>
       </c>
       <c r="B5" s="74" t="s">
@@ -16933,7 +16939,7 @@
       <c r="D5" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="142" t="s">
+      <c r="E5" s="141" t="s">
         <v>484</v>
       </c>
       <c r="F5" s="128" t="s">
@@ -17069,7 +17075,7 @@
       <c r="D9" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="229" t="s">
+      <c r="E9" s="214" t="s">
         <v>606</v>
       </c>
       <c r="F9" s="128" t="s">
@@ -17138,7 +17144,7 @@
       <c r="C11" s="135" t="s">
         <v>428</v>
       </c>
-      <c r="D11" s="157" t="s">
+      <c r="D11" s="155" t="s">
         <v>429</v>
       </c>
       <c r="E11" s="127"/>
@@ -17193,7 +17199,7 @@
       <c r="L12" s="107"/>
     </row>
     <row r="13" spans="1:12" ht="57.6">
-      <c r="A13" s="194" t="s">
+      <c r="A13" s="192" t="s">
         <v>116</v>
       </c>
       <c r="B13" s="74" t="s">
@@ -17302,7 +17308,7 @@
       <c r="C16" s="122" t="s">
         <v>139</v>
       </c>
-      <c r="D16" s="191" t="s">
+      <c r="D16" s="189" t="s">
         <v>140</v>
       </c>
       <c r="E16" s="35" t="s">
@@ -17336,7 +17342,7 @@
       <c r="C17" s="126" t="s">
         <v>319</v>
       </c>
-      <c r="D17" s="144" t="s">
+      <c r="D17" s="143" t="s">
         <v>320</v>
       </c>
       <c r="E17" s="80" t="s">
@@ -17508,7 +17514,7 @@
       <c r="C22" s="122" t="s">
         <v>265</v>
       </c>
-      <c r="D22" s="145" t="s">
+      <c r="D22" s="144" t="s">
         <v>266</v>
       </c>
       <c r="E22" s="35" t="s">
@@ -17566,7 +17572,7 @@
       <c r="K23" s="106" t="s">
         <v>517</v>
       </c>
-      <c r="L23" s="198"/>
+      <c r="L23" s="196"/>
     </row>
     <row r="24" spans="1:12">
       <c r="A24" s="23"/>
@@ -18044,15 +18050,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Status xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">Draft</Status>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="221af607-abea-4d5e-830c-567dcc03c0ec" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18299,21 +18302,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Status xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">Draft</Status>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="cfc87205-1831-4b6c-a7b4-76d40079a43e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="221af607-abea-4d5e-830c-567dcc03c0ec" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16D2CAB5-B21B-4A93-9D82-49FE3E36CF14}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1A00443-9B7C-473F-A198-CBEB23A0BCC5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cfc87205-1831-4b6c-a7b4-76d40079a43e"/>
-    <ds:schemaRef ds:uri="221af607-abea-4d5e-830c-567dcc03c0ec"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -18338,9 +18341,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1A00443-9B7C-473F-A198-CBEB23A0BCC5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16D2CAB5-B21B-4A93-9D82-49FE3E36CF14}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="cfc87205-1831-4b6c-a7b4-76d40079a43e"/>
+    <ds:schemaRef ds:uri="221af607-abea-4d5e-830c-567dcc03c0ec"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
docs: adjusted usage notes also in exce;
</commit_message>
<xml_diff>
--- a/Documents/Metadata_CoreGenericHealth_v2.xlsx
+++ b/Documents/Metadata_CoreGenericHealth_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://healthri-my.sharepoint.com/personal/lucie_kulhankova_health-ri_nl/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DFDBD4BD-8827-48F6-A70B-F430D1049778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B604F9AE-9787-411E-AB68-6C0D2821F0CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="19410" windowHeight="20985" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28695" yWindow="0" windowWidth="19410" windowHeight="20985" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="14" r:id="rId1"/>
@@ -1017,9 +1017,9 @@
         <rFont val="Aptos Display"/>
         <scheme val="major"/>
       </rPr>
-      <t xml:space="preserve">This property makes use of another small class (prov:Attribution). There, you can choose one of the roles as listed in the controlled vocabulary and link that to a specific Agent (expressed with foaf:Agent). Note that for HealthDCAT-AP, the list of roles might be extended in the future.
-Example: https://standards.iso.org/iso/19115/resources/Codelists/gml/CI_RoleCode.xml#processor
-Next to the CI_RoleCodes, we propose that the CRediT Taxonomy can also be used: https://jats4r.niso.org/credit-taxonomy/#table-1-credit-terms-and-urls
+      <t xml:space="preserve">This property makes use of another small class (prov:Attribution). There, you can choose one of the roles as listed in the controlled vocabulary and link that to a specific Agent (expressed with foaf:Agent).
+Repeat this property if you wish to specify multiple roles for the same agent.
+Refer to the Attribution class for more information how to fill this.
 Use this property if you would like to indicate the </t>
     </r>
     <r>
@@ -1039,8 +1039,27 @@
         <rFont val="Aptos Display"/>
         <scheme val="major"/>
       </rPr>
-      <t>of the (research project that resulted in creation of the) dataset.
-The value for role then becomes: https://standards.iso.org/iso/19115/resources/Codelists/gml/CI_RoleCode.xml#funder</t>
+      <t xml:space="preserve">of the (research project that resulted in creation of the) dataset.
+The value for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Display"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve">role in the Attribution class </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Display"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>then becomes: https://standards.iso.org/iso/19115/resources/Codelists/gml/CI_RoleCode.xml#funder</t>
     </r>
   </si>
   <si>
@@ -11683,9 +11702,9 @@
   </sheetPr>
   <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.45"/>
@@ -12988,7 +13007,7 @@
       </c>
       <c r="L36" s="107"/>
     </row>
-    <row r="37" spans="1:14" ht="192.75" customHeight="1">
+    <row r="37" spans="1:14" ht="228" customHeight="1">
       <c r="A37" s="125" t="s">
         <v>291</v>
       </c>
@@ -14849,9 +14868,9 @@
   </sheetPr>
   <dimension ref="A1:Q57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="20" zoomScaleNormal="20" workbookViewId="0">
+    <sheetView zoomScale="20" zoomScaleNormal="20" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>

</xml_diff>